<commit_message>
update imminent infections calc
had factored out the immunity in the ineqaulity
</commit_message>
<xml_diff>
--- a/Supplemental_Quarantine_Calculation.xlsx
+++ b/Supplemental_Quarantine_Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Sufficient-strategies-for-travel-quarantine-and-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39559501-EFF5-4328-A24F-AD715E1C4E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C678D9DB-C2F5-42AF-A504-84F11255FC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,49 +572,49 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1045.806593051916</c:v>
+                  <c:v>271.36926860459835</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1044.1810743802675</c:v>
+                  <c:v>270.94747377565096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1042.5567962690311</c:v>
+                  <c:v>270.52600085132144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1040.9618393884966</c:v>
+                  <c:v>270.11213629452669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1039.6349482140884</c:v>
+                  <c:v>269.76783029195474</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1038.7167219965486</c:v>
+                  <c:v>269.52956599077055</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1038.1404350626988</c:v>
+                  <c:v>269.38002919803637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1037.7245476064693</c:v>
+                  <c:v>269.2721133792142</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1037.3941448206347</c:v>
+                  <c:v>269.18637939844518</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1037.1274766240322</c:v>
+                  <c:v>269.11718347450193</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1036.9078135268296</c:v>
+                  <c:v>269.06018458539251</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1036.722559349085</c:v>
+                  <c:v>269.01211423370944</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1036.562354954264</c:v>
+                  <c:v>268.97054388051157</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1036.4203112949012</c:v>
+                  <c:v>268.93368593353813</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1036.2913905699284</c:v>
+                  <c:v>268.90023316791559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -717,49 +717,49 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1041.938884803252</c:v>
+                  <c:v>270.36566319075882</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1040.3131700012955</c:v>
+                  <c:v>269.94381746928644</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1038.7785659601959</c:v>
+                  <c:v>269.54561346197033</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1037.9041614707946</c:v>
+                  <c:v>269.31872016417526</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1037.6354205518505</c:v>
+                  <c:v>269.24898640355207</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1037.5318679550969</c:v>
+                  <c:v>269.22211624167915</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1037.4180547967007</c:v>
+                  <c:v>269.1925836361699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1037.2781452491301</c:v>
+                  <c:v>269.15627945540905</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1037.1224777778082</c:v>
+                  <c:v>269.11588635775718</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1036.9636090819058</c:v>
+                  <c:v>269.07466259602376</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1036.8094831457165</c:v>
+                  <c:v>269.03466950088114</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1036.6637428075887</c:v>
+                  <c:v>268.99685232777603</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1036.5272529889073</c:v>
+                  <c:v>268.96143550929963</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1036.399406883454</c:v>
+                  <c:v>268.92826158941682</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1036.2789748913519</c:v>
+                  <c:v>268.89701150758481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -862,49 +862,49 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1042.0857387119697</c:v>
+                  <c:v>270.40376931675308</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1040.4604355213589</c:v>
+                  <c:v>269.98203040152055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1038.9030114552506</c:v>
+                  <c:v>269.57790498049633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1038.1436272979317</c:v>
+                  <c:v>269.38085752953293</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1037.9863349321472</c:v>
+                  <c:v>269.34004279902388</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1037.8228065372271</c:v>
+                  <c:v>269.29760992355688</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1037.6348279349231</c:v>
+                  <c:v>269.24883262939994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1037.4350091765612</c:v>
+                  <c:v>269.19698301335205</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1037.233214213496</c:v>
+                  <c:v>269.14462060533231</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1037.0406387157025</c:v>
+                  <c:v>269.09465049390383</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1036.8623799986808</c:v>
+                  <c:v>269.0483953469369</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1036.699546009902</c:v>
+                  <c:v>269.00614265821571</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1036.5510792814443</c:v>
+                  <c:v>268.96761803255231</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1036.4149653184136</c:v>
+                  <c:v>268.93229874231258</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1036.2889336777525</c:v>
+                  <c:v>268.89959564560769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1007,49 +1007,49 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1041.3075559341617</c:v>
+                  <c:v>270.2018439390996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039.9749402357229</c:v>
+                  <c:v>269.85605251856464</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1038.4158291184376</c:v>
+                  <c:v>269.45148933605844</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1037.671586710635</c:v>
+                  <c:v>269.25837091510783</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1037.5559583846507</c:v>
+                  <c:v>269.22836730405703</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1037.4526595558734</c:v>
+                  <c:v>269.20156299071726</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1037.3314148189334</c:v>
+                  <c:v>269.17010201523266</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1037.1950820730958</c:v>
+                  <c:v>269.13472595452458</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1037.0486835276176</c:v>
+                  <c:v>269.09673798765266</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1036.9018371027616</c:v>
+                  <c:v>269.05863380359506</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1036.7598856375005</c:v>
+                  <c:v>269.02179977944445</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1036.62505322075</c:v>
+                  <c:v>268.98681302896802</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1036.4977061008833</c:v>
+                  <c:v>268.95376858747488</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1036.3772474889433</c:v>
+                  <c:v>268.9225115982415</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1036.2626653032153</c:v>
+                  <c:v>268.89277944303933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,49 +1152,49 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1037.7675243278152</c:v>
+                  <c:v>269.28326511751465</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3042,7 +3042,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3540,7 +3540,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3610,36 +3610,36 @@
         <v>0</v>
       </c>
       <c r="B4" s="11">
-        <f>Inequality_Components_Lambda_j!B4+Inequality_Components_Lambda_j!H4-Inequality_Components_Lambda_j!N4+Inequality_Components_Lambda_j!T4+Inequality_Components_Lambda_j!Z4-Inequality_Components_Lambda_j!AF4</f>
-        <v>471.400779319251</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B4+Inequality_Components_Lambda_j!H4-Inequality_Components_Lambda_j!N4+Inequality_Components_Lambda_j!T4+Inequality_Components_Lambda_j!Z4-Inequality_Components_Lambda_j!AF4)</f>
+        <v>122.32059498706221</v>
       </c>
       <c r="C4" s="11">
-        <f>Inequality_Components_Lambda_j!C4+Inequality_Components_Lambda_j!I4-Inequality_Components_Lambda_j!O4+Inequality_Components_Lambda_j!U4+Inequality_Components_Lambda_j!AA4-Inequality_Components_Lambda_j!AG4</f>
-        <v>96.508641693181673</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C4+Inequality_Components_Lambda_j!I4-Inequality_Components_Lambda_j!O4+Inequality_Components_Lambda_j!U4+Inequality_Components_Lambda_j!AA4-Inequality_Components_Lambda_j!AG4)</f>
+        <v>25.042373689646318</v>
       </c>
       <c r="D4" s="11">
-        <f>Inequality_Components_Lambda_j!D4+Inequality_Components_Lambda_j!J4-Inequality_Components_Lambda_j!P4+Inequality_Components_Lambda_j!V4+Inequality_Components_Lambda_j!AB4-Inequality_Components_Lambda_j!AH4</f>
-        <v>118.48896626220737</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D4+Inequality_Components_Lambda_j!J4-Inequality_Components_Lambda_j!P4+Inequality_Components_Lambda_j!V4+Inequality_Components_Lambda_j!AB4-Inequality_Components_Lambda_j!AH4)</f>
+        <v>30.745899218761128</v>
       </c>
       <c r="E4" s="11">
-        <f>Inequality_Components_Lambda_j!E4+Inequality_Components_Lambda_j!K4-Inequality_Components_Lambda_j!Q4+Inequality_Components_Lambda_j!W4+Inequality_Components_Lambda_j!AC4-Inequality_Components_Lambda_j!AI4</f>
-        <v>128.11380064694191</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E4+Inequality_Components_Lambda_j!K4-Inequality_Components_Lambda_j!Q4+Inequality_Components_Lambda_j!W4+Inequality_Components_Lambda_j!AC4-Inequality_Components_Lambda_j!AI4)</f>
+        <v>33.243382295248239</v>
       </c>
       <c r="F4" s="11">
-        <f>Inequality_Components_Lambda_j!F4+Inequality_Components_Lambda_j!L4-Inequality_Components_Lambda_j!R4+Inequality_Components_Lambda_j!X4+Inequality_Components_Lambda_j!AD4-Inequality_Components_Lambda_j!AJ4</f>
-        <v>102.5061454531256</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F4+Inequality_Components_Lambda_j!L4-Inequality_Components_Lambda_j!R4+Inequality_Components_Lambda_j!X4+Inequality_Components_Lambda_j!AD4-Inequality_Components_Lambda_j!AJ4)</f>
+        <v>26.598625313610327</v>
       </c>
       <c r="G4" s="11">
-        <f>Inequality_Components_Lambda_j!G4+Inequality_Components_Lambda_j!M4-Inequality_Components_Lambda_j!S4+Inequality_Components_Lambda_j!Y4+Inequality_Components_Lambda_j!AE4-Inequality_Components_Lambda_j!AK4</f>
-        <v>128.7882596772086</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G4+Inequality_Components_Lambda_j!M4-Inequality_Components_Lambda_j!S4+Inequality_Components_Lambda_j!Y4+Inequality_Components_Lambda_j!AE4-Inequality_Components_Lambda_j!AK4)</f>
+        <v>33.418393100270151</v>
       </c>
       <c r="H4" s="11">
         <f>SUM(B4:G4)</f>
-        <v>1045.806593051916</v>
+        <v>271.36926860459835</v>
       </c>
       <c r="I4" s="9">
         <f>(H4-H68)/Background_Calculations!$B$10</f>
-        <v>4.1499120548498932E-7</v>
+        <v>1.0768325678763004E-7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3647,36 +3647,36 @@
         <v>1</v>
       </c>
       <c r="B5" s="11">
-        <f>Inequality_Components_Lambda_j!B5+Inequality_Components_Lambda_j!H5-Inequality_Components_Lambda_j!N5+Inequality_Components_Lambda_j!T5+Inequality_Components_Lambda_j!Z5-Inequality_Components_Lambda_j!AF5</f>
-        <v>470.56684807657922</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B5+Inequality_Components_Lambda_j!H5-Inequality_Components_Lambda_j!N5+Inequality_Components_Lambda_j!T5+Inequality_Components_Lambda_j!Z5-Inequality_Components_Lambda_j!AF5)</f>
+        <v>122.10420381789778</v>
       </c>
       <c r="C5" s="11">
-        <f>Inequality_Components_Lambda_j!C5+Inequality_Components_Lambda_j!I5-Inequality_Components_Lambda_j!O5+Inequality_Components_Lambda_j!U5+Inequality_Components_Lambda_j!AA5-Inequality_Components_Lambda_j!AG5</f>
-        <v>96.41056230556562</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C5+Inequality_Components_Lambda_j!I5-Inequality_Components_Lambda_j!O5+Inequality_Components_Lambda_j!U5+Inequality_Components_Lambda_j!AA5-Inequality_Components_Lambda_j!AG5)</f>
+        <v>25.016923733737276</v>
       </c>
       <c r="D5" s="11">
-        <f>Inequality_Components_Lambda_j!D5+Inequality_Components_Lambda_j!J5-Inequality_Components_Lambda_j!P5+Inequality_Components_Lambda_j!V5+Inequality_Components_Lambda_j!AB5-Inequality_Components_Lambda_j!AH5</f>
-        <v>118.34388589043442</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D5+Inequality_Components_Lambda_j!J5-Inequality_Components_Lambda_j!P5+Inequality_Components_Lambda_j!V5+Inequality_Components_Lambda_j!AB5-Inequality_Components_Lambda_j!AH5)</f>
+        <v>30.708253295854853</v>
       </c>
       <c r="E5" s="11">
-        <f>Inequality_Components_Lambda_j!E5+Inequality_Components_Lambda_j!K5-Inequality_Components_Lambda_j!Q5+Inequality_Components_Lambda_j!W5+Inequality_Components_Lambda_j!AC5-Inequality_Components_Lambda_j!AI5</f>
-        <v>127.95838851242561</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E5+Inequality_Components_Lambda_j!K5-Inequality_Components_Lambda_j!Q5+Inequality_Components_Lambda_j!W5+Inequality_Components_Lambda_j!AC5-Inequality_Components_Lambda_j!AI5)</f>
+        <v>33.203055453214382</v>
       </c>
       <c r="F5" s="11">
-        <f>Inequality_Components_Lambda_j!F5+Inequality_Components_Lambda_j!L5-Inequality_Components_Lambda_j!R5+Inequality_Components_Lambda_j!X5+Inequality_Components_Lambda_j!AD5-Inequality_Components_Lambda_j!AJ5</f>
-        <v>102.38125830152062</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F5+Inequality_Components_Lambda_j!L5-Inequality_Components_Lambda_j!R5+Inequality_Components_Lambda_j!X5+Inequality_Components_Lambda_j!AD5-Inequality_Components_Lambda_j!AJ5)</f>
+        <v>26.566219192617865</v>
       </c>
       <c r="G5" s="11">
-        <f>Inequality_Components_Lambda_j!G5+Inequality_Components_Lambda_j!M5-Inequality_Components_Lambda_j!S5+Inequality_Components_Lambda_j!Y5+Inequality_Components_Lambda_j!AE5-Inequality_Components_Lambda_j!AK5</f>
-        <v>128.52013129374211</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G5+Inequality_Components_Lambda_j!M5-Inequality_Components_Lambda_j!S5+Inequality_Components_Lambda_j!Y5+Inequality_Components_Lambda_j!AE5-Inequality_Components_Lambda_j!AK5)</f>
+        <v>33.348818282328814</v>
       </c>
       <c r="H5" s="11">
         <f t="shared" ref="H5:H18" si="0">SUM(B5:G5)</f>
-        <v>1044.1810743802675</v>
+        <v>270.94747377565096</v>
       </c>
       <c r="I5" s="9">
         <f>(H5-H69)/Background_Calculations!$B$10</f>
-        <v>3.310790041794568E-7</v>
+        <v>8.5909448086698986E-8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,36 +3684,36 @@
         <v>2</v>
       </c>
       <c r="B6" s="11">
-        <f>Inequality_Components_Lambda_j!B6+Inequality_Components_Lambda_j!H6-Inequality_Components_Lambda_j!N6+Inequality_Components_Lambda_j!T6+Inequality_Components_Lambda_j!Z6-Inequality_Components_Lambda_j!AF6</f>
-        <v>469.73352390102053</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B6+Inequality_Components_Lambda_j!H6-Inequality_Components_Lambda_j!N6+Inequality_Components_Lambda_j!T6+Inequality_Components_Lambda_j!Z6-Inequality_Components_Lambda_j!AF6)</f>
+        <v>121.88797017246631</v>
       </c>
       <c r="C6" s="11">
-        <f>Inequality_Components_Lambda_j!C6+Inequality_Components_Lambda_j!I6-Inequality_Components_Lambda_j!O6+Inequality_Components_Lambda_j!U6+Inequality_Components_Lambda_j!AA6-Inequality_Components_Lambda_j!AG6</f>
-        <v>96.312554258263802</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C6+Inequality_Components_Lambda_j!I6-Inequality_Components_Lambda_j!O6+Inequality_Components_Lambda_j!U6+Inequality_Components_Lambda_j!AA6-Inequality_Components_Lambda_j!AG6)</f>
+        <v>24.991492289443123</v>
       </c>
       <c r="D6" s="11">
-        <f>Inequality_Components_Lambda_j!D6+Inequality_Components_Lambda_j!J6-Inequality_Components_Lambda_j!P6+Inequality_Components_Lambda_j!V6+Inequality_Components_Lambda_j!AB6-Inequality_Components_Lambda_j!AH6</f>
-        <v>118.19891284432298</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D6+Inequality_Components_Lambda_j!J6-Inequality_Components_Lambda_j!P6+Inequality_Components_Lambda_j!V6+Inequality_Components_Lambda_j!AB6-Inequality_Components_Lambda_j!AH6)</f>
+        <v>30.670635222157461</v>
       </c>
       <c r="E6" s="11">
-        <f>Inequality_Components_Lambda_j!E6+Inequality_Components_Lambda_j!K6-Inequality_Components_Lambda_j!Q6+Inequality_Components_Lambda_j!W6+Inequality_Components_Lambda_j!AC6-Inequality_Components_Lambda_j!AI6</f>
-        <v>127.80309887266525</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E6+Inequality_Components_Lambda_j!K6-Inequality_Components_Lambda_j!Q6+Inequality_Components_Lambda_j!W6+Inequality_Components_Lambda_j!AC6-Inequality_Components_Lambda_j!AI6)</f>
+        <v>33.162760396514976</v>
       </c>
       <c r="F6" s="11">
-        <f>Inequality_Components_Lambda_j!F6+Inequality_Components_Lambda_j!L6-Inequality_Components_Lambda_j!R6+Inequality_Components_Lambda_j!X6+Inequality_Components_Lambda_j!AD6-Inequality_Components_Lambda_j!AJ6</f>
-        <v>102.25646962020588</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F6+Inequality_Components_Lambda_j!L6-Inequality_Components_Lambda_j!R6+Inequality_Components_Lambda_j!X6+Inequality_Components_Lambda_j!AD6-Inequality_Components_Lambda_j!AJ6)</f>
+        <v>26.533838623013985</v>
       </c>
       <c r="G6" s="11">
-        <f>Inequality_Components_Lambda_j!G6+Inequality_Components_Lambda_j!M6-Inequality_Components_Lambda_j!S6+Inequality_Components_Lambda_j!Y6+Inequality_Components_Lambda_j!AE6-Inequality_Components_Lambda_j!AK6</f>
-        <v>128.25223677255258</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G6+Inequality_Components_Lambda_j!M6-Inequality_Components_Lambda_j!S6+Inequality_Components_Lambda_j!Y6+Inequality_Components_Lambda_j!AE6-Inequality_Components_Lambda_j!AK6)</f>
+        <v>33.279304147725561</v>
       </c>
       <c r="H6" s="11">
         <f t="shared" si="0"/>
-        <v>1042.5567962690311</v>
+        <v>270.52600085132144</v>
       </c>
       <c r="I6" s="9">
         <f>(H6-H70)/Background_Calculations!$B$10</f>
-        <v>2.4723084283657903E-7</v>
+        <v>6.4152256681875571E-8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3721,36 +3721,36 @@
         <v>3</v>
       </c>
       <c r="B7" s="11">
-        <f>Inequality_Components_Lambda_j!B7+Inequality_Components_Lambda_j!H7-Inequality_Components_Lambda_j!N7+Inequality_Components_Lambda_j!T7+Inequality_Components_Lambda_j!Z7-Inequality_Components_Lambda_j!AF7</f>
-        <v>468.91454432466367</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B7+Inequality_Components_Lambda_j!H7-Inequality_Components_Lambda_j!N7+Inequality_Components_Lambda_j!T7+Inequality_Components_Lambda_j!Z7-Inequality_Components_Lambda_j!AF7)</f>
+        <v>121.67545870991232</v>
       </c>
       <c r="C7" s="11">
-        <f>Inequality_Components_Lambda_j!C7+Inequality_Components_Lambda_j!I7-Inequality_Components_Lambda_j!O7+Inequality_Components_Lambda_j!U7+Inequality_Components_Lambda_j!AA7-Inequality_Components_Lambda_j!AG7</f>
-        <v>96.216232264242223</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C7+Inequality_Components_Lambda_j!I7-Inequality_Components_Lambda_j!O7+Inequality_Components_Lambda_j!U7+Inequality_Components_Lambda_j!AA7-Inequality_Components_Lambda_j!AG7)</f>
+        <v>24.966498347693442</v>
       </c>
       <c r="D7" s="11">
-        <f>Inequality_Components_Lambda_j!D7+Inequality_Components_Lambda_j!J7-Inequality_Components_Lambda_j!P7+Inequality_Components_Lambda_j!V7+Inequality_Components_Lambda_j!AB7-Inequality_Components_Lambda_j!AH7</f>
-        <v>118.0564763273193</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D7+Inequality_Components_Lambda_j!J7-Inequality_Components_Lambda_j!P7+Inequality_Components_Lambda_j!V7+Inequality_Components_Lambda_j!AB7-Inequality_Components_Lambda_j!AH7)</f>
+        <v>30.633675335215962</v>
       </c>
       <c r="E7" s="11">
-        <f>Inequality_Components_Lambda_j!E7+Inequality_Components_Lambda_j!K7-Inequality_Components_Lambda_j!Q7+Inequality_Components_Lambda_j!W7+Inequality_Components_Lambda_j!AC7-Inequality_Components_Lambda_j!AI7</f>
-        <v>127.6507051054981</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E7+Inequality_Components_Lambda_j!K7-Inequality_Components_Lambda_j!Q7+Inequality_Components_Lambda_j!W7+Inequality_Components_Lambda_j!AC7-Inequality_Components_Lambda_j!AI7)</f>
+        <v>33.123216770178331</v>
       </c>
       <c r="F7" s="11">
-        <f>Inequality_Components_Lambda_j!F7+Inequality_Components_Lambda_j!L7-Inequality_Components_Lambda_j!R7+Inequality_Components_Lambda_j!X7+Inequality_Components_Lambda_j!AD7-Inequality_Components_Lambda_j!AJ7</f>
-        <v>102.1340088541758</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F7+Inequality_Components_Lambda_j!L7-Inequality_Components_Lambda_j!R7+Inequality_Components_Lambda_j!X7+Inequality_Components_Lambda_j!AD7-Inequality_Components_Lambda_j!AJ7)</f>
+        <v>26.502062108378176</v>
       </c>
       <c r="G7" s="11">
-        <f>Inequality_Components_Lambda_j!G7+Inequality_Components_Lambda_j!M7-Inequality_Components_Lambda_j!S7+Inequality_Components_Lambda_j!Y7+Inequality_Components_Lambda_j!AE7-Inequality_Components_Lambda_j!AK7</f>
-        <v>127.98987251259766</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G7+Inequality_Components_Lambda_j!M7-Inequality_Components_Lambda_j!S7+Inequality_Components_Lambda_j!Y7+Inequality_Components_Lambda_j!AE7-Inequality_Components_Lambda_j!AK7)</f>
+        <v>33.211225023148437</v>
       </c>
       <c r="H7" s="11">
         <f t="shared" si="0"/>
-        <v>1040.9618393884966</v>
+        <v>270.11213629452669</v>
       </c>
       <c r="I7" s="9">
         <f>(H7-H71)/Background_Calculations!$B$10</f>
-        <v>1.6489629622855576E-7</v>
+        <v>4.2787822911473416E-8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3758,36 +3758,36 @@
         <v>4</v>
       </c>
       <c r="B8" s="11">
-        <f>Inequality_Components_Lambda_j!B8+Inequality_Components_Lambda_j!H8-Inequality_Components_Lambda_j!N8+Inequality_Components_Lambda_j!T8+Inequality_Components_Lambda_j!Z8-Inequality_Components_Lambda_j!AF8</f>
-        <v>468.2267119236181</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B8+Inequality_Components_Lambda_j!H8-Inequality_Components_Lambda_j!N8+Inequality_Components_Lambda_j!T8+Inequality_Components_Lambda_j!Z8-Inequality_Components_Lambda_j!AF8)</f>
+        <v>121.49697773949735</v>
       </c>
       <c r="C8" s="11">
-        <f>Inequality_Components_Lambda_j!C8+Inequality_Components_Lambda_j!I8-Inequality_Components_Lambda_j!O8+Inequality_Components_Lambda_j!U8+Inequality_Components_Lambda_j!AA8-Inequality_Components_Lambda_j!AG8</f>
-        <v>96.135324903875102</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C8+Inequality_Components_Lambda_j!I8-Inequality_Components_Lambda_j!O8+Inequality_Components_Lambda_j!U8+Inequality_Components_Lambda_j!AA8-Inequality_Components_Lambda_j!AG8)</f>
+        <v>24.945504244813019</v>
       </c>
       <c r="D8" s="11">
-        <f>Inequality_Components_Lambda_j!D8+Inequality_Components_Lambda_j!J8-Inequality_Components_Lambda_j!P8+Inequality_Components_Lambda_j!V8+Inequality_Components_Lambda_j!AB8-Inequality_Components_Lambda_j!AH8</f>
-        <v>117.93722986451431</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D8+Inequality_Components_Lambda_j!J8-Inequality_Components_Lambda_j!P8+Inequality_Components_Lambda_j!V8+Inequality_Components_Lambda_j!AB8-Inequality_Components_Lambda_j!AH8)</f>
+        <v>30.602732878350544</v>
       </c>
       <c r="E8" s="11">
-        <f>Inequality_Components_Lambda_j!E8+Inequality_Components_Lambda_j!K8-Inequality_Components_Lambda_j!Q8+Inequality_Components_Lambda_j!W8+Inequality_Components_Lambda_j!AC8-Inequality_Components_Lambda_j!AI8</f>
-        <v>127.52478588738884</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E8+Inequality_Components_Lambda_j!K8-Inequality_Components_Lambda_j!Q8+Inequality_Components_Lambda_j!W8+Inequality_Components_Lambda_j!AC8-Inequality_Components_Lambda_j!AI8)</f>
+        <v>33.090542845239824</v>
       </c>
       <c r="F8" s="11">
-        <f>Inequality_Components_Lambda_j!F8+Inequality_Components_Lambda_j!L8-Inequality_Components_Lambda_j!R8+Inequality_Components_Lambda_j!X8+Inequality_Components_Lambda_j!AD8-Inequality_Components_Lambda_j!AJ8</f>
-        <v>102.03283027699331</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F8+Inequality_Components_Lambda_j!L8-Inequality_Components_Lambda_j!R8+Inequality_Components_Lambda_j!X8+Inequality_Components_Lambda_j!AD8-Inequality_Components_Lambda_j!AJ8)</f>
+        <v>26.47580796476225</v>
       </c>
       <c r="G8" s="11">
-        <f>Inequality_Components_Lambda_j!G8+Inequality_Components_Lambda_j!M8-Inequality_Components_Lambda_j!S8+Inequality_Components_Lambda_j!Y8+Inequality_Components_Lambda_j!AE8-Inequality_Components_Lambda_j!AK8</f>
-        <v>127.77806535769886</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G8+Inequality_Components_Lambda_j!M8-Inequality_Components_Lambda_j!S8+Inequality_Components_Lambda_j!Y8+Inequality_Components_Lambda_j!AE8-Inequality_Components_Lambda_j!AK8)</f>
+        <v>33.156264619291768</v>
       </c>
       <c r="H8" s="11">
         <f t="shared" si="0"/>
-        <v>1039.6349482140884</v>
+        <v>269.76783029195474</v>
       </c>
       <c r="I8" s="9">
         <f>(H8-H72)/Background_Calculations!$B$10</f>
-        <v>9.6399784143236819E-8</v>
+        <v>2.5014126981409747E-8</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3795,36 +3795,36 @@
         <v>5</v>
       </c>
       <c r="B9" s="11">
-        <f>Inequality_Components_Lambda_j!B9+Inequality_Components_Lambda_j!H9-Inequality_Components_Lambda_j!N9+Inequality_Components_Lambda_j!T9+Inequality_Components_Lambda_j!Z9-Inequality_Components_Lambda_j!AF9</f>
-        <v>467.73880944027707</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B9+Inequality_Components_Lambda_j!H9-Inequality_Components_Lambda_j!N9+Inequality_Components_Lambda_j!T9+Inequality_Components_Lambda_j!Z9-Inequality_Components_Lambda_j!AF9)</f>
+        <v>121.37037522911515</v>
       </c>
       <c r="C9" s="11">
-        <f>Inequality_Components_Lambda_j!C9+Inequality_Components_Lambda_j!I9-Inequality_Components_Lambda_j!O9+Inequality_Components_Lambda_j!U9+Inequality_Components_Lambda_j!AA9-Inequality_Components_Lambda_j!AG9</f>
-        <v>96.077916984641163</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C9+Inequality_Components_Lambda_j!I9-Inequality_Components_Lambda_j!O9+Inequality_Components_Lambda_j!U9+Inequality_Components_Lambda_j!AA9-Inequality_Components_Lambda_j!AG9)</f>
+        <v>24.930607852728549</v>
       </c>
       <c r="D9" s="11">
-        <f>Inequality_Components_Lambda_j!D9+Inequality_Components_Lambda_j!J9-Inequality_Components_Lambda_j!P9+Inequality_Components_Lambda_j!V9+Inequality_Components_Lambda_j!AB9-Inequality_Components_Lambda_j!AH9</f>
-        <v>117.85333638678384</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D9+Inequality_Components_Lambda_j!J9-Inequality_Components_Lambda_j!P9+Inequality_Components_Lambda_j!V9+Inequality_Components_Lambda_j!AB9-Inequality_Components_Lambda_j!AH9)</f>
+        <v>30.580963928103277</v>
       </c>
       <c r="E9" s="11">
-        <f>Inequality_Components_Lambda_j!E9+Inequality_Components_Lambda_j!K9-Inequality_Components_Lambda_j!Q9+Inequality_Components_Lambda_j!W9+Inequality_Components_Lambda_j!AC9-Inequality_Components_Lambda_j!AI9</f>
-        <v>127.43922758772183</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E9+Inequality_Components_Lambda_j!K9-Inequality_Components_Lambda_j!Q9+Inequality_Components_Lambda_j!W9+Inequality_Components_Lambda_j!AC9-Inequality_Components_Lambda_j!AI9)</f>
+        <v>33.068341901625637</v>
       </c>
       <c r="F9" s="11">
-        <f>Inequality_Components_Lambda_j!F9+Inequality_Components_Lambda_j!L9-Inequality_Components_Lambda_j!R9+Inequality_Components_Lambda_j!X9+Inequality_Components_Lambda_j!AD9-Inequality_Components_Lambda_j!AJ9</f>
-        <v>101.9640967732461</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F9+Inequality_Components_Lambda_j!L9-Inequality_Components_Lambda_j!R9+Inequality_Components_Lambda_j!X9+Inequality_Components_Lambda_j!AD9-Inequality_Components_Lambda_j!AJ9)</f>
+        <v>26.457972773471209</v>
       </c>
       <c r="G9" s="11">
-        <f>Inequality_Components_Lambda_j!G9+Inequality_Components_Lambda_j!M9-Inequality_Components_Lambda_j!S9+Inequality_Components_Lambda_j!Y9+Inequality_Components_Lambda_j!AE9-Inequality_Components_Lambda_j!AK9</f>
-        <v>127.64333482387867</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G9+Inequality_Components_Lambda_j!M9-Inequality_Components_Lambda_j!S9+Inequality_Components_Lambda_j!Y9+Inequality_Components_Lambda_j!AE9-Inequality_Components_Lambda_j!AK9)</f>
+        <v>33.121304305726717</v>
       </c>
       <c r="H9" s="11">
         <f t="shared" si="0"/>
-        <v>1038.7167219965486</v>
+        <v>269.52956599077055</v>
       </c>
       <c r="I9" s="9">
         <f>(H9-H73)/Background_Calculations!$B$10</f>
-        <v>4.8999293115916874E-8</v>
+        <v>1.2714494652601166E-8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3832,36 +3832,36 @@
         <v>6</v>
       </c>
       <c r="B10" s="11">
-        <f>Inequality_Components_Lambda_j!B10+Inequality_Components_Lambda_j!H10-Inequality_Components_Lambda_j!N10+Inequality_Components_Lambda_j!T10+Inequality_Components_Lambda_j!Z10-Inequality_Components_Lambda_j!AF10</f>
-        <v>467.41867096149707</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B10+Inequality_Components_Lambda_j!H10-Inequality_Components_Lambda_j!N10+Inequality_Components_Lambda_j!T10+Inequality_Components_Lambda_j!Z10-Inequality_Components_Lambda_j!AF10)</f>
+        <v>121.28730466385396</v>
       </c>
       <c r="C10" s="11">
-        <f>Inequality_Components_Lambda_j!C10+Inequality_Components_Lambda_j!I10-Inequality_Components_Lambda_j!O10+Inequality_Components_Lambda_j!U10+Inequality_Components_Lambda_j!AA10-Inequality_Components_Lambda_j!AG10</f>
-        <v>96.040185560209707</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C10+Inequality_Components_Lambda_j!I10-Inequality_Components_Lambda_j!O10+Inequality_Components_Lambda_j!U10+Inequality_Components_Lambda_j!AA10-Inequality_Components_Lambda_j!AG10)</f>
+        <v>24.920817180993069</v>
       </c>
       <c r="D10" s="11">
-        <f>Inequality_Components_Lambda_j!D10+Inequality_Components_Lambda_j!J10-Inequality_Components_Lambda_j!P10+Inequality_Components_Lambda_j!V10+Inequality_Components_Lambda_j!AB10-Inequality_Components_Lambda_j!AH10</f>
-        <v>117.7990445843924</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D10+Inequality_Components_Lambda_j!J10-Inequality_Components_Lambda_j!P10+Inequality_Components_Lambda_j!V10+Inequality_Components_Lambda_j!AB10-Inequality_Components_Lambda_j!AH10)</f>
+        <v>30.566876116069892</v>
       </c>
       <c r="E10" s="11">
-        <f>Inequality_Components_Lambda_j!E10+Inequality_Components_Lambda_j!K10-Inequality_Components_Lambda_j!Q10+Inequality_Components_Lambda_j!W10+Inequality_Components_Lambda_j!AC10-Inequality_Components_Lambda_j!AI10</f>
-        <v>127.38735645846731</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E10+Inequality_Components_Lambda_j!K10-Inequality_Components_Lambda_j!Q10+Inequality_Components_Lambda_j!W10+Inequality_Components_Lambda_j!AC10-Inequality_Components_Lambda_j!AI10)</f>
+        <v>33.054882213667064</v>
       </c>
       <c r="F10" s="11">
-        <f>Inequality_Components_Lambda_j!F10+Inequality_Components_Lambda_j!L10-Inequality_Components_Lambda_j!R10+Inequality_Components_Lambda_j!X10+Inequality_Components_Lambda_j!AD10-Inequality_Components_Lambda_j!AJ10</f>
-        <v>101.92244349363757</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F10+Inequality_Components_Lambda_j!L10-Inequality_Components_Lambda_j!R10+Inequality_Components_Lambda_j!X10+Inequality_Components_Lambda_j!AD10-Inequality_Components_Lambda_j!AJ10)</f>
+        <v>26.447164446102224</v>
       </c>
       <c r="G10" s="11">
-        <f>Inequality_Components_Lambda_j!G10+Inequality_Components_Lambda_j!M10-Inequality_Components_Lambda_j!S10+Inequality_Components_Lambda_j!Y10+Inequality_Components_Lambda_j!AE10-Inequality_Components_Lambda_j!AK10</f>
-        <v>127.57273400449475</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G10+Inequality_Components_Lambda_j!M10-Inequality_Components_Lambda_j!S10+Inequality_Components_Lambda_j!Y10+Inequality_Components_Lambda_j!AE10-Inequality_Components_Lambda_j!AK10)</f>
+        <v>33.102984577350178</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>1038.1404350626988</v>
+        <v>269.38002919803637</v>
       </c>
       <c r="I10" s="9">
         <f>(H10-H74)/Background_Calculations!$B$10</f>
-        <v>1.925032372763341E-8</v>
+        <v>4.9951361036346628E-9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3869,36 +3869,36 @@
         <v>7</v>
       </c>
       <c r="B11" s="11">
-        <f>Inequality_Components_Lambda_j!B11+Inequality_Components_Lambda_j!H11-Inequality_Components_Lambda_j!N11+Inequality_Components_Lambda_j!T11+Inequality_Components_Lambda_j!Z11-Inequality_Components_Lambda_j!AF11</f>
-        <v>467.18532704295905</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B11+Inequality_Components_Lambda_j!H11-Inequality_Components_Lambda_j!N11+Inequality_Components_Lambda_j!T11+Inequality_Components_Lambda_j!Z11-Inequality_Components_Lambda_j!AF11)</f>
+        <v>121.22675583108918</v>
       </c>
       <c r="C11" s="11">
-        <f>Inequality_Components_Lambda_j!C11+Inequality_Components_Lambda_j!I11-Inequality_Components_Lambda_j!O11+Inequality_Components_Lambda_j!U11+Inequality_Components_Lambda_j!AA11-Inequality_Components_Lambda_j!AG11</f>
-        <v>96.011920896052018</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C11+Inequality_Components_Lambda_j!I11-Inequality_Components_Lambda_j!O11+Inequality_Components_Lambda_j!U11+Inequality_Components_Lambda_j!AA11-Inequality_Components_Lambda_j!AG11)</f>
+        <v>24.913482974753801</v>
       </c>
       <c r="D11" s="11">
-        <f>Inequality_Components_Lambda_j!D11+Inequality_Components_Lambda_j!J11-Inequality_Components_Lambda_j!P11+Inequality_Components_Lambda_j!V11+Inequality_Components_Lambda_j!AB11-Inequality_Components_Lambda_j!AH11</f>
-        <v>117.75899474770415</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D11+Inequality_Components_Lambda_j!J11-Inequality_Components_Lambda_j!P11+Inequality_Components_Lambda_j!V11+Inequality_Components_Lambda_j!AB11-Inequality_Components_Lambda_j!AH11)</f>
+        <v>30.556483855242668</v>
       </c>
       <c r="E11" s="11">
-        <f>Inequality_Components_Lambda_j!E11+Inequality_Components_Lambda_j!K11-Inequality_Components_Lambda_j!Q11+Inequality_Components_Lambda_j!W11+Inequality_Components_Lambda_j!AC11-Inequality_Components_Lambda_j!AI11</f>
-        <v>127.34986921698315</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E11+Inequality_Components_Lambda_j!K11-Inequality_Components_Lambda_j!Q11+Inequality_Components_Lambda_j!W11+Inequality_Components_Lambda_j!AC11-Inequality_Components_Lambda_j!AI11)</f>
+        <v>33.045154903310497</v>
       </c>
       <c r="F11" s="11">
-        <f>Inequality_Components_Lambda_j!F11+Inequality_Components_Lambda_j!L11-Inequality_Components_Lambda_j!R11+Inequality_Components_Lambda_j!X11+Inequality_Components_Lambda_j!AD11-Inequality_Components_Lambda_j!AJ11</f>
-        <v>101.89235304047124</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F11+Inequality_Components_Lambda_j!L11-Inequality_Components_Lambda_j!R11+Inequality_Components_Lambda_j!X11+Inequality_Components_Lambda_j!AD11-Inequality_Components_Lambda_j!AJ11)</f>
+        <v>26.439356478240882</v>
       </c>
       <c r="G11" s="11">
-        <f>Inequality_Components_Lambda_j!G11+Inequality_Components_Lambda_j!M11-Inequality_Components_Lambda_j!S11+Inequality_Components_Lambda_j!Y11+Inequality_Components_Lambda_j!AE11-Inequality_Components_Lambda_j!AK11</f>
-        <v>127.52608266229971</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G11+Inequality_Components_Lambda_j!M11-Inequality_Components_Lambda_j!S11+Inequality_Components_Lambda_j!Y11+Inequality_Components_Lambda_j!AE11-Inequality_Components_Lambda_j!AK11)</f>
+        <v>33.090879336577174</v>
       </c>
       <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>1037.7245476064693</v>
+        <v>269.2721133792142</v>
       </c>
       <c r="I11" s="9">
         <f>(H11-H75)/Background_Calculations!$B$10</f>
-        <v>-2.2185357547269918E-9</v>
+        <v>-5.7567281477256118E-10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3906,36 +3906,36 @@
         <v>8</v>
       </c>
       <c r="B12" s="11">
-        <f>Inequality_Components_Lambda_j!B12+Inequality_Components_Lambda_j!H12-Inequality_Components_Lambda_j!N12+Inequality_Components_Lambda_j!T12+Inequality_Components_Lambda_j!Z12-Inequality_Components_Lambda_j!AF12</f>
-        <v>467.00279646098386</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B12+Inequality_Components_Lambda_j!H12-Inequality_Components_Lambda_j!N12+Inequality_Components_Lambda_j!T12+Inequality_Components_Lambda_j!Z12-Inequality_Components_Lambda_j!AF12)</f>
+        <v>121.17939220682284</v>
       </c>
       <c r="C12" s="11">
-        <f>Inequality_Components_Lambda_j!C12+Inequality_Components_Lambda_j!I12-Inequality_Components_Lambda_j!O12+Inequality_Components_Lambda_j!U12+Inequality_Components_Lambda_j!AA12-Inequality_Components_Lambda_j!AG12</f>
-        <v>95.988834731349598</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C12+Inequality_Components_Lambda_j!I12-Inequality_Components_Lambda_j!O12+Inequality_Components_Lambda_j!U12+Inequality_Components_Lambda_j!AA12-Inequality_Components_Lambda_j!AG12)</f>
+        <v>24.907492502259363</v>
       </c>
       <c r="D12" s="11">
-        <f>Inequality_Components_Lambda_j!D12+Inequality_Components_Lambda_j!J12-Inequality_Components_Lambda_j!P12+Inequality_Components_Lambda_j!V12+Inequality_Components_Lambda_j!AB12-Inequality_Components_Lambda_j!AH12</f>
-        <v>117.72673553943609</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D12+Inequality_Components_Lambda_j!J12-Inequality_Components_Lambda_j!P12+Inequality_Components_Lambda_j!V12+Inequality_Components_Lambda_j!AB12-Inequality_Components_Lambda_j!AH12)</f>
+        <v>30.54811313181099</v>
       </c>
       <c r="E12" s="11">
-        <f>Inequality_Components_Lambda_j!E12+Inequality_Components_Lambda_j!K12-Inequality_Components_Lambda_j!Q12+Inequality_Components_Lambda_j!W12+Inequality_Components_Lambda_j!AC12-Inequality_Components_Lambda_j!AI12</f>
-        <v>127.31924987593975</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E12+Inequality_Components_Lambda_j!K12-Inequality_Components_Lambda_j!Q12+Inequality_Components_Lambda_j!W12+Inequality_Components_Lambda_j!AC12-Inequality_Components_Lambda_j!AI12)</f>
+        <v>33.037209697916587</v>
       </c>
       <c r="F12" s="11">
-        <f>Inequality_Components_Lambda_j!F12+Inequality_Components_Lambda_j!L12-Inequality_Components_Lambda_j!R12+Inequality_Components_Lambda_j!X12+Inequality_Components_Lambda_j!AD12-Inequality_Components_Lambda_j!AJ12</f>
-        <v>101.86778351058281</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F12+Inequality_Components_Lambda_j!L12-Inequality_Components_Lambda_j!R12+Inequality_Components_Lambda_j!X12+Inequality_Components_Lambda_j!AD12-Inequality_Components_Lambda_j!AJ12)</f>
+        <v>26.432981097362546</v>
       </c>
       <c r="G12" s="11">
-        <f>Inequality_Components_Lambda_j!G12+Inequality_Components_Lambda_j!M12-Inequality_Components_Lambda_j!S12+Inequality_Components_Lambda_j!Y12+Inequality_Components_Lambda_j!AE12-Inequality_Components_Lambda_j!AK12</f>
-        <v>127.48874470234267</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G12+Inequality_Components_Lambda_j!M12-Inequality_Components_Lambda_j!S12+Inequality_Components_Lambda_j!Y12+Inequality_Components_Lambda_j!AE12-Inequality_Components_Lambda_j!AK12)</f>
+        <v>33.081190762272854</v>
       </c>
       <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>1037.3941448206347</v>
+        <v>269.18637939844518</v>
       </c>
       <c r="I12" s="9">
         <f>(H12-H76)/Background_Calculations!$B$10</f>
-        <v>-1.9274522597835416E-8</v>
+        <v>-5.0014153045336905E-9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3943,36 +3943,36 @@
         <v>9</v>
       </c>
       <c r="B13" s="11">
-        <f>Inequality_Components_Lambda_j!B13+Inequality_Components_Lambda_j!H13-Inequality_Components_Lambda_j!N13+Inequality_Components_Lambda_j!T13+Inequality_Components_Lambda_j!Z13-Inequality_Components_Lambda_j!AF13</f>
-        <v>466.85815064967431</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B13+Inequality_Components_Lambda_j!H13-Inequality_Components_Lambda_j!N13+Inequality_Components_Lambda_j!T13+Inequality_Components_Lambda_j!Z13-Inequality_Components_Lambda_j!AF13)</f>
+        <v>121.14185904506752</v>
       </c>
       <c r="C13" s="11">
-        <f>Inequality_Components_Lambda_j!C13+Inequality_Components_Lambda_j!I13-Inequality_Components_Lambda_j!O13+Inequality_Components_Lambda_j!U13+Inequality_Components_Lambda_j!AA13-Inequality_Components_Lambda_j!AG13</f>
-        <v>95.969609487372452</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C13+Inequality_Components_Lambda_j!I13-Inequality_Components_Lambda_j!O13+Inequality_Components_Lambda_j!U13+Inequality_Components_Lambda_j!AA13-Inequality_Components_Lambda_j!AG13)</f>
+        <v>24.902503873930296</v>
       </c>
       <c r="D13" s="11">
-        <f>Inequality_Components_Lambda_j!D13+Inequality_Components_Lambda_j!J13-Inequality_Components_Lambda_j!P13+Inequality_Components_Lambda_j!V13+Inequality_Components_Lambda_j!AB13-Inequality_Components_Lambda_j!AH13</f>
-        <v>117.70028477027095</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D13+Inequality_Components_Lambda_j!J13-Inequality_Components_Lambda_j!P13+Inequality_Components_Lambda_j!V13+Inequality_Components_Lambda_j!AB13-Inequality_Components_Lambda_j!AH13)</f>
+        <v>30.54124960089613</v>
       </c>
       <c r="E13" s="11">
-        <f>Inequality_Components_Lambda_j!E13+Inequality_Components_Lambda_j!K13-Inequality_Components_Lambda_j!Q13+Inequality_Components_Lambda_j!W13+Inequality_Components_Lambda_j!AC13-Inequality_Components_Lambda_j!AI13</f>
-        <v>127.29375101803623</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E13+Inequality_Components_Lambda_j!K13-Inequality_Components_Lambda_j!Q13+Inequality_Components_Lambda_j!W13+Inequality_Components_Lambda_j!AC13-Inequality_Components_Lambda_j!AI13)</f>
+        <v>33.030593172006824</v>
       </c>
       <c r="F13" s="11">
-        <f>Inequality_Components_Lambda_j!F13+Inequality_Components_Lambda_j!L13-Inequality_Components_Lambda_j!R13+Inequality_Components_Lambda_j!X13+Inequality_Components_Lambda_j!AD13-Inequality_Components_Lambda_j!AJ13</f>
-        <v>101.84733020148197</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F13+Inequality_Components_Lambda_j!L13-Inequality_Components_Lambda_j!R13+Inequality_Components_Lambda_j!X13+Inequality_Components_Lambda_j!AD13-Inequality_Components_Lambda_j!AJ13)</f>
+        <v>26.427673806733363</v>
       </c>
       <c r="G13" s="11">
-        <f>Inequality_Components_Lambda_j!G13+Inequality_Components_Lambda_j!M13-Inequality_Components_Lambda_j!S13+Inequality_Components_Lambda_j!Y13+Inequality_Components_Lambda_j!AE13-Inequality_Components_Lambda_j!AK13</f>
-        <v>127.45835049719629</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G13+Inequality_Components_Lambda_j!M13-Inequality_Components_Lambda_j!S13+Inequality_Components_Lambda_j!Y13+Inequality_Components_Lambda_j!AE13-Inequality_Components_Lambda_j!AK13)</f>
+        <v>33.073303975867809</v>
       </c>
       <c r="H13" s="11">
         <f t="shared" si="0"/>
-        <v>1037.1274766240322</v>
+        <v>269.11718347450193</v>
       </c>
       <c r="I13" s="9">
         <f>(H13-H77)/Background_Calculations!$B$10</f>
-        <v>-3.3040415162083315E-8</v>
+        <v>-8.5734335167639625E-9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3980,36 +3980,36 @@
         <v>10</v>
       </c>
       <c r="B14" s="11">
-        <f>Inequality_Components_Lambda_j!B14+Inequality_Components_Lambda_j!H14-Inequality_Components_Lambda_j!N14+Inequality_Components_Lambda_j!T14+Inequality_Components_Lambda_j!Z14-Inequality_Components_Lambda_j!AF14</f>
-        <v>466.74144535594456</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B14+Inequality_Components_Lambda_j!H14-Inequality_Components_Lambda_j!N14+Inequality_Components_Lambda_j!T14+Inequality_Components_Lambda_j!Z14-Inequality_Components_Lambda_j!AF14)</f>
+        <v>121.11157597895172</v>
       </c>
       <c r="C14" s="11">
-        <f>Inequality_Components_Lambda_j!C14+Inequality_Components_Lambda_j!I14-Inequality_Components_Lambda_j!O14+Inequality_Components_Lambda_j!U14+Inequality_Components_Lambda_j!AA14-Inequality_Components_Lambda_j!AG14</f>
-        <v>95.953231723306203</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C14+Inequality_Components_Lambda_j!I14-Inequality_Components_Lambda_j!O14+Inequality_Components_Lambda_j!U14+Inequality_Components_Lambda_j!AA14-Inequality_Components_Lambda_j!AG14)</f>
+        <v>24.898254118874664</v>
       </c>
       <c r="D14" s="11">
-        <f>Inequality_Components_Lambda_j!D14+Inequality_Components_Lambda_j!J14-Inequality_Components_Lambda_j!P14+Inequality_Components_Lambda_j!V14+Inequality_Components_Lambda_j!AB14-Inequality_Components_Lambda_j!AH14</f>
-        <v>117.678117801483</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D14+Inequality_Components_Lambda_j!J14-Inequality_Components_Lambda_j!P14+Inequality_Components_Lambda_j!V14+Inequality_Components_Lambda_j!AB14-Inequality_Components_Lambda_j!AH14)</f>
+        <v>30.535497644322962</v>
       </c>
       <c r="E14" s="11">
-        <f>Inequality_Components_Lambda_j!E14+Inequality_Components_Lambda_j!K14-Inequality_Components_Lambda_j!Q14+Inequality_Components_Lambda_j!W14+Inequality_Components_Lambda_j!AC14-Inequality_Components_Lambda_j!AI14</f>
-        <v>127.27202858392185</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E14+Inequality_Components_Lambda_j!K14-Inequality_Components_Lambda_j!Q14+Inequality_Components_Lambda_j!W14+Inequality_Components_Lambda_j!AC14-Inequality_Components_Lambda_j!AI14)</f>
+        <v>33.024956564724853</v>
       </c>
       <c r="F14" s="11">
-        <f>Inequality_Components_Lambda_j!F14+Inequality_Components_Lambda_j!L14-Inequality_Components_Lambda_j!R14+Inequality_Components_Lambda_j!X14+Inequality_Components_Lambda_j!AD14-Inequality_Components_Lambda_j!AJ14</f>
-        <v>101.82991265945215</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F14+Inequality_Components_Lambda_j!L14-Inequality_Components_Lambda_j!R14+Inequality_Components_Lambda_j!X14+Inequality_Components_Lambda_j!AD14-Inequality_Components_Lambda_j!AJ14)</f>
+        <v>26.423154246737354</v>
       </c>
       <c r="G14" s="11">
-        <f>Inequality_Components_Lambda_j!G14+Inequality_Components_Lambda_j!M14-Inequality_Components_Lambda_j!S14+Inequality_Components_Lambda_j!Y14+Inequality_Components_Lambda_j!AE14-Inequality_Components_Lambda_j!AK14</f>
-        <v>127.43307740272185</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G14+Inequality_Components_Lambda_j!M14-Inequality_Components_Lambda_j!S14+Inequality_Components_Lambda_j!Y14+Inequality_Components_Lambda_j!AE14-Inequality_Components_Lambda_j!AK14)</f>
+        <v>33.066746031780944</v>
       </c>
       <c r="H14" s="11">
         <f t="shared" si="0"/>
-        <v>1036.9078135268296</v>
+        <v>269.06018458539251</v>
       </c>
       <c r="I14" s="9">
         <f>(H14-H78)/Background_Calculations!$B$10</f>
-        <v>-4.4379819841553944E-8</v>
+        <v>-1.1515818824643041E-8</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4017,36 +4017,36 @@
         <v>11</v>
       </c>
       <c r="B15" s="11">
-        <f>Inequality_Components_Lambda_j!B15+Inequality_Components_Lambda_j!H15-Inequality_Components_Lambda_j!N15+Inequality_Components_Lambda_j!T15+Inequality_Components_Lambda_j!Z15-Inequality_Components_Lambda_j!AF15</f>
-        <v>466.64519322647357</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B15+Inequality_Components_Lambda_j!H15-Inequality_Components_Lambda_j!N15+Inequality_Components_Lambda_j!T15+Inequality_Components_Lambda_j!Z15-Inequality_Components_Lambda_j!AF15)</f>
+        <v>121.08660016588102</v>
       </c>
       <c r="C15" s="11">
-        <f>Inequality_Components_Lambda_j!C15+Inequality_Components_Lambda_j!I15-Inequality_Components_Lambda_j!O15+Inequality_Components_Lambda_j!U15+Inequality_Components_Lambda_j!AA15-Inequality_Components_Lambda_j!AG15</f>
-        <v>95.938938386422564</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C15+Inequality_Components_Lambda_j!I15-Inequality_Components_Lambda_j!O15+Inequality_Components_Lambda_j!U15+Inequality_Components_Lambda_j!AA15-Inequality_Components_Lambda_j!AG15)</f>
+        <v>24.894545237708872</v>
       </c>
       <c r="D15" s="11">
-        <f>Inequality_Components_Lambda_j!D15+Inequality_Components_Lambda_j!J15-Inequality_Components_Lambda_j!P15+Inequality_Components_Lambda_j!V15+Inequality_Components_Lambda_j!AB15-Inequality_Components_Lambda_j!AH15</f>
-        <v>117.65908668272053</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D15+Inequality_Components_Lambda_j!J15-Inequality_Components_Lambda_j!P15+Inequality_Components_Lambda_j!V15+Inequality_Components_Lambda_j!AB15-Inequality_Components_Lambda_j!AH15)</f>
+        <v>30.530559388230859</v>
       </c>
       <c r="E15" s="11">
-        <f>Inequality_Components_Lambda_j!E15+Inequality_Components_Lambda_j!K15-Inequality_Components_Lambda_j!Q15+Inequality_Components_Lambda_j!W15+Inequality_Components_Lambda_j!AC15-Inequality_Components_Lambda_j!AI15</f>
-        <v>127.25307058736124</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E15+Inequality_Components_Lambda_j!K15-Inequality_Components_Lambda_j!Q15+Inequality_Components_Lambda_j!W15+Inequality_Components_Lambda_j!AC15-Inequality_Components_Lambda_j!AI15)</f>
+        <v>33.020037282617587</v>
       </c>
       <c r="F15" s="11">
-        <f>Inequality_Components_Lambda_j!F15+Inequality_Components_Lambda_j!L15-Inequality_Components_Lambda_j!R15+Inequality_Components_Lambda_j!X15+Inequality_Components_Lambda_j!AD15-Inequality_Components_Lambda_j!AJ15</f>
-        <v>101.81471737555962</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F15+Inequality_Components_Lambda_j!L15-Inequality_Components_Lambda_j!R15+Inequality_Components_Lambda_j!X15+Inequality_Components_Lambda_j!AD15-Inequality_Components_Lambda_j!AJ15)</f>
+        <v>26.419211325451958</v>
       </c>
       <c r="G15" s="11">
-        <f>Inequality_Components_Lambda_j!G15+Inequality_Components_Lambda_j!M15-Inequality_Components_Lambda_j!S15+Inequality_Components_Lambda_j!Y15+Inequality_Components_Lambda_j!AE15-Inequality_Components_Lambda_j!AK15</f>
-        <v>127.4115530905475</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G15+Inequality_Components_Lambda_j!M15-Inequality_Components_Lambda_j!S15+Inequality_Components_Lambda_j!Y15+Inequality_Components_Lambda_j!AE15-Inequality_Components_Lambda_j!AK15)</f>
+        <v>33.06116083381913</v>
       </c>
       <c r="H15" s="11">
         <f t="shared" si="0"/>
-        <v>1036.722559349085</v>
+        <v>269.01211423370944</v>
       </c>
       <c r="I15" s="9">
         <f>(H15-H79)/Background_Calculations!$B$10</f>
-        <v>-5.3942974129920031E-8</v>
+        <v>-1.3997296950739558E-8</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4054,36 +4054,36 @@
         <v>12</v>
       </c>
       <c r="B16" s="11">
-        <f>Inequality_Components_Lambda_j!B16+Inequality_Components_Lambda_j!H16-Inequality_Components_Lambda_j!N16+Inequality_Components_Lambda_j!T16+Inequality_Components_Lambda_j!Z16-Inequality_Components_Lambda_j!AF16</f>
-        <v>466.56383105381752</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B16+Inequality_Components_Lambda_j!H16-Inequality_Components_Lambda_j!N16+Inequality_Components_Lambda_j!T16+Inequality_Components_Lambda_j!Z16-Inequality_Components_Lambda_j!AF16)</f>
+        <v>121.06548804684061</v>
       </c>
       <c r="C16" s="11">
-        <f>Inequality_Components_Lambda_j!C16+Inequality_Components_Lambda_j!I16-Inequality_Components_Lambda_j!O16+Inequality_Components_Lambda_j!U16+Inequality_Components_Lambda_j!AA16-Inequality_Components_Lambda_j!AG16</f>
-        <v>95.926162517953159</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C16+Inequality_Components_Lambda_j!I16-Inequality_Components_Lambda_j!O16+Inequality_Components_Lambda_j!U16+Inequality_Components_Lambda_j!AA16-Inequality_Components_Lambda_j!AG16)</f>
+        <v>24.891230114142655</v>
       </c>
       <c r="D16" s="11">
-        <f>Inequality_Components_Lambda_j!D16+Inequality_Components_Lambda_j!J16-Inequality_Components_Lambda_j!P16+Inequality_Components_Lambda_j!V16+Inequality_Components_Lambda_j!AB16-Inequality_Components_Lambda_j!AH16</f>
-        <v>117.64233847093851</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D16+Inequality_Components_Lambda_j!J16-Inequality_Components_Lambda_j!P16+Inequality_Components_Lambda_j!V16+Inequality_Components_Lambda_j!AB16-Inequality_Components_Lambda_j!AH16)</f>
+        <v>30.526213508206851</v>
       </c>
       <c r="E16" s="11">
-        <f>Inequality_Components_Lambda_j!E16+Inequality_Components_Lambda_j!K16-Inequality_Components_Lambda_j!Q16+Inequality_Components_Lambda_j!W16+Inequality_Components_Lambda_j!AC16-Inequality_Components_Lambda_j!AI16</f>
-        <v>127.23612510853494</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E16+Inequality_Components_Lambda_j!K16-Inequality_Components_Lambda_j!Q16+Inequality_Components_Lambda_j!W16+Inequality_Components_Lambda_j!AC16-Inequality_Components_Lambda_j!AI16)</f>
+        <v>33.015640215104526</v>
       </c>
       <c r="F16" s="11">
-        <f>Inequality_Components_Lambda_j!F16+Inequality_Components_Lambda_j!L16-Inequality_Components_Lambda_j!R16+Inequality_Components_Lambda_j!X16+Inequality_Components_Lambda_j!AD16-Inequality_Components_Lambda_j!AJ16</f>
-        <v>101.80113990137514</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F16+Inequality_Components_Lambda_j!L16-Inequality_Components_Lambda_j!R16+Inequality_Components_Lambda_j!X16+Inequality_Components_Lambda_j!AD16-Inequality_Components_Lambda_j!AJ16)</f>
+        <v>26.415688198648759</v>
       </c>
       <c r="G16" s="11">
-        <f>Inequality_Components_Lambda_j!G16+Inequality_Components_Lambda_j!M16-Inequality_Components_Lambda_j!S16+Inequality_Components_Lambda_j!Y16+Inequality_Components_Lambda_j!AE16-Inequality_Components_Lambda_j!AK16</f>
-        <v>127.39275790164481</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G16+Inequality_Components_Lambda_j!M16-Inequality_Components_Lambda_j!S16+Inequality_Components_Lambda_j!Y16+Inequality_Components_Lambda_j!AE16-Inequality_Components_Lambda_j!AK16)</f>
+        <v>33.05628379756817</v>
       </c>
       <c r="H16" s="11">
         <f t="shared" si="0"/>
-        <v>1036.562354954264</v>
+        <v>268.97054388051157</v>
       </c>
       <c r="I16" s="9">
         <f>(H16-H80)/Background_Calculations!$B$10</f>
-        <v>-6.2213013510407294E-8</v>
+        <v>-1.6143233448869208E-8</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -4091,36 +4091,36 @@
         <v>13</v>
       </c>
       <c r="B17" s="11">
-        <f>Inequality_Components_Lambda_j!B17+Inequality_Components_Lambda_j!H17-Inequality_Components_Lambda_j!N17+Inequality_Components_Lambda_j!T17+Inequality_Components_Lambda_j!Z17-Inequality_Components_Lambda_j!AF17</f>
-        <v>466.49326388755037</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B17+Inequality_Components_Lambda_j!H17-Inequality_Components_Lambda_j!N17+Inequality_Components_Lambda_j!T17+Inequality_Components_Lambda_j!Z17-Inequality_Components_Lambda_j!AF17)</f>
+        <v>121.04717705088339</v>
       </c>
       <c r="C17" s="11">
-        <f>Inequality_Components_Lambda_j!C17+Inequality_Components_Lambda_j!I17-Inequality_Components_Lambda_j!O17+Inequality_Components_Lambda_j!U17+Inequality_Components_Lambda_j!AA17-Inequality_Components_Lambda_j!AG17</f>
-        <v>95.914486792447917</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C17+Inequality_Components_Lambda_j!I17-Inequality_Components_Lambda_j!O17+Inequality_Components_Lambda_j!U17+Inequality_Components_Lambda_j!AA17-Inequality_Components_Lambda_j!AG17)</f>
+        <v>24.88820045922191</v>
       </c>
       <c r="D17" s="11">
-        <f>Inequality_Components_Lambda_j!D17+Inequality_Components_Lambda_j!J17-Inequality_Components_Lambda_j!P17+Inequality_Components_Lambda_j!V17+Inequality_Components_Lambda_j!AB17-Inequality_Components_Lambda_j!AH17</f>
-        <v>117.62724533416745</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D17+Inequality_Components_Lambda_j!J17-Inequality_Components_Lambda_j!P17+Inequality_Components_Lambda_j!V17+Inequality_Components_Lambda_j!AB17-Inequality_Components_Lambda_j!AH17)</f>
+        <v>30.522297092386065</v>
       </c>
       <c r="E17" s="11">
-        <f>Inequality_Components_Lambda_j!E17+Inequality_Components_Lambda_j!K17-Inequality_Components_Lambda_j!Q17+Inequality_Components_Lambda_j!W17+Inequality_Components_Lambda_j!AC17-Inequality_Components_Lambda_j!AI17</f>
-        <v>127.22063867637142</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E17+Inequality_Components_Lambda_j!K17-Inequality_Components_Lambda_j!Q17+Inequality_Components_Lambda_j!W17+Inequality_Components_Lambda_j!AC17-Inequality_Components_Lambda_j!AI17)</f>
+        <v>33.011621745726515</v>
       </c>
       <c r="F17" s="11">
-        <f>Inequality_Components_Lambda_j!F17+Inequality_Components_Lambda_j!L17-Inequality_Components_Lambda_j!R17+Inequality_Components_Lambda_j!X17+Inequality_Components_Lambda_j!AD17-Inequality_Components_Lambda_j!AJ17</f>
-        <v>101.78873531616208</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F17+Inequality_Components_Lambda_j!L17-Inequality_Components_Lambda_j!R17+Inequality_Components_Lambda_j!X17+Inequality_Components_Lambda_j!AD17-Inequality_Components_Lambda_j!AJ17)</f>
+        <v>26.412469416859683</v>
       </c>
       <c r="G17" s="11">
-        <f>Inequality_Components_Lambda_j!G17+Inequality_Components_Lambda_j!M17-Inequality_Components_Lambda_j!S17+Inequality_Components_Lambda_j!Y17+Inequality_Components_Lambda_j!AE17-Inequality_Components_Lambda_j!AK17</f>
-        <v>127.37594128820206</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G17+Inequality_Components_Lambda_j!M17-Inequality_Components_Lambda_j!S17+Inequality_Components_Lambda_j!Y17+Inequality_Components_Lambda_j!AE17-Inequality_Components_Lambda_j!AK17)</f>
+        <v>33.051920168460562</v>
       </c>
       <c r="H17" s="11">
         <f t="shared" si="0"/>
-        <v>1036.4203112949012</v>
+        <v>268.93368593353813</v>
       </c>
       <c r="I17" s="9">
         <f>(H17-H81)/Background_Calculations!$B$10</f>
-        <v>-6.9545563019997398E-8</v>
+        <v>-1.8045907050894056E-8</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4128,36 +4128,36 @@
         <v>14</v>
       </c>
       <c r="B18" s="11">
-        <f>Inequality_Components_Lambda_j!B18+Inequality_Components_Lambda_j!H18-Inequality_Components_Lambda_j!N18+Inequality_Components_Lambda_j!T18+Inequality_Components_Lambda_j!Z18-Inequality_Components_Lambda_j!AF18</f>
-        <v>466.43049718514152</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B18+Inequality_Components_Lambda_j!H18-Inequality_Components_Lambda_j!N18+Inequality_Components_Lambda_j!T18+Inequality_Components_Lambda_j!Z18-Inequality_Components_Lambda_j!AF18)</f>
+        <v>121.03089014445291</v>
       </c>
       <c r="C18" s="11">
-        <f>Inequality_Components_Lambda_j!C18+Inequality_Components_Lambda_j!I18-Inequality_Components_Lambda_j!O18+Inequality_Components_Lambda_j!U18+Inequality_Components_Lambda_j!AA18-Inequality_Components_Lambda_j!AG18</f>
-        <v>95.90360602945789</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C18+Inequality_Components_Lambda_j!I18-Inequality_Components_Lambda_j!O18+Inequality_Components_Lambda_j!U18+Inequality_Components_Lambda_j!AA18-Inequality_Components_Lambda_j!AG18)</f>
+        <v>24.885377083739215</v>
       </c>
       <c r="D18" s="11">
-        <f>Inequality_Components_Lambda_j!D18+Inequality_Components_Lambda_j!J18-Inequality_Components_Lambda_j!P18+Inequality_Components_Lambda_j!V18+Inequality_Components_Lambda_j!AB18-Inequality_Components_Lambda_j!AH18</f>
-        <v>117.61334815340982</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D18+Inequality_Components_Lambda_j!J18-Inequality_Components_Lambda_j!P18+Inequality_Components_Lambda_j!V18+Inequality_Components_Lambda_j!AB18-Inequality_Components_Lambda_j!AH18)</f>
+        <v>30.518691007089874</v>
       </c>
       <c r="E18" s="11">
-        <f>Inequality_Components_Lambda_j!E18+Inequality_Components_Lambda_j!K18-Inequality_Components_Lambda_j!Q18+Inequality_Components_Lambda_j!W18+Inequality_Components_Lambda_j!AC18-Inequality_Components_Lambda_j!AI18</f>
-        <v>127.20620655027778</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E18+Inequality_Components_Lambda_j!K18-Inequality_Components_Lambda_j!Q18+Inequality_Components_Lambda_j!W18+Inequality_Components_Lambda_j!AC18-Inequality_Components_Lambda_j!AI18)</f>
+        <v>33.007876851088767</v>
       </c>
       <c r="F18" s="11">
-        <f>Inequality_Components_Lambda_j!F18+Inequality_Components_Lambda_j!L18-Inequality_Components_Lambda_j!R18+Inequality_Components_Lambda_j!X18+Inequality_Components_Lambda_j!AD18-Inequality_Components_Lambda_j!AJ18</f>
-        <v>101.77717825967686</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F18+Inequality_Components_Lambda_j!L18-Inequality_Components_Lambda_j!R18+Inequality_Components_Lambda_j!X18+Inequality_Components_Lambda_j!AD18-Inequality_Components_Lambda_j!AJ18)</f>
+        <v>26.409470554559089</v>
       </c>
       <c r="G18" s="11">
-        <f>Inequality_Components_Lambda_j!G18+Inequality_Components_Lambda_j!M18-Inequality_Components_Lambda_j!S18+Inequality_Components_Lambda_j!Y18+Inequality_Components_Lambda_j!AE18-Inequality_Components_Lambda_j!AK18</f>
-        <v>127.36055439196467</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G18+Inequality_Components_Lambda_j!M18-Inequality_Components_Lambda_j!S18+Inequality_Components_Lambda_j!Y18+Inequality_Components_Lambda_j!AE18-Inequality_Components_Lambda_j!AK18)</f>
+        <v>33.047927526985767</v>
       </c>
       <c r="H18" s="11">
         <f t="shared" si="0"/>
-        <v>1036.2913905699284</v>
+        <v>268.90023316791559</v>
       </c>
       <c r="I18" s="9">
         <f>(H18-H82)/Background_Calculations!$B$10</f>
-        <v>-7.6200683022654277E-8</v>
+        <v>-1.9772799059030011E-8</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4177,36 +4177,36 @@
         <v>0</v>
       </c>
       <c r="B20" s="11">
-        <f>Inequality_Components_Lambda_j!B20+Inequality_Components_Lambda_j!H20-Inequality_Components_Lambda_j!N20+Inequality_Components_Lambda_j!T20+Inequality_Components_Lambda_j!Z20-Inequality_Components_Lambda_j!AF20</f>
-        <v>469.29047101456348</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B20+Inequality_Components_Lambda_j!H20-Inequality_Components_Lambda_j!N20+Inequality_Components_Lambda_j!T20+Inequality_Components_Lambda_j!Z20-Inequality_Components_Lambda_j!AF20)</f>
+        <v>121.77300538017126</v>
       </c>
       <c r="C20" s="11">
-        <f>Inequality_Components_Lambda_j!C20+Inequality_Components_Lambda_j!I20-Inequality_Components_Lambda_j!O20+Inequality_Components_Lambda_j!U20+Inequality_Components_Lambda_j!AA20-Inequality_Components_Lambda_j!AG20</f>
-        <v>96.279860294331385</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C20+Inequality_Components_Lambda_j!I20-Inequality_Components_Lambda_j!O20+Inequality_Components_Lambda_j!U20+Inequality_Components_Lambda_j!AA20-Inequality_Components_Lambda_j!AG20)</f>
+        <v>24.983008754209102</v>
       </c>
       <c r="D20" s="11">
-        <f>Inequality_Components_Lambda_j!D20+Inequality_Components_Lambda_j!J20-Inequality_Components_Lambda_j!P20+Inequality_Components_Lambda_j!V20+Inequality_Components_Lambda_j!AB20-Inequality_Components_Lambda_j!AH20</f>
-        <v>118.1447833800249</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D20+Inequality_Components_Lambda_j!J20-Inequality_Components_Lambda_j!P20+Inequality_Components_Lambda_j!V20+Inequality_Components_Lambda_j!AB20-Inequality_Components_Lambda_j!AH20)</f>
+        <v>30.656589534136256</v>
       </c>
       <c r="E20" s="11">
-        <f>Inequality_Components_Lambda_j!E20+Inequality_Components_Lambda_j!K20-Inequality_Components_Lambda_j!Q20+Inequality_Components_Lambda_j!W20+Inequality_Components_Lambda_j!AC20-Inequality_Components_Lambda_j!AI20</f>
-        <v>127.77001557108333</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E20+Inequality_Components_Lambda_j!K20-Inequality_Components_Lambda_j!Q20+Inequality_Components_Lambda_j!W20+Inequality_Components_Lambda_j!AC20-Inequality_Components_Lambda_j!AI20)</f>
+        <v>33.154175834691635</v>
       </c>
       <c r="F20" s="11">
-        <f>Inequality_Components_Lambda_j!F20+Inequality_Components_Lambda_j!L20-Inequality_Components_Lambda_j!R20+Inequality_Components_Lambda_j!X20+Inequality_Components_Lambda_j!AD20-Inequality_Components_Lambda_j!AJ20</f>
-        <v>102.22978573529247</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F20+Inequality_Components_Lambda_j!L20-Inequality_Components_Lambda_j!R20+Inequality_Components_Lambda_j!X20+Inequality_Components_Lambda_j!AD20-Inequality_Components_Lambda_j!AJ20)</f>
+        <v>26.526914602472718</v>
       </c>
       <c r="G20" s="11">
-        <f>Inequality_Components_Lambda_j!G20+Inequality_Components_Lambda_j!M20-Inequality_Components_Lambda_j!S20+Inequality_Components_Lambda_j!Y20+Inequality_Components_Lambda_j!AE20-Inequality_Components_Lambda_j!AK20</f>
-        <v>128.22396880795625</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G20+Inequality_Components_Lambda_j!M20-Inequality_Components_Lambda_j!S20+Inequality_Components_Lambda_j!Y20+Inequality_Components_Lambda_j!AE20-Inequality_Components_Lambda_j!AK20)</f>
+        <v>33.271969085077828</v>
       </c>
       <c r="H20" s="11">
         <f>SUM(B20:G20)</f>
-        <v>1041.938884803252</v>
+        <v>270.36566319075882</v>
       </c>
       <c r="I20" s="9">
         <f>(H20-H68)/Background_Calculations!$B$10</f>
-        <v>2.1533314014647631E-7</v>
+        <v>5.5875337883800961E-8</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4214,36 +4214,36 @@
         <v>1</v>
       </c>
       <c r="B21" s="11">
-        <f>Inequality_Components_Lambda_j!B21+Inequality_Components_Lambda_j!H21-Inequality_Components_Lambda_j!N21+Inequality_Components_Lambda_j!T21+Inequality_Components_Lambda_j!Z21-Inequality_Components_Lambda_j!AF21</f>
-        <v>468.45645864291345</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B21+Inequality_Components_Lambda_j!H21-Inequality_Components_Lambda_j!N21+Inequality_Components_Lambda_j!T21+Inequality_Components_Lambda_j!Z21-Inequality_Components_Lambda_j!AF21)</f>
+        <v>121.55659315939783</v>
       </c>
       <c r="C21" s="11">
-        <f>Inequality_Components_Lambda_j!C21+Inequality_Components_Lambda_j!I21-Inequality_Components_Lambda_j!O21+Inequality_Components_Lambda_j!U21+Inequality_Components_Lambda_j!AA21-Inequality_Components_Lambda_j!AG21</f>
-        <v>96.18177006200095</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C21+Inequality_Components_Lambda_j!I21-Inequality_Components_Lambda_j!O21+Inequality_Components_Lambda_j!U21+Inequality_Components_Lambda_j!AA21-Inequality_Components_Lambda_j!AG21)</f>
+        <v>24.957555984278589</v>
       </c>
       <c r="D21" s="11">
-        <f>Inequality_Components_Lambda_j!D21+Inequality_Components_Lambda_j!J21-Inequality_Components_Lambda_j!P21+Inequality_Components_Lambda_j!V21+Inequality_Components_Lambda_j!AB21-Inequality_Components_Lambda_j!AH21</f>
-        <v>117.99968669326711</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D21+Inequality_Components_Lambda_j!J21-Inequality_Components_Lambda_j!P21+Inequality_Components_Lambda_j!V21+Inequality_Components_Lambda_j!AB21-Inequality_Components_Lambda_j!AH21)</f>
+        <v>30.618939377765077</v>
       </c>
       <c r="E21" s="11">
-        <f>Inequality_Components_Lambda_j!E21+Inequality_Components_Lambda_j!K21-Inequality_Components_Lambda_j!Q21+Inequality_Components_Lambda_j!W21+Inequality_Components_Lambda_j!AC21-Inequality_Components_Lambda_j!AI21</f>
-        <v>127.61458147009314</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E21+Inequality_Components_Lambda_j!K21-Inequality_Components_Lambda_j!Q21+Inequality_Components_Lambda_j!W21+Inequality_Components_Lambda_j!AC21-Inequality_Components_Lambda_j!AI21)</f>
+        <v>33.113843292726273</v>
       </c>
       <c r="F21" s="11">
-        <f>Inequality_Components_Lambda_j!F21+Inequality_Components_Lambda_j!L21-Inequality_Components_Lambda_j!R21+Inequality_Components_Lambda_j!X21+Inequality_Components_Lambda_j!AD21-Inequality_Components_Lambda_j!AJ21</f>
-        <v>102.10488092542089</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F21+Inequality_Components_Lambda_j!L21-Inequality_Components_Lambda_j!R21+Inequality_Components_Lambda_j!X21+Inequality_Components_Lambda_j!AD21-Inequality_Components_Lambda_j!AJ21)</f>
+        <v>26.494503899456273</v>
       </c>
       <c r="G21" s="11">
-        <f>Inequality_Components_Lambda_j!G21+Inequality_Components_Lambda_j!M21-Inequality_Components_Lambda_j!S21+Inequality_Components_Lambda_j!Y21+Inequality_Components_Lambda_j!AE21-Inequality_Components_Lambda_j!AK21</f>
-        <v>127.95579220759994</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G21+Inequality_Components_Lambda_j!M21-Inequality_Components_Lambda_j!S21+Inequality_Components_Lambda_j!Y21+Inequality_Components_Lambda_j!AE21-Inequality_Components_Lambda_j!AK21)</f>
+        <v>33.202381755662373</v>
       </c>
       <c r="H21" s="11">
         <f t="shared" ref="H21:H34" si="1">SUM(B21:G21)</f>
-        <v>1040.3131700012955</v>
+        <v>269.94381746928644</v>
       </c>
       <c r="I21" s="9">
         <f>(H21-H69)/Background_Calculations!$B$10</f>
-        <v>1.3141081424122217E-7</v>
+        <v>3.40989020190748E-8</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4251,36 +4251,36 @@
         <v>2</v>
       </c>
       <c r="B22" s="11">
-        <f>Inequality_Components_Lambda_j!B22+Inequality_Components_Lambda_j!H22-Inequality_Components_Lambda_j!N22+Inequality_Components_Lambda_j!T22+Inequality_Components_Lambda_j!Z22-Inequality_Components_Lambda_j!AF22</f>
-        <v>467.66947790173242</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B22+Inequality_Components_Lambda_j!H22-Inequality_Components_Lambda_j!N22+Inequality_Components_Lambda_j!T22+Inequality_Components_Lambda_j!Z22-Inequality_Components_Lambda_j!AF22)</f>
+        <v>121.35238485782558</v>
       </c>
       <c r="C22" s="11">
-        <f>Inequality_Components_Lambda_j!C22+Inequality_Components_Lambda_j!I22-Inequality_Components_Lambda_j!O22+Inequality_Components_Lambda_j!U22+Inequality_Components_Lambda_j!AA22-Inequality_Components_Lambda_j!AG22</f>
-        <v>96.088990820656917</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C22+Inequality_Components_Lambda_j!I22-Inequality_Components_Lambda_j!O22+Inequality_Components_Lambda_j!U22+Inequality_Components_Lambda_j!AA22-Inequality_Components_Lambda_j!AG22)</f>
+        <v>24.933481327422825</v>
       </c>
       <c r="D22" s="11">
-        <f>Inequality_Components_Lambda_j!D22+Inequality_Components_Lambda_j!J22-Inequality_Components_Lambda_j!P22+Inequality_Components_Lambda_j!V22+Inequality_Components_Lambda_j!AB22-Inequality_Components_Lambda_j!AH22</f>
-        <v>117.86257995758983</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D22+Inequality_Components_Lambda_j!J22-Inequality_Components_Lambda_j!P22+Inequality_Components_Lambda_j!V22+Inequality_Components_Lambda_j!AB22-Inequality_Components_Lambda_j!AH22)</f>
+        <v>30.583362479676371</v>
       </c>
       <c r="E22" s="11">
-        <f>Inequality_Components_Lambda_j!E22+Inequality_Components_Lambda_j!K22-Inequality_Components_Lambda_j!Q22+Inequality_Components_Lambda_j!W22+Inequality_Components_Lambda_j!AC22-Inequality_Components_Lambda_j!AI22</f>
-        <v>127.46771528098274</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E22+Inequality_Components_Lambda_j!K22-Inequality_Components_Lambda_j!Q22+Inequality_Components_Lambda_j!W22+Inequality_Components_Lambda_j!AC22-Inequality_Components_Lambda_j!AI22)</f>
+        <v>33.075733980176111</v>
       </c>
       <c r="F22" s="11">
-        <f>Inequality_Components_Lambda_j!F22+Inequality_Components_Lambda_j!L22-Inequality_Components_Lambda_j!R22+Inequality_Components_Lambda_j!X22+Inequality_Components_Lambda_j!AD22-Inequality_Components_Lambda_j!AJ22</f>
-        <v>101.98686363300077</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F22+Inequality_Components_Lambda_j!L22-Inequality_Components_Lambda_j!R22+Inequality_Components_Lambda_j!X22+Inequality_Components_Lambda_j!AD22-Inequality_Components_Lambda_j!AJ22)</f>
+        <v>26.463880391687709</v>
       </c>
       <c r="G22" s="11">
-        <f>Inequality_Components_Lambda_j!G22+Inequality_Components_Lambda_j!M22-Inequality_Components_Lambda_j!S22+Inequality_Components_Lambda_j!Y22+Inequality_Components_Lambda_j!AE22-Inequality_Components_Lambda_j!AK22</f>
-        <v>127.70293836623324</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G22+Inequality_Components_Lambda_j!M22-Inequality_Components_Lambda_j!S22+Inequality_Components_Lambda_j!Y22+Inequality_Components_Lambda_j!AE22-Inequality_Components_Lambda_j!AK22)</f>
+        <v>33.136770425181744</v>
       </c>
       <c r="H22" s="11">
         <f t="shared" si="1"/>
-        <v>1038.7785659601959</v>
+        <v>269.54561346197033</v>
       </c>
       <c r="I22" s="9">
         <f>(H22-H70)/Background_Calculations!$B$10</f>
-        <v>5.2191789897171538E-8</v>
+        <v>1.3542894016599474E-8</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4288,36 +4288,36 @@
         <v>3</v>
       </c>
       <c r="B23" s="11">
-        <f>Inequality_Components_Lambda_j!B23+Inequality_Components_Lambda_j!H23-Inequality_Components_Lambda_j!N23+Inequality_Components_Lambda_j!T23+Inequality_Components_Lambda_j!Z23-Inequality_Components_Lambda_j!AF23</f>
-        <v>467.22351436614497</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B23+Inequality_Components_Lambda_j!H23-Inequality_Components_Lambda_j!N23+Inequality_Components_Lambda_j!T23+Inequality_Components_Lambda_j!Z23-Inequality_Components_Lambda_j!AF23)</f>
+        <v>121.23666480090424</v>
       </c>
       <c r="C23" s="11">
-        <f>Inequality_Components_Lambda_j!C23+Inequality_Components_Lambda_j!I23-Inequality_Components_Lambda_j!O23+Inequality_Components_Lambda_j!U23+Inequality_Components_Lambda_j!AA23-Inequality_Components_Lambda_j!AG23</f>
-        <v>96.034702101703573</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C23+Inequality_Components_Lambda_j!I23-Inequality_Components_Lambda_j!O23+Inequality_Components_Lambda_j!U23+Inequality_Components_Lambda_j!AA23-Inequality_Components_Lambda_j!AG23)</f>
+        <v>24.919394315489907</v>
       </c>
       <c r="D23" s="11">
-        <f>Inequality_Components_Lambda_j!D23+Inequality_Components_Lambda_j!J23-Inequality_Components_Lambda_j!P23+Inequality_Components_Lambda_j!V23+Inequality_Components_Lambda_j!AB23-Inequality_Components_Lambda_j!AH23</f>
-        <v>117.78337906128461</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D23+Inequality_Components_Lambda_j!J23-Inequality_Components_Lambda_j!P23+Inequality_Components_Lambda_j!V23+Inequality_Components_Lambda_j!AB23-Inequality_Components_Lambda_j!AH23)</f>
+        <v>30.562811175595893</v>
       </c>
       <c r="E23" s="11">
-        <f>Inequality_Components_Lambda_j!E23+Inequality_Components_Lambda_j!K23-Inequality_Components_Lambda_j!Q23+Inequality_Components_Lambda_j!W23+Inequality_Components_Lambda_j!AC23-Inequality_Components_Lambda_j!AI23</f>
-        <v>127.38289462360169</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E23+Inequality_Components_Lambda_j!K23-Inequality_Components_Lambda_j!Q23+Inequality_Components_Lambda_j!W23+Inequality_Components_Lambda_j!AC23-Inequality_Components_Lambda_j!AI23)</f>
+        <v>33.053724442361968</v>
       </c>
       <c r="F23" s="11">
-        <f>Inequality_Components_Lambda_j!F23+Inequality_Components_Lambda_j!L23-Inequality_Components_Lambda_j!R23+Inequality_Components_Lambda_j!X23+Inequality_Components_Lambda_j!AD23-Inequality_Components_Lambda_j!AJ23</f>
-        <v>101.9187231003518</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F23+Inequality_Components_Lambda_j!L23-Inequality_Components_Lambda_j!R23+Inequality_Components_Lambda_j!X23+Inequality_Components_Lambda_j!AD23-Inequality_Components_Lambda_j!AJ23)</f>
+        <v>26.446199066450202</v>
       </c>
       <c r="G23" s="11">
-        <f>Inequality_Components_Lambda_j!G23+Inequality_Components_Lambda_j!M23-Inequality_Components_Lambda_j!S23+Inequality_Components_Lambda_j!Y23+Inequality_Components_Lambda_j!AE23-Inequality_Components_Lambda_j!AK23</f>
-        <v>127.56094821770795</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G23+Inequality_Components_Lambda_j!M23-Inequality_Components_Lambda_j!S23+Inequality_Components_Lambda_j!Y23+Inequality_Components_Lambda_j!AE23-Inequality_Components_Lambda_j!AK23)</f>
+        <v>33.099926363373029</v>
       </c>
       <c r="H23" s="11">
         <f t="shared" si="1"/>
-        <v>1037.9041614707946</v>
+        <v>269.31872016417526</v>
       </c>
       <c r="I23" s="9">
         <f>(H23-H71)/Background_Calculations!$B$10</f>
-        <v>7.0534553970254866E-9</v>
+        <v>1.8302533613258918E-9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4325,36 +4325,36 @@
         <v>4</v>
       </c>
       <c r="B24" s="11">
-        <f>Inequality_Components_Lambda_j!B24+Inequality_Components_Lambda_j!H24-Inequality_Components_Lambda_j!N24+Inequality_Components_Lambda_j!T24+Inequality_Components_Lambda_j!Z24-Inequality_Components_Lambda_j!AF24</f>
-        <v>467.09013309611345</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B24+Inequality_Components_Lambda_j!H24-Inequality_Components_Lambda_j!N24+Inequality_Components_Lambda_j!T24+Inequality_Components_Lambda_j!Z24-Inequality_Components_Lambda_j!AF24)</f>
+        <v>121.20205459865987</v>
       </c>
       <c r="C24" s="11">
-        <f>Inequality_Components_Lambda_j!C24+Inequality_Components_Lambda_j!I24-Inequality_Components_Lambda_j!O24+Inequality_Components_Lambda_j!U24+Inequality_Components_Lambda_j!AA24-Inequality_Components_Lambda_j!AG24</f>
-        <v>96.015716633506031</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C24+Inequality_Components_Lambda_j!I24-Inequality_Components_Lambda_j!O24+Inequality_Components_Lambda_j!U24+Inequality_Components_Lambda_j!AA24-Inequality_Components_Lambda_j!AG24)</f>
+        <v>24.914467904953664</v>
       </c>
       <c r="D24" s="11">
-        <f>Inequality_Components_Lambda_j!D24+Inequality_Components_Lambda_j!J24-Inequality_Components_Lambda_j!P24+Inequality_Components_Lambda_j!V24+Inequality_Components_Lambda_j!AB24-Inequality_Components_Lambda_j!AH24</f>
-        <v>117.75728901514731</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D24+Inequality_Components_Lambda_j!J24-Inequality_Components_Lambda_j!P24+Inequality_Components_Lambda_j!V24+Inequality_Components_Lambda_j!AB24-Inequality_Components_Lambda_j!AH24)</f>
+        <v>30.556041246256015</v>
       </c>
       <c r="E24" s="11">
-        <f>Inequality_Components_Lambda_j!E24+Inequality_Components_Lambda_j!K24-Inequality_Components_Lambda_j!Q24+Inequality_Components_Lambda_j!W24+Inequality_Components_Lambda_j!AC24-Inequality_Components_Lambda_j!AI24</f>
-        <v>127.35504063886631</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E24+Inequality_Components_Lambda_j!K24-Inequality_Components_Lambda_j!Q24+Inequality_Components_Lambda_j!W24+Inequality_Components_Lambda_j!AC24-Inequality_Components_Lambda_j!AI24)</f>
+        <v>33.046496800544084</v>
       </c>
       <c r="F24" s="11">
-        <f>Inequality_Components_Lambda_j!F24+Inequality_Components_Lambda_j!L24-Inequality_Components_Lambda_j!R24+Inequality_Components_Lambda_j!X24+Inequality_Components_Lambda_j!AD24-Inequality_Components_Lambda_j!AJ24</f>
-        <v>101.89637656716299</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F24+Inequality_Components_Lambda_j!L24-Inequality_Components_Lambda_j!R24+Inequality_Components_Lambda_j!X24+Inequality_Components_Lambda_j!AD24-Inequality_Components_Lambda_j!AJ24)</f>
+        <v>26.440400515927013</v>
       </c>
       <c r="G24" s="11">
-        <f>Inequality_Components_Lambda_j!G24+Inequality_Components_Lambda_j!M24-Inequality_Components_Lambda_j!S24+Inequality_Components_Lambda_j!Y24+Inequality_Components_Lambda_j!AE24-Inequality_Components_Lambda_j!AK24</f>
-        <v>127.52086460105444</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G24+Inequality_Components_Lambda_j!M24-Inequality_Components_Lambda_j!S24+Inequality_Components_Lambda_j!Y24+Inequality_Components_Lambda_j!AE24-Inequality_Components_Lambda_j!AK24)</f>
+        <v>33.089525337211448</v>
       </c>
       <c r="H24" s="11">
         <f t="shared" si="1"/>
-        <v>1037.6354205518505</v>
+        <v>269.24898640355207</v>
       </c>
       <c r="I24" s="9">
         <f>(H24-H72)/Background_Calculations!$B$10</f>
-        <v>-6.8194348273619751E-9</v>
+        <v>-1.7695289489388758E-9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -4362,36 +4362,36 @@
         <v>5</v>
       </c>
       <c r="B25" s="11">
-        <f>Inequality_Components_Lambda_j!B25+Inequality_Components_Lambda_j!H25-Inequality_Components_Lambda_j!N25+Inequality_Components_Lambda_j!T25+Inequality_Components_Lambda_j!Z25-Inequality_Components_Lambda_j!AF25</f>
-        <v>467.04288859264085</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B25+Inequality_Components_Lambda_j!H25-Inequality_Components_Lambda_j!N25+Inequality_Components_Lambda_j!T25+Inequality_Components_Lambda_j!Z25-Inequality_Components_Lambda_j!AF25)</f>
+        <v>121.18979544248499</v>
       </c>
       <c r="C25" s="11">
-        <f>Inequality_Components_Lambda_j!C25+Inequality_Components_Lambda_j!I25-Inequality_Components_Lambda_j!O25+Inequality_Components_Lambda_j!U25+Inequality_Components_Lambda_j!AA25-Inequality_Components_Lambda_j!AG25</f>
-        <v>96.006385575147903</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C25+Inequality_Components_Lambda_j!I25-Inequality_Components_Lambda_j!O25+Inequality_Components_Lambda_j!U25+Inequality_Components_Lambda_j!AA25-Inequality_Components_Lambda_j!AG25)</f>
+        <v>24.912046651828302</v>
       </c>
       <c r="D25" s="11">
-        <f>Inequality_Components_Lambda_j!D25+Inequality_Components_Lambda_j!J25-Inequality_Components_Lambda_j!P25+Inequality_Components_Lambda_j!V25+Inequality_Components_Lambda_j!AB25-Inequality_Components_Lambda_j!AH25</f>
-        <v>117.74572323812011</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D25+Inequality_Components_Lambda_j!J25-Inequality_Components_Lambda_j!P25+Inequality_Components_Lambda_j!V25+Inequality_Components_Lambda_j!AB25-Inequality_Components_Lambda_j!AH25)</f>
+        <v>30.553040121121057</v>
       </c>
       <c r="E25" s="11">
-        <f>Inequality_Components_Lambda_j!E25+Inequality_Components_Lambda_j!K25-Inequality_Components_Lambda_j!Q25+Inequality_Components_Lambda_j!W25+Inequality_Components_Lambda_j!AC25-Inequality_Components_Lambda_j!AI25</f>
-        <v>127.34256901911614</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E25+Inequality_Components_Lambda_j!K25-Inequality_Components_Lambda_j!Q25+Inequality_Components_Lambda_j!W25+Inequality_Components_Lambda_j!AC25-Inequality_Components_Lambda_j!AI25)</f>
+        <v>33.043260624417059</v>
       </c>
       <c r="F25" s="11">
-        <f>Inequality_Components_Lambda_j!F25+Inequality_Components_Lambda_j!L25-Inequality_Components_Lambda_j!R25+Inequality_Components_Lambda_j!X25+Inequality_Components_Lambda_j!AD25-Inequality_Components_Lambda_j!AJ25</f>
-        <v>101.88639550980609</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F25+Inequality_Components_Lambda_j!L25-Inequality_Components_Lambda_j!R25+Inequality_Components_Lambda_j!X25+Inequality_Components_Lambda_j!AD25-Inequality_Components_Lambda_j!AJ25)</f>
+        <v>26.437810598964511</v>
       </c>
       <c r="G25" s="11">
-        <f>Inequality_Components_Lambda_j!G25+Inequality_Components_Lambda_j!M25-Inequality_Components_Lambda_j!S25+Inequality_Components_Lambda_j!Y25+Inequality_Components_Lambda_j!AE25-Inequality_Components_Lambda_j!AK25</f>
-        <v>127.50790602026585</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G25+Inequality_Components_Lambda_j!M25-Inequality_Components_Lambda_j!S25+Inequality_Components_Lambda_j!Y25+Inequality_Components_Lambda_j!AE25-Inequality_Components_Lambda_j!AK25)</f>
+        <v>33.086162802863207</v>
       </c>
       <c r="H25" s="11">
         <f t="shared" si="1"/>
-        <v>1037.5318679550969</v>
+        <v>269.22211624167915</v>
       </c>
       <c r="I25" s="9">
         <f>(H25-H73)/Background_Calculations!$B$10</f>
-        <v>-1.2165006364653514E-8</v>
+        <v>-3.156615096590574E-9</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -4399,36 +4399,36 @@
         <v>6</v>
       </c>
       <c r="B26" s="11">
-        <f>Inequality_Components_Lambda_j!B26+Inequality_Components_Lambda_j!H26-Inequality_Components_Lambda_j!N26+Inequality_Components_Lambda_j!T26+Inequality_Components_Lambda_j!Z26-Inequality_Components_Lambda_j!AF26</f>
-        <v>466.98927758122267</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B26+Inequality_Components_Lambda_j!H26-Inequality_Components_Lambda_j!N26+Inequality_Components_Lambda_j!T26+Inequality_Components_Lambda_j!Z26-Inequality_Components_Lambda_j!AF26)</f>
+        <v>121.17588428428962</v>
       </c>
       <c r="C26" s="11">
-        <f>Inequality_Components_Lambda_j!C26+Inequality_Components_Lambda_j!I26-Inequality_Components_Lambda_j!O26+Inequality_Components_Lambda_j!U26+Inequality_Components_Lambda_j!AA26-Inequality_Components_Lambda_j!AG26</f>
-        <v>95.996425131624179</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C26+Inequality_Components_Lambda_j!I26-Inequality_Components_Lambda_j!O26+Inequality_Components_Lambda_j!U26+Inequality_Components_Lambda_j!AA26-Inequality_Components_Lambda_j!AG26)</f>
+        <v>24.909462083809732</v>
       </c>
       <c r="D26" s="11">
-        <f>Inequality_Components_Lambda_j!D26+Inequality_Components_Lambda_j!J26-Inequality_Components_Lambda_j!P26+Inequality_Components_Lambda_j!V26+Inequality_Components_Lambda_j!AB26-Inequality_Components_Lambda_j!AH26</f>
-        <v>117.73321060264479</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D26+Inequality_Components_Lambda_j!J26-Inequality_Components_Lambda_j!P26+Inequality_Components_Lambda_j!V26+Inequality_Components_Lambda_j!AB26-Inequality_Components_Lambda_j!AH26)</f>
+        <v>30.549793302101353</v>
       </c>
       <c r="E26" s="11">
-        <f>Inequality_Components_Lambda_j!E26+Inequality_Components_Lambda_j!K26-Inequality_Components_Lambda_j!Q26+Inequality_Components_Lambda_j!W26+Inequality_Components_Lambda_j!AC26-Inequality_Components_Lambda_j!AI26</f>
-        <v>127.32931990379251</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E26+Inequality_Components_Lambda_j!K26-Inequality_Components_Lambda_j!Q26+Inequality_Components_Lambda_j!W26+Inequality_Components_Lambda_j!AC26-Inequality_Components_Lambda_j!AI26)</f>
+        <v>33.039822701230385</v>
       </c>
       <c r="F26" s="11">
-        <f>Inequality_Components_Lambda_j!F26+Inequality_Components_Lambda_j!L26-Inequality_Components_Lambda_j!R26+Inequality_Components_Lambda_j!X26+Inequality_Components_Lambda_j!AD26-Inequality_Components_Lambda_j!AJ26</f>
-        <v>101.87578944434854</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F26+Inequality_Components_Lambda_j!L26-Inequality_Components_Lambda_j!R26+Inequality_Components_Lambda_j!X26+Inequality_Components_Lambda_j!AD26-Inequality_Components_Lambda_j!AJ26)</f>
+        <v>26.435058502883734</v>
       </c>
       <c r="G26" s="11">
-        <f>Inequality_Components_Lambda_j!G26+Inequality_Components_Lambda_j!M26-Inequality_Components_Lambda_j!S26+Inequality_Components_Lambda_j!Y26+Inequality_Components_Lambda_j!AE26-Inequality_Components_Lambda_j!AK26</f>
-        <v>127.49403213306792</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G26+Inequality_Components_Lambda_j!M26-Inequality_Components_Lambda_j!S26+Inequality_Components_Lambda_j!Y26+Inequality_Components_Lambda_j!AE26-Inequality_Components_Lambda_j!AK26)</f>
+        <v>33.082562761855037</v>
       </c>
       <c r="H26" s="11">
         <f t="shared" si="1"/>
-        <v>1037.4180547967007</v>
+        <v>269.1925836361699</v>
       </c>
       <c r="I26" s="9">
         <f>(H26-H74)/Background_Calculations!$B$10</f>
-        <v>-1.8040246572674393E-8</v>
+        <v>-4.6811413796726248E-9</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4436,36 +4436,36 @@
         <v>7</v>
       </c>
       <c r="B27" s="11">
-        <f>Inequality_Components_Lambda_j!B27+Inequality_Components_Lambda_j!H27-Inequality_Components_Lambda_j!N27+Inequality_Components_Lambda_j!T27+Inequality_Components_Lambda_j!Z27-Inequality_Components_Lambda_j!AF27</f>
-        <v>466.91997896217299</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B27+Inequality_Components_Lambda_j!H27-Inequality_Components_Lambda_j!N27+Inequality_Components_Lambda_j!T27+Inequality_Components_Lambda_j!Z27-Inequality_Components_Lambda_j!AF27)</f>
+        <v>121.1579024550568</v>
       </c>
       <c r="C27" s="11">
-        <f>Inequality_Components_Lambda_j!C27+Inequality_Components_Lambda_j!I27-Inequality_Components_Lambda_j!O27+Inequality_Components_Lambda_j!U27+Inequality_Components_Lambda_j!AA27-Inequality_Components_Lambda_j!AG27</f>
-        <v>95.98487868657007</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C27+Inequality_Components_Lambda_j!I27-Inequality_Components_Lambda_j!O27+Inequality_Components_Lambda_j!U27+Inequality_Components_Lambda_j!AA27-Inequality_Components_Lambda_j!AG27)</f>
+        <v>24.906465974997516</v>
       </c>
       <c r="D27" s="11">
-        <f>Inequality_Components_Lambda_j!D27+Inequality_Components_Lambda_j!J27-Inequality_Components_Lambda_j!P27+Inequality_Components_Lambda_j!V27+Inequality_Components_Lambda_j!AB27-Inequality_Components_Lambda_j!AH27</f>
-        <v>117.71831195772711</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D27+Inequality_Components_Lambda_j!J27-Inequality_Components_Lambda_j!P27+Inequality_Components_Lambda_j!V27+Inequality_Components_Lambda_j!AB27-Inequality_Components_Lambda_j!AH27)</f>
+        <v>30.545927353654125</v>
       </c>
       <c r="E27" s="11">
-        <f>Inequality_Components_Lambda_j!E27+Inequality_Components_Lambda_j!K27-Inequality_Components_Lambda_j!Q27+Inequality_Components_Lambda_j!W27+Inequality_Components_Lambda_j!AC27-Inequality_Components_Lambda_j!AI27</f>
-        <v>127.31400492771871</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E27+Inequality_Components_Lambda_j!K27-Inequality_Components_Lambda_j!Q27+Inequality_Components_Lambda_j!W27+Inequality_Components_Lambda_j!AC27-Inequality_Components_Lambda_j!AI27)</f>
+        <v>33.035848721831655</v>
       </c>
       <c r="F27" s="11">
-        <f>Inequality_Components_Lambda_j!F27+Inequality_Components_Lambda_j!L27-Inequality_Components_Lambda_j!R27+Inequality_Components_Lambda_j!X27+Inequality_Components_Lambda_j!AD27-Inequality_Components_Lambda_j!AJ27</f>
-        <v>101.8635226881453</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F27+Inequality_Components_Lambda_j!L27-Inequality_Components_Lambda_j!R27+Inequality_Components_Lambda_j!X27+Inequality_Components_Lambda_j!AD27-Inequality_Components_Lambda_j!AJ27)</f>
+        <v>26.431875485410771</v>
       </c>
       <c r="G27" s="11">
-        <f>Inequality_Components_Lambda_j!G27+Inequality_Components_Lambda_j!M27-Inequality_Components_Lambda_j!S27+Inequality_Components_Lambda_j!Y27+Inequality_Components_Lambda_j!AE27-Inequality_Components_Lambda_j!AK27</f>
-        <v>127.47744802679595</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G27+Inequality_Components_Lambda_j!M27-Inequality_Components_Lambda_j!S27+Inequality_Components_Lambda_j!Y27+Inequality_Components_Lambda_j!AE27-Inequality_Components_Lambda_j!AK27)</f>
+        <v>33.078259464458192</v>
       </c>
       <c r="H27" s="11">
         <f t="shared" si="1"/>
-        <v>1037.2781452491301</v>
+        <v>269.15627945540905</v>
       </c>
       <c r="I27" s="9">
         <f>(H27-H75)/Background_Calculations!$B$10</f>
-        <v>-2.5262629388126101E-8</v>
+        <v>-6.5552285724992588E-9</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4473,36 +4473,36 @@
         <v>8</v>
       </c>
       <c r="B28" s="11">
-        <f>Inequality_Components_Lambda_j!B28+Inequality_Components_Lambda_j!H28-Inequality_Components_Lambda_j!N28+Inequality_Components_Lambda_j!T28+Inequality_Components_Lambda_j!Z28-Inequality_Components_Lambda_j!AF28</f>
-        <v>466.84131360310539</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B28+Inequality_Components_Lambda_j!H28-Inequality_Components_Lambda_j!N28+Inequality_Components_Lambda_j!T28+Inequality_Components_Lambda_j!Z28-Inequality_Components_Lambda_j!AF28)</f>
+        <v>121.13749011390642</v>
       </c>
       <c r="C28" s="11">
-        <f>Inequality_Components_Lambda_j!C28+Inequality_Components_Lambda_j!I28-Inequality_Components_Lambda_j!O28+Inequality_Components_Lambda_j!U28+Inequality_Components_Lambda_j!AA28-Inequality_Components_Lambda_j!AG28</f>
-        <v>95.972377656334928</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C28+Inequality_Components_Lambda_j!I28-Inequality_Components_Lambda_j!O28+Inequality_Components_Lambda_j!U28+Inequality_Components_Lambda_j!AA28-Inequality_Components_Lambda_j!AG28)</f>
+        <v>24.903222167342971</v>
       </c>
       <c r="D28" s="11">
-        <f>Inequality_Components_Lambda_j!D28+Inequality_Components_Lambda_j!J28-Inequality_Components_Lambda_j!P28+Inequality_Components_Lambda_j!V28+Inequality_Components_Lambda_j!AB28-Inequality_Components_Lambda_j!AH28</f>
-        <v>117.70197721756506</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D28+Inequality_Components_Lambda_j!J28-Inequality_Components_Lambda_j!P28+Inequality_Components_Lambda_j!V28+Inequality_Components_Lambda_j!AB28-Inequality_Components_Lambda_j!AH28)</f>
+        <v>30.541688762579948</v>
       </c>
       <c r="E28" s="11">
-        <f>Inequality_Components_Lambda_j!E28+Inequality_Components_Lambda_j!K28-Inequality_Components_Lambda_j!Q28+Inequality_Components_Lambda_j!W28+Inequality_Components_Lambda_j!AC28-Inequality_Components_Lambda_j!AI28</f>
-        <v>127.297423948618</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E28+Inequality_Components_Lambda_j!K28-Inequality_Components_Lambda_j!Q28+Inequality_Components_Lambda_j!W28+Inequality_Components_Lambda_j!AC28-Inequality_Components_Lambda_j!AI28)</f>
+        <v>33.03154623588329</v>
       </c>
       <c r="F28" s="11">
-        <f>Inequality_Components_Lambda_j!F28+Inequality_Components_Lambda_j!L28-Inequality_Components_Lambda_j!R28+Inequality_Components_Lambda_j!X28+Inequality_Components_Lambda_j!AD28-Inequality_Components_Lambda_j!AJ28</f>
-        <v>101.85023822563691</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F28+Inequality_Components_Lambda_j!L28-Inequality_Components_Lambda_j!R28+Inequality_Components_Lambda_j!X28+Inequality_Components_Lambda_j!AD28-Inequality_Components_Lambda_j!AJ28)</f>
+        <v>26.428428390222564</v>
       </c>
       <c r="G28" s="11">
-        <f>Inequality_Components_Lambda_j!G28+Inequality_Components_Lambda_j!M28-Inequality_Components_Lambda_j!S28+Inequality_Components_Lambda_j!Y28+Inequality_Components_Lambda_j!AE28-Inequality_Components_Lambda_j!AK28</f>
-        <v>127.45914712654802</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G28+Inequality_Components_Lambda_j!M28-Inequality_Components_Lambda_j!S28+Inequality_Components_Lambda_j!Y28+Inequality_Components_Lambda_j!AE28-Inequality_Components_Lambda_j!AK28)</f>
+        <v>33.073510687821972</v>
       </c>
       <c r="H28" s="11">
         <f t="shared" si="1"/>
-        <v>1037.1224777778082</v>
+        <v>269.11588635775718</v>
       </c>
       <c r="I28" s="9">
         <f>(H28-H76)/Background_Calculations!$B$10</f>
-        <v>-3.3298464606829551E-8</v>
+        <v>-8.6403930191682045E-9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4510,36 +4510,36 @@
         <v>9</v>
       </c>
       <c r="B29" s="11">
-        <f>Inequality_Components_Lambda_j!B29+Inequality_Components_Lambda_j!H29-Inequality_Components_Lambda_j!N29+Inequality_Components_Lambda_j!T29+Inequality_Components_Lambda_j!Z29-Inequality_Components_Lambda_j!AF29</f>
-        <v>466.76074538939406</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B29+Inequality_Components_Lambda_j!H29-Inequality_Components_Lambda_j!N29+Inequality_Components_Lambda_j!T29+Inequality_Components_Lambda_j!Z29-Inequality_Components_Lambda_j!AF29)</f>
+        <v>121.11658401389435</v>
       </c>
       <c r="C29" s="11">
-        <f>Inequality_Components_Lambda_j!C29+Inequality_Components_Lambda_j!I29-Inequality_Components_Lambda_j!O29+Inequality_Components_Lambda_j!U29+Inequality_Components_Lambda_j!AA29-Inequality_Components_Lambda_j!AG29</f>
-        <v>95.959682701976675</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C29+Inequality_Components_Lambda_j!I29-Inequality_Components_Lambda_j!O29+Inequality_Components_Lambda_j!U29+Inequality_Components_Lambda_j!AA29-Inequality_Components_Lambda_j!AG29)</f>
+        <v>24.899928039631352</v>
       </c>
       <c r="D29" s="11">
-        <f>Inequality_Components_Lambda_j!D29+Inequality_Components_Lambda_j!J29-Inequality_Components_Lambda_j!P29+Inequality_Components_Lambda_j!V29+Inequality_Components_Lambda_j!AB29-Inequality_Components_Lambda_j!AH29</f>
-        <v>117.68535073443809</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D29+Inequality_Components_Lambda_j!J29-Inequality_Components_Lambda_j!P29+Inequality_Components_Lambda_j!V29+Inequality_Components_Lambda_j!AB29-Inequality_Components_Lambda_j!AH29)</f>
+        <v>30.537374469100058</v>
       </c>
       <c r="E29" s="11">
-        <f>Inequality_Components_Lambda_j!E29+Inequality_Components_Lambda_j!K29-Inequality_Components_Lambda_j!Q29+Inequality_Components_Lambda_j!W29+Inequality_Components_Lambda_j!AC29-Inequality_Components_Lambda_j!AI29</f>
-        <v>127.2805857808119</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E29+Inequality_Components_Lambda_j!K29-Inequality_Components_Lambda_j!Q29+Inequality_Components_Lambda_j!W29+Inequality_Components_Lambda_j!AC29-Inequality_Components_Lambda_j!AI29)</f>
+        <v>33.027177013779955</v>
       </c>
       <c r="F29" s="11">
-        <f>Inequality_Components_Lambda_j!F29+Inequality_Components_Lambda_j!L29-Inequality_Components_Lambda_j!R29+Inequality_Components_Lambda_j!X29+Inequality_Components_Lambda_j!AD29-Inequality_Components_Lambda_j!AJ29</f>
-        <v>101.83674701593957</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F29+Inequality_Components_Lambda_j!L29-Inequality_Components_Lambda_j!R29+Inequality_Components_Lambda_j!X29+Inequality_Components_Lambda_j!AD29-Inequality_Components_Lambda_j!AJ29)</f>
+        <v>26.424927647606783</v>
       </c>
       <c r="G29" s="11">
-        <f>Inequality_Components_Lambda_j!G29+Inequality_Components_Lambda_j!M29-Inequality_Components_Lambda_j!S29+Inequality_Components_Lambda_j!Y29+Inequality_Components_Lambda_j!AE29-Inequality_Components_Lambda_j!AK29</f>
-        <v>127.44049745934561</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G29+Inequality_Components_Lambda_j!M29-Inequality_Components_Lambda_j!S29+Inequality_Components_Lambda_j!Y29+Inequality_Components_Lambda_j!AE29-Inequality_Components_Lambda_j!AK29)</f>
+        <v>33.068671412011263</v>
       </c>
       <c r="H29" s="11">
         <f t="shared" si="1"/>
-        <v>1036.9636090819058</v>
+        <v>269.07466259602376</v>
       </c>
       <c r="I29" s="9">
         <f>(H29-H77)/Background_Calculations!$B$10</f>
-        <v>-4.1499552803612077E-8</v>
+        <v>-1.0768437841709679E-8</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4547,36 +4547,36 @@
         <v>10</v>
       </c>
       <c r="B30" s="11">
-        <f>Inequality_Components_Lambda_j!B30+Inequality_Components_Lambda_j!H30-Inequality_Components_Lambda_j!N30+Inequality_Components_Lambda_j!T30+Inequality_Components_Lambda_j!Z30-Inequality_Components_Lambda_j!AF30</f>
-        <v>466.68299634132273</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B30+Inequality_Components_Lambda_j!H30-Inequality_Components_Lambda_j!N30+Inequality_Components_Lambda_j!T30+Inequality_Components_Lambda_j!Z30-Inequality_Components_Lambda_j!AF30)</f>
+        <v>121.09640944007737</v>
       </c>
       <c r="C30" s="11">
-        <f>Inequality_Components_Lambda_j!C30+Inequality_Components_Lambda_j!I30-Inequality_Components_Lambda_j!O30+Inequality_Components_Lambda_j!U30+Inequality_Components_Lambda_j!AA30-Inequality_Components_Lambda_j!AG30</f>
-        <v>95.947275055020754</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C30+Inequality_Components_Lambda_j!I30-Inequality_Components_Lambda_j!O30+Inequality_Components_Lambda_j!U30+Inequality_Components_Lambda_j!AA30-Inequality_Components_Lambda_j!AG30)</f>
+        <v>24.896708463371358</v>
       </c>
       <c r="D30" s="11">
-        <f>Inequality_Components_Lambda_j!D30+Inequality_Components_Lambda_j!J30-Inequality_Components_Lambda_j!P30+Inequality_Components_Lambda_j!V30+Inequality_Components_Lambda_j!AB30-Inequality_Components_Lambda_j!AH30</f>
-        <v>117.6691564817735</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D30+Inequality_Components_Lambda_j!J30-Inequality_Components_Lambda_j!P30+Inequality_Components_Lambda_j!V30+Inequality_Components_Lambda_j!AB30-Inequality_Components_Lambda_j!AH30)</f>
+        <v>30.533172332174946</v>
       </c>
       <c r="E30" s="11">
-        <f>Inequality_Components_Lambda_j!E30+Inequality_Components_Lambda_j!K30-Inequality_Components_Lambda_j!Q30+Inequality_Components_Lambda_j!W30+Inequality_Components_Lambda_j!AC30-Inequality_Components_Lambda_j!AI30</f>
-        <v>127.26412864976211</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E30+Inequality_Components_Lambda_j!K30-Inequality_Components_Lambda_j!Q30+Inequality_Components_Lambda_j!W30+Inequality_Components_Lambda_j!AC30-Inequality_Components_Lambda_j!AI30)</f>
+        <v>33.022906664323386</v>
       </c>
       <c r="F30" s="11">
-        <f>Inequality_Components_Lambda_j!F30+Inequality_Components_Lambda_j!L30-Inequality_Components_Lambda_j!R30+Inequality_Components_Lambda_j!X30+Inequality_Components_Lambda_j!AD30-Inequality_Components_Lambda_j!AJ30</f>
-        <v>101.82356211159946</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F30+Inequality_Components_Lambda_j!L30-Inequality_Components_Lambda_j!R30+Inequality_Components_Lambda_j!X30+Inequality_Components_Lambda_j!AD30-Inequality_Components_Lambda_j!AJ30)</f>
+        <v>26.42150638609326</v>
       </c>
       <c r="G30" s="11">
-        <f>Inequality_Components_Lambda_j!G30+Inequality_Components_Lambda_j!M30-Inequality_Components_Lambda_j!S30+Inequality_Components_Lambda_j!Y30+Inequality_Components_Lambda_j!AE30-Inequality_Components_Lambda_j!AK30</f>
-        <v>127.42236450623784</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G30+Inequality_Components_Lambda_j!M30-Inequality_Components_Lambda_j!S30+Inequality_Components_Lambda_j!Y30+Inequality_Components_Lambda_j!AE30-Inequality_Components_Lambda_j!AK30)</f>
+        <v>33.063966214840782</v>
       </c>
       <c r="H30" s="11">
         <f t="shared" si="1"/>
-        <v>1036.8094831457165</v>
+        <v>269.03466950088114</v>
       </c>
       <c r="I30" s="9">
         <f>(H30-H78)/Background_Calculations!$B$10</f>
-        <v>-4.9455811202541875E-8</v>
+        <v>-1.2832953438467194E-8</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4584,36 +4584,36 @@
         <v>11</v>
       </c>
       <c r="B31" s="11">
-        <f>Inequality_Components_Lambda_j!B31+Inequality_Components_Lambda_j!H31-Inequality_Components_Lambda_j!N31+Inequality_Components_Lambda_j!T31+Inequality_Components_Lambda_j!Z31-Inequality_Components_Lambda_j!AF31</f>
-        <v>466.61023181520869</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B31+Inequality_Components_Lambda_j!H31-Inequality_Components_Lambda_j!N31+Inequality_Components_Lambda_j!T31+Inequality_Components_Lambda_j!Z31-Inequality_Components_Lambda_j!AF31)</f>
+        <v>121.07752826609824</v>
       </c>
       <c r="C31" s="11">
-        <f>Inequality_Components_Lambda_j!C31+Inequality_Components_Lambda_j!I31-Inequality_Components_Lambda_j!O31+Inequality_Components_Lambda_j!U31+Inequality_Components_Lambda_j!AA31-Inequality_Components_Lambda_j!AG31</f>
-        <v>95.935375391716093</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C31+Inequality_Components_Lambda_j!I31-Inequality_Components_Lambda_j!O31+Inequality_Components_Lambda_j!U31+Inequality_Components_Lambda_j!AA31-Inequality_Components_Lambda_j!AG31)</f>
+        <v>24.893620700347984</v>
       </c>
       <c r="D31" s="11">
-        <f>Inequality_Components_Lambda_j!D31+Inequality_Components_Lambda_j!J31-Inequality_Components_Lambda_j!P31+Inequality_Components_Lambda_j!V31+Inequality_Components_Lambda_j!AB31-Inequality_Components_Lambda_j!AH31</f>
-        <v>117.65372644891903</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D31+Inequality_Components_Lambda_j!J31-Inequality_Components_Lambda_j!P31+Inequality_Components_Lambda_j!V31+Inequality_Components_Lambda_j!AB31-Inequality_Components_Lambda_j!AH31)</f>
+        <v>30.529168497471588</v>
       </c>
       <c r="E31" s="11">
-        <f>Inequality_Components_Lambda_j!E31+Inequality_Components_Lambda_j!K31-Inequality_Components_Lambda_j!Q31+Inequality_Components_Lambda_j!W31+Inequality_Components_Lambda_j!AC31-Inequality_Components_Lambda_j!AI31</f>
-        <v>127.24834522374456</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E31+Inequality_Components_Lambda_j!K31-Inequality_Components_Lambda_j!Q31+Inequality_Components_Lambda_j!W31+Inequality_Components_Lambda_j!AC31-Inequality_Components_Lambda_j!AI31)</f>
+        <v>33.018811130022002</v>
       </c>
       <c r="F31" s="11">
-        <f>Inequality_Components_Lambda_j!F31+Inequality_Components_Lambda_j!L31-Inequality_Components_Lambda_j!R31+Inequality_Components_Lambda_j!X31+Inequality_Components_Lambda_j!AD31-Inequality_Components_Lambda_j!AJ31</f>
-        <v>101.81091878089259</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F31+Inequality_Components_Lambda_j!L31-Inequality_Components_Lambda_j!R31+Inequality_Components_Lambda_j!X31+Inequality_Components_Lambda_j!AD31-Inequality_Components_Lambda_j!AJ31)</f>
+        <v>26.418225653853245</v>
       </c>
       <c r="G31" s="11">
-        <f>Inequality_Components_Lambda_j!G31+Inequality_Components_Lambda_j!M31-Inequality_Components_Lambda_j!S31+Inequality_Components_Lambda_j!Y31+Inequality_Components_Lambda_j!AE31-Inequality_Components_Lambda_j!AK31</f>
-        <v>127.40514514710759</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G31+Inequality_Components_Lambda_j!M31-Inequality_Components_Lambda_j!S31+Inequality_Components_Lambda_j!Y31+Inequality_Components_Lambda_j!AE31-Inequality_Components_Lambda_j!AK31)</f>
+        <v>33.059498079982902</v>
       </c>
       <c r="H31" s="11">
         <f t="shared" si="1"/>
-        <v>1036.6637428075887</v>
+        <v>268.99685232777603</v>
       </c>
       <c r="I31" s="9">
         <f>(H31-H79)/Background_Calculations!$B$10</f>
-        <v>-5.697918992750757E-8</v>
+        <v>-1.4785144020925477E-8</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4621,36 +4621,36 @@
         <v>12</v>
       </c>
       <c r="B32" s="11">
-        <f>Inequality_Components_Lambda_j!B32+Inequality_Components_Lambda_j!H32-Inequality_Components_Lambda_j!N32+Inequality_Components_Lambda_j!T32+Inequality_Components_Lambda_j!Z32-Inequality_Components_Lambda_j!AF32</f>
-        <v>466.54296593295493</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B32+Inequality_Components_Lambda_j!H32-Inequality_Components_Lambda_j!N32+Inequality_Components_Lambda_j!T32+Inequality_Components_Lambda_j!Z32-Inequality_Components_Lambda_j!AF32)</f>
+        <v>121.06007389796696</v>
       </c>
       <c r="C32" s="11">
-        <f>Inequality_Components_Lambda_j!C32+Inequality_Components_Lambda_j!I32-Inequality_Components_Lambda_j!O32+Inequality_Components_Lambda_j!U32+Inequality_Components_Lambda_j!AA32-Inequality_Components_Lambda_j!AG32</f>
-        <v>95.924036107362369</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C32+Inequality_Components_Lambda_j!I32-Inequality_Components_Lambda_j!O32+Inequality_Components_Lambda_j!U32+Inequality_Components_Lambda_j!AA32-Inequality_Components_Lambda_j!AG32)</f>
+        <v>24.890678346262618</v>
       </c>
       <c r="D32" s="11">
-        <f>Inequality_Components_Lambda_j!D32+Inequality_Components_Lambda_j!J32-Inequality_Components_Lambda_j!P32+Inequality_Components_Lambda_j!V32+Inequality_Components_Lambda_j!AB32-Inequality_Components_Lambda_j!AH32</f>
-        <v>117.63913946031298</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D32+Inequality_Components_Lambda_j!J32-Inequality_Components_Lambda_j!P32+Inequality_Components_Lambda_j!V32+Inequality_Components_Lambda_j!AB32-Inequality_Components_Lambda_j!AH32)</f>
+        <v>30.525383418609522</v>
       </c>
       <c r="E32" s="11">
-        <f>Inequality_Components_Lambda_j!E32+Inequality_Components_Lambda_j!K32-Inequality_Components_Lambda_j!Q32+Inequality_Components_Lambda_j!W32+Inequality_Components_Lambda_j!AC32-Inequality_Components_Lambda_j!AI32</f>
-        <v>127.23330499117085</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E32+Inequality_Components_Lambda_j!K32-Inequality_Components_Lambda_j!Q32+Inequality_Components_Lambda_j!W32+Inequality_Components_Lambda_j!AC32-Inequality_Components_Lambda_j!AI32)</f>
+        <v>33.014908441953018</v>
       </c>
       <c r="F32" s="11">
-        <f>Inequality_Components_Lambda_j!F32+Inequality_Components_Lambda_j!L32-Inequality_Components_Lambda_j!R32+Inequality_Components_Lambda_j!X32+Inequality_Components_Lambda_j!AD32-Inequality_Components_Lambda_j!AJ32</f>
-        <v>101.79887288371286</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F32+Inequality_Components_Lambda_j!L32-Inequality_Components_Lambda_j!R32+Inequality_Components_Lambda_j!X32+Inequality_Components_Lambda_j!AD32-Inequality_Components_Lambda_j!AJ32)</f>
+        <v>26.415099945592207</v>
       </c>
       <c r="G32" s="11">
-        <f>Inequality_Components_Lambda_j!G32+Inequality_Components_Lambda_j!M32-Inequality_Components_Lambda_j!S32+Inequality_Components_Lambda_j!Y32+Inequality_Components_Lambda_j!AE32-Inequality_Components_Lambda_j!AK32</f>
-        <v>127.38893361339335</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G32+Inequality_Components_Lambda_j!M32-Inequality_Components_Lambda_j!S32+Inequality_Components_Lambda_j!Y32+Inequality_Components_Lambda_j!AE32-Inequality_Components_Lambda_j!AK32)</f>
+        <v>33.055291458915278</v>
       </c>
       <c r="H32" s="11">
         <f t="shared" si="1"/>
-        <v>1036.5272529889073</v>
+        <v>268.96143550929963</v>
       </c>
       <c r="I32" s="9">
         <f>(H32-H80)/Background_Calculations!$B$10</f>
-        <v>-6.4025040178944742E-8</v>
+        <v>-1.6613423974534769E-8</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4658,36 +4658,36 @@
         <v>13</v>
       </c>
       <c r="B33" s="11">
-        <f>Inequality_Components_Lambda_j!B33+Inequality_Components_Lambda_j!H33-Inequality_Components_Lambda_j!N33+Inequality_Components_Lambda_j!T33+Inequality_Components_Lambda_j!Z33-Inequality_Components_Lambda_j!AF33</f>
-        <v>466.48083800008294</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B33+Inequality_Components_Lambda_j!H33-Inequality_Components_Lambda_j!N33+Inequality_Components_Lambda_j!T33+Inequality_Components_Lambda_j!Z33-Inequality_Components_Lambda_j!AF33)</f>
+        <v>121.04395274151662</v>
       </c>
       <c r="C33" s="11">
-        <f>Inequality_Components_Lambda_j!C33+Inequality_Components_Lambda_j!I33-Inequality_Components_Lambda_j!O33+Inequality_Components_Lambda_j!U33+Inequality_Components_Lambda_j!AA33-Inequality_Components_Lambda_j!AG33</f>
-        <v>95.913220442787875</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C33+Inequality_Components_Lambda_j!I33-Inequality_Components_Lambda_j!O33+Inequality_Components_Lambda_j!U33+Inequality_Components_Lambda_j!AA33-Inequality_Components_Lambda_j!AG33)</f>
+        <v>24.887871862726797</v>
       </c>
       <c r="D33" s="11">
-        <f>Inequality_Components_Lambda_j!D33+Inequality_Components_Lambda_j!J33-Inequality_Components_Lambda_j!P33+Inequality_Components_Lambda_j!V33+Inequality_Components_Lambda_j!AB33-Inequality_Components_Lambda_j!AH33</f>
-        <v>117.62534021479136</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D33+Inequality_Components_Lambda_j!J33-Inequality_Components_Lambda_j!P33+Inequality_Components_Lambda_j!V33+Inequality_Components_Lambda_j!AB33-Inequality_Components_Lambda_j!AH33)</f>
+        <v>30.521802745864321</v>
       </c>
       <c r="E33" s="11">
-        <f>Inequality_Components_Lambda_j!E33+Inequality_Components_Lambda_j!K33-Inequality_Components_Lambda_j!Q33+Inequality_Components_Lambda_j!W33+Inequality_Components_Lambda_j!AC33-Inequality_Components_Lambda_j!AI33</f>
-        <v>127.21895920078909</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E33+Inequality_Components_Lambda_j!K33-Inequality_Components_Lambda_j!Q33+Inequality_Components_Lambda_j!W33+Inequality_Components_Lambda_j!AC33-Inequality_Components_Lambda_j!AI33)</f>
+        <v>33.011185949984309</v>
       </c>
       <c r="F33" s="11">
-        <f>Inequality_Components_Lambda_j!F33+Inequality_Components_Lambda_j!L33-Inequality_Components_Lambda_j!R33+Inequality_Components_Lambda_j!X33+Inequality_Components_Lambda_j!AD33-Inequality_Components_Lambda_j!AJ33</f>
-        <v>101.78738523021991</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F33+Inequality_Components_Lambda_j!L33-Inequality_Components_Lambda_j!R33+Inequality_Components_Lambda_j!X33+Inequality_Components_Lambda_j!AD33-Inequality_Components_Lambda_j!AJ33)</f>
+        <v>26.412119092203945</v>
       </c>
       <c r="G33" s="11">
-        <f>Inequality_Components_Lambda_j!G33+Inequality_Components_Lambda_j!M33-Inequality_Components_Lambda_j!S33+Inequality_Components_Lambda_j!Y33+Inequality_Components_Lambda_j!AE33-Inequality_Components_Lambda_j!AK33</f>
-        <v>127.37366379478286</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G33+Inequality_Components_Lambda_j!M33-Inequality_Components_Lambda_j!S33+Inequality_Components_Lambda_j!Y33+Inequality_Components_Lambda_j!AE33-Inequality_Components_Lambda_j!AK33)</f>
+        <v>33.051329197120808</v>
       </c>
       <c r="H33" s="11">
         <f t="shared" si="1"/>
-        <v>1036.399406883454</v>
+        <v>268.92826158941682</v>
       </c>
       <c r="I33" s="9">
         <f>(H33-H81)/Background_Calculations!$B$10</f>
-        <v>-7.0624686386665006E-8</v>
+        <v>-1.8325921463399175E-8</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4695,36 +4695,36 @@
         <v>14</v>
       </c>
       <c r="B34" s="11">
-        <f>Inequality_Components_Lambda_j!B34+Inequality_Components_Lambda_j!H34-Inequality_Components_Lambda_j!N34+Inequality_Components_Lambda_j!T34+Inequality_Components_Lambda_j!Z34-Inequality_Components_Lambda_j!AF34</f>
-        <v>466.42311712446804</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B34+Inequality_Components_Lambda_j!H34-Inequality_Components_Lambda_j!N34+Inequality_Components_Lambda_j!T34+Inequality_Components_Lambda_j!Z34-Inequality_Components_Lambda_j!AF34)</f>
+        <v>121.0289751425008</v>
       </c>
       <c r="C34" s="11">
-        <f>Inequality_Components_Lambda_j!C34+Inequality_Components_Lambda_j!I34-Inequality_Components_Lambda_j!O34+Inequality_Components_Lambda_j!U34+Inequality_Components_Lambda_j!AA34-Inequality_Components_Lambda_j!AG34</f>
-        <v>95.902853911160562</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C34+Inequality_Components_Lambda_j!I34-Inequality_Components_Lambda_j!O34+Inequality_Components_Lambda_j!U34+Inequality_Components_Lambda_j!AA34-Inequality_Components_Lambda_j!AG34)</f>
+        <v>24.885181921657043</v>
       </c>
       <c r="D34" s="11">
-        <f>Inequality_Components_Lambda_j!D34+Inequality_Components_Lambda_j!J34-Inequality_Components_Lambda_j!P34+Inequality_Components_Lambda_j!V34+Inequality_Components_Lambda_j!AB34-Inequality_Components_Lambda_j!AH34</f>
-        <v>117.61221665301416</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D34+Inequality_Components_Lambda_j!J34-Inequality_Components_Lambda_j!P34+Inequality_Components_Lambda_j!V34+Inequality_Components_Lambda_j!AB34-Inequality_Components_Lambda_j!AH34)</f>
+        <v>30.518397401716914</v>
       </c>
       <c r="E34" s="11">
-        <f>Inequality_Components_Lambda_j!E34+Inequality_Components_Lambda_j!K34-Inequality_Components_Lambda_j!Q34+Inequality_Components_Lambda_j!W34+Inequality_Components_Lambda_j!AC34-Inequality_Components_Lambda_j!AI34</f>
-        <v>127.20520906565307</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E34+Inequality_Components_Lambda_j!K34-Inequality_Components_Lambda_j!Q34+Inequality_Components_Lambda_j!W34+Inequality_Components_Lambda_j!AC34-Inequality_Components_Lambda_j!AI34)</f>
+        <v>33.007618020560393</v>
       </c>
       <c r="F34" s="11">
-        <f>Inequality_Components_Lambda_j!F34+Inequality_Components_Lambda_j!L34-Inequality_Components_Lambda_j!R34+Inequality_Components_Lambda_j!X34+Inequality_Components_Lambda_j!AD34-Inequality_Components_Lambda_j!AJ34</f>
-        <v>101.77637640820399</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F34+Inequality_Components_Lambda_j!L34-Inequality_Components_Lambda_j!R34+Inequality_Components_Lambda_j!X34+Inequality_Components_Lambda_j!AD34-Inequality_Components_Lambda_j!AJ34)</f>
+        <v>26.409262487552084</v>
       </c>
       <c r="G34" s="11">
-        <f>Inequality_Components_Lambda_j!G34+Inequality_Components_Lambda_j!M34-Inequality_Components_Lambda_j!S34+Inequality_Components_Lambda_j!Y34+Inequality_Components_Lambda_j!AE34-Inequality_Components_Lambda_j!AK34</f>
-        <v>127.35920172885218</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G34+Inequality_Components_Lambda_j!M34-Inequality_Components_Lambda_j!S34+Inequality_Components_Lambda_j!Y34+Inequality_Components_Lambda_j!AE34-Inequality_Components_Lambda_j!AK34)</f>
+        <v>33.047576533597557</v>
       </c>
       <c r="H34" s="11">
         <f t="shared" si="1"/>
-        <v>1036.2789748913519</v>
+        <v>268.89701150758481</v>
       </c>
       <c r="I34" s="9">
         <f>(H34-H82)/Background_Calculations!$B$10</f>
-        <v>-7.6841602710763762E-8</v>
+        <v>-1.993910696734848E-8</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4744,36 +4744,36 @@
         <v>0</v>
       </c>
       <c r="B36" s="11">
-        <f>Inequality_Components_Lambda_j!B36+Inequality_Components_Lambda_j!H36-Inequality_Components_Lambda_j!N36+Inequality_Components_Lambda_j!T36+Inequality_Components_Lambda_j!Z36-Inequality_Components_Lambda_j!AF36</f>
-        <v>469.38868762983583</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B36+Inequality_Components_Lambda_j!H36-Inequality_Components_Lambda_j!N36+Inequality_Components_Lambda_j!T36+Inequality_Components_Lambda_j!Z36-Inequality_Components_Lambda_j!AF36)</f>
+        <v>121.79849094435527</v>
       </c>
       <c r="C36" s="11">
-        <f>Inequality_Components_Lambda_j!C36+Inequality_Components_Lambda_j!I36-Inequality_Components_Lambda_j!O36+Inequality_Components_Lambda_j!U36+Inequality_Components_Lambda_j!AA36-Inequality_Components_Lambda_j!AG36</f>
-        <v>96.289075803423145</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C36+Inequality_Components_Lambda_j!I36-Inequality_Components_Lambda_j!O36+Inequality_Components_Lambda_j!U36+Inequality_Components_Lambda_j!AA36-Inequality_Components_Lambda_j!AG36)</f>
+        <v>24.985400024238061</v>
       </c>
       <c r="D36" s="11">
-        <f>Inequality_Components_Lambda_j!D36+Inequality_Components_Lambda_j!J36-Inequality_Components_Lambda_j!P36+Inequality_Components_Lambda_j!V36+Inequality_Components_Lambda_j!AB36-Inequality_Components_Lambda_j!AH36</f>
-        <v>118.15864735889694</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D36+Inequality_Components_Lambda_j!J36-Inequality_Components_Lambda_j!P36+Inequality_Components_Lambda_j!V36+Inequality_Components_Lambda_j!AB36-Inequality_Components_Lambda_j!AH36)</f>
+        <v>30.660187004100063</v>
       </c>
       <c r="E36" s="11">
-        <f>Inequality_Components_Lambda_j!E36+Inequality_Components_Lambda_j!K36-Inequality_Components_Lambda_j!Q36+Inequality_Components_Lambda_j!W36+Inequality_Components_Lambda_j!AC36-Inequality_Components_Lambda_j!AI36</f>
-        <v>127.77990064732329</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E36+Inequality_Components_Lambda_j!K36-Inequality_Components_Lambda_j!Q36+Inequality_Components_Lambda_j!W36+Inequality_Components_Lambda_j!AC36-Inequality_Components_Lambda_j!AI36)</f>
+        <v>33.156740846164276</v>
       </c>
       <c r="F36" s="11">
-        <f>Inequality_Components_Lambda_j!F36+Inequality_Components_Lambda_j!L36-Inequality_Components_Lambda_j!R36+Inequality_Components_Lambda_j!X36+Inequality_Components_Lambda_j!AD36-Inequality_Components_Lambda_j!AJ36</f>
-        <v>102.23773208628985</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F36+Inequality_Components_Lambda_j!L36-Inequality_Components_Lambda_j!R36+Inequality_Components_Lambda_j!X36+Inequality_Components_Lambda_j!AD36-Inequality_Components_Lambda_j!AJ36)</f>
+        <v>26.528976547264964</v>
       </c>
       <c r="G36" s="11">
-        <f>Inequality_Components_Lambda_j!G36+Inequality_Components_Lambda_j!M36-Inequality_Components_Lambda_j!S36+Inequality_Components_Lambda_j!Y36+Inequality_Components_Lambda_j!AE36-Inequality_Components_Lambda_j!AK36</f>
-        <v>128.23169518620074</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G36+Inequality_Components_Lambda_j!M36-Inequality_Components_Lambda_j!S36+Inequality_Components_Lambda_j!Y36+Inequality_Components_Lambda_j!AE36-Inequality_Components_Lambda_j!AK36)</f>
+        <v>33.273973950630499</v>
       </c>
       <c r="H36" s="11">
         <f>SUM(B36:G36)</f>
-        <v>1042.0857387119697</v>
+        <v>270.40376931675308</v>
       </c>
       <c r="I36" s="9">
         <f>(H36-H68)/Background_Calculations!$B$10</f>
-        <v>2.2291400339077827E-7</v>
+        <v>5.7842444734786376E-8</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4781,36 +4781,36 @@
         <v>1</v>
       </c>
       <c r="B37" s="11">
-        <f>Inequality_Components_Lambda_j!B37+Inequality_Components_Lambda_j!H37-Inequality_Components_Lambda_j!N37+Inequality_Components_Lambda_j!T37+Inequality_Components_Lambda_j!Z37-Inequality_Components_Lambda_j!AF37</f>
-        <v>468.55488859336782</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B37+Inequality_Components_Lambda_j!H37-Inequality_Components_Lambda_j!N37+Inequality_Components_Lambda_j!T37+Inequality_Components_Lambda_j!Z37-Inequality_Components_Lambda_j!AF37)</f>
+        <v>121.5821340804831</v>
       </c>
       <c r="C37" s="11">
-        <f>Inequality_Components_Lambda_j!C37+Inequality_Components_Lambda_j!I37-Inequality_Components_Lambda_j!O37+Inequality_Components_Lambda_j!U37+Inequality_Components_Lambda_j!AA37-Inequality_Components_Lambda_j!AG37</f>
-        <v>96.191009589721261</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C37+Inequality_Components_Lambda_j!I37-Inequality_Components_Lambda_j!O37+Inequality_Components_Lambda_j!U37+Inequality_Components_Lambda_j!AA37-Inequality_Components_Lambda_j!AG37)</f>
+        <v>24.959953486738769</v>
       </c>
       <c r="D37" s="11">
-        <f>Inequality_Components_Lambda_j!D37+Inequality_Components_Lambda_j!J37-Inequality_Components_Lambda_j!P37+Inequality_Components_Lambda_j!V37+Inequality_Components_Lambda_j!AB37-Inequality_Components_Lambda_j!AH37</f>
-        <v>118.01358680619921</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D37+Inequality_Components_Lambda_j!J37-Inequality_Components_Lambda_j!P37+Inequality_Components_Lambda_j!V37+Inequality_Components_Lambda_j!AB37-Inequality_Components_Lambda_j!AH37)</f>
+        <v>30.62254622391136</v>
       </c>
       <c r="E37" s="11">
-        <f>Inequality_Components_Lambda_j!E37+Inequality_Components_Lambda_j!K37-Inequality_Components_Lambda_j!Q37+Inequality_Components_Lambda_j!W37+Inequality_Components_Lambda_j!AC37-Inequality_Components_Lambda_j!AI37</f>
-        <v>127.62450510295245</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E37+Inequality_Components_Lambda_j!K37-Inequality_Components_Lambda_j!Q37+Inequality_Components_Lambda_j!W37+Inequality_Components_Lambda_j!AC37-Inequality_Components_Lambda_j!AI37)</f>
+        <v>33.116418308994888</v>
       </c>
       <c r="F37" s="11">
-        <f>Inequality_Components_Lambda_j!F37+Inequality_Components_Lambda_j!L37-Inequality_Components_Lambda_j!R37+Inequality_Components_Lambda_j!X37+Inequality_Components_Lambda_j!AD37-Inequality_Components_Lambda_j!AJ37</f>
-        <v>102.11285827106344</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F37+Inequality_Components_Lambda_j!L37-Inequality_Components_Lambda_j!R37+Inequality_Components_Lambda_j!X37+Inequality_Components_Lambda_j!AD37-Inequality_Components_Lambda_j!AJ37)</f>
+        <v>26.496573886839037</v>
       </c>
       <c r="G37" s="11">
-        <f>Inequality_Components_Lambda_j!G37+Inequality_Components_Lambda_j!M37-Inequality_Components_Lambda_j!S37+Inequality_Components_Lambda_j!Y37+Inequality_Components_Lambda_j!AE37-Inequality_Components_Lambda_j!AK37</f>
-        <v>127.96358715805469</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G37+Inequality_Components_Lambda_j!M37-Inequality_Components_Lambda_j!S37+Inequality_Components_Lambda_j!Y37+Inequality_Components_Lambda_j!AE37-Inequality_Components_Lambda_j!AK37)</f>
+        <v>33.20440441455338</v>
       </c>
       <c r="H37" s="11">
         <f t="shared" ref="H37:H50" si="2">SUM(B37:G37)</f>
-        <v>1040.4604355213589</v>
+        <v>269.98203040152055</v>
       </c>
       <c r="I37" s="9">
         <f>(H37-H69)/Background_Calculations!$B$10</f>
-        <v>1.3901292560448122E-7</v>
+        <v>3.6071522400513362E-8</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4818,36 +4818,36 @@
         <v>2</v>
       </c>
       <c r="B38" s="11">
-        <f>Inequality_Components_Lambda_j!B38+Inequality_Components_Lambda_j!H38-Inequality_Components_Lambda_j!N38+Inequality_Components_Lambda_j!T38+Inequality_Components_Lambda_j!Z38-Inequality_Components_Lambda_j!AF38</f>
-        <v>467.75610864585161</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B38+Inequality_Components_Lambda_j!H38-Inequality_Components_Lambda_j!N38+Inequality_Components_Lambda_j!T38+Inequality_Components_Lambda_j!Z38-Inequality_Components_Lambda_j!AF38)</f>
+        <v>121.37486408278599</v>
       </c>
       <c r="C38" s="11">
-        <f>Inequality_Components_Lambda_j!C38+Inequality_Components_Lambda_j!I38-Inequality_Components_Lambda_j!O38+Inequality_Components_Lambda_j!U38+Inequality_Components_Lambda_j!AA38-Inequality_Components_Lambda_j!AG38</f>
-        <v>96.096899564383619</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C38+Inequality_Components_Lambda_j!I38-Inequality_Components_Lambda_j!O38+Inequality_Components_Lambda_j!U38+Inequality_Components_Lambda_j!AA38-Inequality_Components_Lambda_j!AG38)</f>
+        <v>24.935533513759147</v>
       </c>
       <c r="D38" s="11">
-        <f>Inequality_Components_Lambda_j!D38+Inequality_Components_Lambda_j!J38-Inequality_Components_Lambda_j!P38+Inequality_Components_Lambda_j!V38+Inequality_Components_Lambda_j!AB38-Inequality_Components_Lambda_j!AH38</f>
-        <v>117.87447801496675</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D38+Inequality_Components_Lambda_j!J38-Inequality_Components_Lambda_j!P38+Inequality_Components_Lambda_j!V38+Inequality_Components_Lambda_j!AB38-Inequality_Components_Lambda_j!AH38)</f>
+        <v>30.586449825988435</v>
       </c>
       <c r="E38" s="11">
-        <f>Inequality_Components_Lambda_j!E38+Inequality_Components_Lambda_j!K38-Inequality_Components_Lambda_j!Q38+Inequality_Components_Lambda_j!W38+Inequality_Components_Lambda_j!AC38-Inequality_Components_Lambda_j!AI38</f>
-        <v>127.47549636035869</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E38+Inequality_Components_Lambda_j!K38-Inequality_Components_Lambda_j!Q38+Inequality_Components_Lambda_j!W38+Inequality_Components_Lambda_j!AC38-Inequality_Components_Lambda_j!AI38)</f>
+        <v>33.077753039754846</v>
       </c>
       <c r="F38" s="11">
-        <f>Inequality_Components_Lambda_j!F38+Inequality_Components_Lambda_j!L38-Inequality_Components_Lambda_j!R38+Inequality_Components_Lambda_j!X38+Inequality_Components_Lambda_j!AD38-Inequality_Components_Lambda_j!AJ38</f>
-        <v>101.99311863664047</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F38+Inequality_Components_Lambda_j!L38-Inequality_Components_Lambda_j!R38+Inequality_Components_Lambda_j!X38+Inequality_Components_Lambda_j!AD38-Inequality_Components_Lambda_j!AJ38)</f>
+        <v>26.465503460211185</v>
       </c>
       <c r="G38" s="11">
-        <f>Inequality_Components_Lambda_j!G38+Inequality_Components_Lambda_j!M38-Inequality_Components_Lambda_j!S38+Inequality_Components_Lambda_j!Y38+Inequality_Components_Lambda_j!AE38-Inequality_Components_Lambda_j!AK38</f>
-        <v>127.70691023304958</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G38+Inequality_Components_Lambda_j!M38-Inequality_Components_Lambda_j!S38+Inequality_Components_Lambda_j!Y38+Inequality_Components_Lambda_j!AE38-Inequality_Components_Lambda_j!AK38)</f>
+        <v>33.137801057996754</v>
       </c>
       <c r="H38" s="11">
         <f t="shared" si="2"/>
-        <v>1038.9030114552506</v>
+        <v>269.57790498049633</v>
       </c>
       <c r="I38" s="9">
         <f>(H38-H70)/Background_Calculations!$B$10</f>
-        <v>5.8615890471794848E-8</v>
+        <v>1.5209840358265701E-8</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4855,36 +4855,36 @@
         <v>3</v>
       </c>
       <c r="B39" s="11">
-        <f>Inequality_Components_Lambda_j!B39+Inequality_Components_Lambda_j!H39-Inequality_Components_Lambda_j!N39+Inequality_Components_Lambda_j!T39+Inequality_Components_Lambda_j!Z39-Inequality_Components_Lambda_j!AF39</f>
-        <v>467.36972625530865</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B39+Inequality_Components_Lambda_j!H39-Inequality_Components_Lambda_j!N39+Inequality_Components_Lambda_j!T39+Inequality_Components_Lambda_j!Z39-Inequality_Components_Lambda_j!AF39)</f>
+        <v>121.2746043335934</v>
       </c>
       <c r="C39" s="11">
-        <f>Inequality_Components_Lambda_j!C39+Inequality_Components_Lambda_j!I39-Inequality_Components_Lambda_j!O39+Inequality_Components_Lambda_j!U39+Inequality_Components_Lambda_j!AA39-Inequality_Components_Lambda_j!AG39</f>
-        <v>96.049321624493658</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C39+Inequality_Components_Lambda_j!I39-Inequality_Components_Lambda_j!O39+Inequality_Components_Lambda_j!U39+Inequality_Components_Lambda_j!AA39-Inequality_Components_Lambda_j!AG39)</f>
+        <v>24.923187836427001</v>
       </c>
       <c r="D39" s="11">
-        <f>Inequality_Components_Lambda_j!D39+Inequality_Components_Lambda_j!J39-Inequality_Components_Lambda_j!P39+Inequality_Components_Lambda_j!V39+Inequality_Components_Lambda_j!AB39-Inequality_Components_Lambda_j!AH39</f>
-        <v>117.80537293629068</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D39+Inequality_Components_Lambda_j!J39-Inequality_Components_Lambda_j!P39+Inequality_Components_Lambda_j!V39+Inequality_Components_Lambda_j!AB39-Inequality_Components_Lambda_j!AH39)</f>
+        <v>30.568518217236129</v>
       </c>
       <c r="E39" s="11">
-        <f>Inequality_Components_Lambda_j!E39+Inequality_Components_Lambda_j!K39-Inequality_Components_Lambda_j!Q39+Inequality_Components_Lambda_j!W39+Inequality_Components_Lambda_j!AC39-Inequality_Components_Lambda_j!AI39</f>
-        <v>127.40145572276273</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E39+Inequality_Components_Lambda_j!K39-Inequality_Components_Lambda_j!Q39+Inequality_Components_Lambda_j!W39+Inequality_Components_Lambda_j!AC39-Inequality_Components_Lambda_j!AI39)</f>
+        <v>33.05854073625158</v>
       </c>
       <c r="F39" s="11">
-        <f>Inequality_Components_Lambda_j!F39+Inequality_Components_Lambda_j!L39-Inequality_Components_Lambda_j!R39+Inequality_Components_Lambda_j!X39+Inequality_Components_Lambda_j!AD39-Inequality_Components_Lambda_j!AJ39</f>
-        <v>101.93364387640356</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F39+Inequality_Components_Lambda_j!L39-Inequality_Components_Lambda_j!R39+Inequality_Components_Lambda_j!X39+Inequality_Components_Lambda_j!AD39-Inequality_Components_Lambda_j!AJ39)</f>
+        <v>26.450070757555501</v>
       </c>
       <c r="G39" s="11">
-        <f>Inequality_Components_Lambda_j!G39+Inequality_Components_Lambda_j!M39-Inequality_Components_Lambda_j!S39+Inequality_Components_Lambda_j!Y39+Inequality_Components_Lambda_j!AE39-Inequality_Components_Lambda_j!AK39</f>
-        <v>127.58410688267244</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G39+Inequality_Components_Lambda_j!M39-Inequality_Components_Lambda_j!S39+Inequality_Components_Lambda_j!Y39+Inequality_Components_Lambda_j!AE39-Inequality_Components_Lambda_j!AK39)</f>
+        <v>33.105935648469362</v>
       </c>
       <c r="H39" s="11">
         <f t="shared" si="2"/>
-        <v>1038.1436272979317</v>
+        <v>269.38085752953293</v>
       </c>
       <c r="I39" s="9">
         <f>(H39-H71)/Background_Calculations!$B$10</f>
-        <v>1.9415112659409993E-8</v>
+        <v>5.0378960672694617E-9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4892,36 +4892,36 @@
         <v>4</v>
       </c>
       <c r="B40" s="11">
-        <f>Inequality_Components_Lambda_j!B40+Inequality_Components_Lambda_j!H40-Inequality_Components_Lambda_j!N40+Inequality_Components_Lambda_j!T40+Inequality_Components_Lambda_j!Z40-Inequality_Components_Lambda_j!AF40</f>
-        <v>467.29447353150891</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B40+Inequality_Components_Lambda_j!H40-Inequality_Components_Lambda_j!N40+Inequality_Components_Lambda_j!T40+Inequality_Components_Lambda_j!Z40-Inequality_Components_Lambda_j!AF40)</f>
+        <v>121.25507751405171</v>
       </c>
       <c r="C40" s="11">
-        <f>Inequality_Components_Lambda_j!C40+Inequality_Components_Lambda_j!I40-Inequality_Components_Lambda_j!O40+Inequality_Components_Lambda_j!U40+Inequality_Components_Lambda_j!AA40-Inequality_Components_Lambda_j!AG40</f>
-        <v>96.036850166336095</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C40+Inequality_Components_Lambda_j!I40-Inequality_Components_Lambda_j!O40+Inequality_Components_Lambda_j!U40+Inequality_Components_Lambda_j!AA40-Inequality_Components_Lambda_j!AG40)</f>
+        <v>24.919951702230549</v>
       </c>
       <c r="D40" s="11">
-        <f>Inequality_Components_Lambda_j!D40+Inequality_Components_Lambda_j!J40-Inequality_Components_Lambda_j!P40+Inequality_Components_Lambda_j!V40+Inequality_Components_Lambda_j!AB40-Inequality_Components_Lambda_j!AH40</f>
-        <v>117.78908268489801</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D40+Inequality_Components_Lambda_j!J40-Inequality_Components_Lambda_j!P40+Inequality_Components_Lambda_j!V40+Inequality_Components_Lambda_j!AB40-Inequality_Components_Lambda_j!AH40)</f>
+        <v>30.564291170251355</v>
       </c>
       <c r="E40" s="11">
-        <f>Inequality_Components_Lambda_j!E40+Inequality_Components_Lambda_j!K40-Inequality_Components_Lambda_j!Q40+Inequality_Components_Lambda_j!W40+Inequality_Components_Lambda_j!AC40-Inequality_Components_Lambda_j!AI40</f>
-        <v>127.38397736660258</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E40+Inequality_Components_Lambda_j!K40-Inequality_Components_Lambda_j!Q40+Inequality_Components_Lambda_j!W40+Inequality_Components_Lambda_j!AC40-Inequality_Components_Lambda_j!AI40)</f>
+        <v>33.05400539600884</v>
       </c>
       <c r="F40" s="11">
-        <f>Inequality_Components_Lambda_j!F40+Inequality_Components_Lambda_j!L40-Inequality_Components_Lambda_j!R40+Inequality_Components_Lambda_j!X40+Inequality_Components_Lambda_j!AD40-Inequality_Components_Lambda_j!AJ40</f>
-        <v>101.91963803624287</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F40+Inequality_Components_Lambda_j!L40-Inequality_Components_Lambda_j!R40+Inequality_Components_Lambda_j!X40+Inequality_Components_Lambda_j!AD40-Inequality_Components_Lambda_j!AJ40)</f>
+        <v>26.446436476966859</v>
       </c>
       <c r="G40" s="11">
-        <f>Inequality_Components_Lambda_j!G40+Inequality_Components_Lambda_j!M40-Inequality_Components_Lambda_j!S40+Inequality_Components_Lambda_j!Y40+Inequality_Components_Lambda_j!AE40-Inequality_Components_Lambda_j!AK40</f>
-        <v>127.56231314655865</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G40+Inequality_Components_Lambda_j!M40-Inequality_Components_Lambda_j!S40+Inequality_Components_Lambda_j!Y40+Inequality_Components_Lambda_j!AE40-Inequality_Components_Lambda_j!AK40)</f>
+        <v>33.100280539514564</v>
       </c>
       <c r="H40" s="11">
         <f t="shared" si="2"/>
-        <v>1037.9863349321472</v>
+        <v>269.34004279902388</v>
       </c>
       <c r="I40" s="9">
         <f>(H40-H72)/Background_Calculations!$B$10</f>
-        <v>1.1295397462198024E-8</v>
+        <v>2.9309661731737708E-9</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4929,36 +4929,36 @@
         <v>5</v>
       </c>
       <c r="B41" s="11">
-        <f>Inequality_Components_Lambda_j!B41+Inequality_Components_Lambda_j!H41-Inequality_Components_Lambda_j!N41+Inequality_Components_Lambda_j!T41+Inequality_Components_Lambda_j!Z41-Inequality_Components_Lambda_j!AF41</f>
-        <v>467.2145979112729</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B41+Inequality_Components_Lambda_j!H41-Inequality_Components_Lambda_j!N41+Inequality_Components_Lambda_j!T41+Inequality_Components_Lambda_j!Z41-Inequality_Components_Lambda_j!AF41)</f>
+        <v>121.23435113042898</v>
       </c>
       <c r="C41" s="11">
-        <f>Inequality_Components_Lambda_j!C41+Inequality_Components_Lambda_j!I41-Inequality_Components_Lambda_j!O41+Inequality_Components_Lambda_j!U41+Inequality_Components_Lambda_j!AA41-Inequality_Components_Lambda_j!AG41</f>
-        <v>96.023974158925299</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C41+Inequality_Components_Lambda_j!I41-Inequality_Components_Lambda_j!O41+Inequality_Components_Lambda_j!U41+Inequality_Components_Lambda_j!AA41-Inequality_Components_Lambda_j!AG41)</f>
+        <v>24.916610594288763</v>
       </c>
       <c r="D41" s="11">
-        <f>Inequality_Components_Lambda_j!D41+Inequality_Components_Lambda_j!J41-Inequality_Components_Lambda_j!P41+Inequality_Components_Lambda_j!V41+Inequality_Components_Lambda_j!AB41-Inequality_Components_Lambda_j!AH41</f>
-        <v>117.77218382227788</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D41+Inequality_Components_Lambda_j!J41-Inequality_Components_Lambda_j!P41+Inequality_Components_Lambda_j!V41+Inequality_Components_Lambda_j!AB41-Inequality_Components_Lambda_j!AH41)</f>
+        <v>30.559906198861867</v>
       </c>
       <c r="E41" s="11">
-        <f>Inequality_Components_Lambda_j!E41+Inequality_Components_Lambda_j!K41-Inequality_Components_Lambda_j!Q41+Inequality_Components_Lambda_j!W41+Inequality_Components_Lambda_j!AC41-Inequality_Components_Lambda_j!AI41</f>
-        <v>127.36615844701882</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E41+Inequality_Components_Lambda_j!K41-Inequality_Components_Lambda_j!Q41+Inequality_Components_Lambda_j!W41+Inequality_Components_Lambda_j!AC41-Inequality_Components_Lambda_j!AI41)</f>
+        <v>33.049381685270262</v>
       </c>
       <c r="F41" s="11">
-        <f>Inequality_Components_Lambda_j!F41+Inequality_Components_Lambda_j!L41-Inequality_Components_Lambda_j!R41+Inequality_Components_Lambda_j!X41+Inequality_Components_Lambda_j!AD41-Inequality_Components_Lambda_j!AJ41</f>
-        <v>101.90535842616525</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F41+Inequality_Components_Lambda_j!L41-Inequality_Components_Lambda_j!R41+Inequality_Components_Lambda_j!X41+Inequality_Components_Lambda_j!AD41-Inequality_Components_Lambda_j!AJ41)</f>
+        <v>26.442731157676977</v>
       </c>
       <c r="G41" s="11">
-        <f>Inequality_Components_Lambda_j!G41+Inequality_Components_Lambda_j!M41-Inequality_Components_Lambda_j!S41+Inequality_Components_Lambda_j!Y41+Inequality_Components_Lambda_j!AE41-Inequality_Components_Lambda_j!AK41</f>
-        <v>127.54053377156696</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G41+Inequality_Components_Lambda_j!M41-Inequality_Components_Lambda_j!S41+Inequality_Components_Lambda_j!Y41+Inequality_Components_Lambda_j!AE41-Inequality_Components_Lambda_j!AK41)</f>
+        <v>33.094629157030049</v>
       </c>
       <c r="H41" s="11">
         <f t="shared" si="2"/>
-        <v>1037.8228065372271</v>
+        <v>269.29760992355688</v>
       </c>
       <c r="I41" s="9">
         <f>(H41-H73)/Background_Calculations!$B$10</f>
-        <v>2.8537672102401334E-9</v>
+        <v>7.4050472215360434E-10</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4966,36 +4966,36 @@
         <v>6</v>
       </c>
       <c r="B42" s="11">
-        <f>Inequality_Components_Lambda_j!B42+Inequality_Components_Lambda_j!H42-Inequality_Components_Lambda_j!N42+Inequality_Components_Lambda_j!T42+Inequality_Components_Lambda_j!Z42-Inequality_Components_Lambda_j!AF42</f>
-        <v>467.11813070049413</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B42+Inequality_Components_Lambda_j!H42-Inequality_Components_Lambda_j!N42+Inequality_Components_Lambda_j!T42+Inequality_Components_Lambda_j!Z42-Inequality_Components_Lambda_j!AF42)</f>
+        <v>121.20931950736666</v>
       </c>
       <c r="C42" s="11">
-        <f>Inequality_Components_Lambda_j!C42+Inequality_Components_Lambda_j!I42-Inequality_Components_Lambda_j!O42+Inequality_Components_Lambda_j!U42+Inequality_Components_Lambda_j!AA42-Inequality_Components_Lambda_j!AG42</f>
-        <v>96.009556837847271</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C42+Inequality_Components_Lambda_j!I42-Inequality_Components_Lambda_j!O42+Inequality_Components_Lambda_j!U42+Inequality_Components_Lambda_j!AA42-Inequality_Components_Lambda_j!AG42)</f>
+        <v>24.912869541304229</v>
       </c>
       <c r="D42" s="11">
-        <f>Inequality_Components_Lambda_j!D42+Inequality_Components_Lambda_j!J42-Inequality_Components_Lambda_j!P42+Inequality_Components_Lambda_j!V42+Inequality_Components_Lambda_j!AB42-Inequality_Components_Lambda_j!AH42</f>
-        <v>117.75296617944669</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D42+Inequality_Components_Lambda_j!J42-Inequality_Components_Lambda_j!P42+Inequality_Components_Lambda_j!V42+Inequality_Components_Lambda_j!AB42-Inequality_Components_Lambda_j!AH42)</f>
+        <v>30.554919542902674</v>
       </c>
       <c r="E42" s="11">
-        <f>Inequality_Components_Lambda_j!E42+Inequality_Components_Lambda_j!K42-Inequality_Components_Lambda_j!Q42+Inequality_Components_Lambda_j!W42+Inequality_Components_Lambda_j!AC42-Inequality_Components_Lambda_j!AI42</f>
-        <v>127.34673561499149</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E42+Inequality_Components_Lambda_j!K42-Inequality_Components_Lambda_j!Q42+Inequality_Components_Lambda_j!W42+Inequality_Components_Lambda_j!AC42-Inequality_Components_Lambda_j!AI42)</f>
+        <v>33.044341786156501</v>
       </c>
       <c r="F42" s="11">
-        <f>Inequality_Components_Lambda_j!F42+Inequality_Components_Lambda_j!L42-Inequality_Components_Lambda_j!R42+Inequality_Components_Lambda_j!X42+Inequality_Components_Lambda_j!AD42-Inequality_Components_Lambda_j!AJ42</f>
-        <v>101.88978947335154</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F42+Inequality_Components_Lambda_j!L42-Inequality_Components_Lambda_j!R42+Inequality_Components_Lambda_j!X42+Inequality_Components_Lambda_j!AD42-Inequality_Components_Lambda_j!AJ42)</f>
+        <v>26.438691275574431</v>
       </c>
       <c r="G42" s="11">
-        <f>Inequality_Components_Lambda_j!G42+Inequality_Components_Lambda_j!M42-Inequality_Components_Lambda_j!S42+Inequality_Components_Lambda_j!Y42+Inequality_Components_Lambda_j!AE42-Inequality_Components_Lambda_j!AK42</f>
-        <v>127.5176491287919</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G42+Inequality_Components_Lambda_j!M42-Inequality_Components_Lambda_j!S42+Inequality_Components_Lambda_j!Y42+Inequality_Components_Lambda_j!AE42-Inequality_Components_Lambda_j!AK42)</f>
+        <v>33.088690976095442</v>
       </c>
       <c r="H42" s="11">
         <f t="shared" si="2"/>
-        <v>1037.6348279349231</v>
+        <v>269.24883262939994</v>
       </c>
       <c r="I42" s="9">
         <f>(H42-H74)/Background_Calculations!$B$10</f>
-        <v>-6.8500267804271121E-9</v>
+        <v>-1.7774670476108457E-9</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -5003,36 +5003,36 @@
         <v>7</v>
       </c>
       <c r="B43" s="11">
-        <f>Inequality_Components_Lambda_j!B43+Inequality_Components_Lambda_j!H43-Inequality_Components_Lambda_j!N43+Inequality_Components_Lambda_j!T43+Inequality_Components_Lambda_j!Z43-Inequality_Components_Lambda_j!AF43</f>
-        <v>467.01322117159253</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B43+Inequality_Components_Lambda_j!H43-Inequality_Components_Lambda_j!N43+Inequality_Components_Lambda_j!T43+Inequality_Components_Lambda_j!Z43-Inequality_Components_Lambda_j!AF43)</f>
+        <v>121.18209724436237</v>
       </c>
       <c r="C43" s="11">
-        <f>Inequality_Components_Lambda_j!C43+Inequality_Components_Lambda_j!I43-Inequality_Components_Lambda_j!O43+Inequality_Components_Lambda_j!U43+Inequality_Components_Lambda_j!AA43-Inequality_Components_Lambda_j!AG43</f>
-        <v>95.994381206249926</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C43+Inequality_Components_Lambda_j!I43-Inequality_Components_Lambda_j!O43+Inequality_Components_Lambda_j!U43+Inequality_Components_Lambda_j!AA43-Inequality_Components_Lambda_j!AG43)</f>
+        <v>24.908931719459787</v>
       </c>
       <c r="D43" s="11">
-        <f>Inequality_Components_Lambda_j!D43+Inequality_Components_Lambda_j!J43-Inequality_Components_Lambda_j!P43+Inequality_Components_Lambda_j!V43+Inequality_Components_Lambda_j!AB43-Inequality_Components_Lambda_j!AH43</f>
-        <v>117.73260772052883</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D43+Inequality_Components_Lambda_j!J43-Inequality_Components_Lambda_j!P43+Inequality_Components_Lambda_j!V43+Inequality_Components_Lambda_j!AB43-Inequality_Components_Lambda_j!AH43)</f>
+        <v>30.549636864304968</v>
       </c>
       <c r="E43" s="11">
-        <f>Inequality_Components_Lambda_j!E43+Inequality_Components_Lambda_j!K43-Inequality_Components_Lambda_j!Q43+Inequality_Components_Lambda_j!W43+Inequality_Components_Lambda_j!AC43-Inequality_Components_Lambda_j!AI43</f>
-        <v>127.32660748945713</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E43+Inequality_Components_Lambda_j!K43-Inequality_Components_Lambda_j!Q43+Inequality_Components_Lambda_j!W43+Inequality_Components_Lambda_j!AC43-Inequality_Components_Lambda_j!AI43)</f>
+        <v>33.039118875208217</v>
       </c>
       <c r="F43" s="11">
-        <f>Inequality_Components_Lambda_j!F43+Inequality_Components_Lambda_j!L43-Inequality_Components_Lambda_j!R43+Inequality_Components_Lambda_j!X43+Inequality_Components_Lambda_j!AD43-Inequality_Components_Lambda_j!AJ43</f>
-        <v>101.87365355376622</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F43+Inequality_Components_Lambda_j!L43-Inequality_Components_Lambda_j!R43+Inequality_Components_Lambda_j!X43+Inequality_Components_Lambda_j!AD43-Inequality_Components_Lambda_j!AJ43)</f>
+        <v>26.434504275104914</v>
       </c>
       <c r="G43" s="11">
-        <f>Inequality_Components_Lambda_j!G43+Inequality_Components_Lambda_j!M43-Inequality_Components_Lambda_j!S43+Inequality_Components_Lambda_j!Y43+Inequality_Components_Lambda_j!AE43-Inequality_Components_Lambda_j!AK43</f>
-        <v>127.49453803496654</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G43+Inequality_Components_Lambda_j!M43-Inequality_Components_Lambda_j!S43+Inequality_Components_Lambda_j!Y43+Inequality_Components_Lambda_j!AE43-Inequality_Components_Lambda_j!AK43)</f>
+        <v>33.082694034911761</v>
       </c>
       <c r="H43" s="11">
         <f t="shared" si="2"/>
-        <v>1037.4350091765612</v>
+        <v>269.19698301335205</v>
       </c>
       <c r="I43" s="9">
         <f>(H43-H75)/Background_Calculations!$B$10</f>
-        <v>-1.7165030950319061E-8</v>
+        <v>-4.4540376064791487E-9</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -5040,36 +5040,36 @@
         <v>8</v>
       </c>
       <c r="B44" s="11">
-        <f>Inequality_Components_Lambda_j!B44+Inequality_Components_Lambda_j!H44-Inequality_Components_Lambda_j!N44+Inequality_Components_Lambda_j!T44+Inequality_Components_Lambda_j!Z44-Inequality_Components_Lambda_j!AF44</f>
-        <v>466.90713695775338</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B44+Inequality_Components_Lambda_j!H44-Inequality_Components_Lambda_j!N44+Inequality_Components_Lambda_j!T44+Inequality_Components_Lambda_j!Z44-Inequality_Components_Lambda_j!AF44)</f>
+        <v>121.15457017032087</v>
       </c>
       <c r="C44" s="11">
-        <f>Inequality_Components_Lambda_j!C44+Inequality_Components_Lambda_j!I44-Inequality_Components_Lambda_j!O44+Inequality_Components_Lambda_j!U44+Inequality_Components_Lambda_j!AA44-Inequality_Components_Lambda_j!AG44</f>
-        <v>95.979085859913894</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C44+Inequality_Components_Lambda_j!I44-Inequality_Components_Lambda_j!O44+Inequality_Components_Lambda_j!U44+Inequality_Components_Lambda_j!AA44-Inequality_Components_Lambda_j!AG44)</f>
+        <v>24.904962833648739</v>
       </c>
       <c r="D44" s="11">
-        <f>Inequality_Components_Lambda_j!D44+Inequality_Components_Lambda_j!J44-Inequality_Components_Lambda_j!P44+Inequality_Components_Lambda_j!V44+Inequality_Components_Lambda_j!AB44-Inequality_Components_Lambda_j!AH44</f>
-        <v>117.71206916058871</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D44+Inequality_Components_Lambda_j!J44-Inequality_Components_Lambda_j!P44+Inequality_Components_Lambda_j!V44+Inequality_Components_Lambda_j!AB44-Inequality_Components_Lambda_j!AH44)</f>
+        <v>30.544307452512985</v>
       </c>
       <c r="E44" s="11">
-        <f>Inequality_Components_Lambda_j!E44+Inequality_Components_Lambda_j!K44-Inequality_Components_Lambda_j!Q44+Inequality_Components_Lambda_j!W44+Inequality_Components_Lambda_j!AC44-Inequality_Components_Lambda_j!AI44</f>
-        <v>127.30632059420314</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E44+Inequality_Components_Lambda_j!K44-Inequality_Components_Lambda_j!Q44+Inequality_Components_Lambda_j!W44+Inequality_Components_Lambda_j!AC44-Inequality_Components_Lambda_j!AI44)</f>
+        <v>33.03385476618088</v>
       </c>
       <c r="F44" s="11">
-        <f>Inequality_Components_Lambda_j!F44+Inequality_Components_Lambda_j!L44-Inequality_Components_Lambda_j!R44+Inequality_Components_Lambda_j!X44+Inequality_Components_Lambda_j!AD44-Inequality_Components_Lambda_j!AJ44</f>
-        <v>101.85739000340806</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F44+Inequality_Components_Lambda_j!L44-Inequality_Components_Lambda_j!R44+Inequality_Components_Lambda_j!X44+Inequality_Components_Lambda_j!AD44-Inequality_Components_Lambda_j!AJ44)</f>
+        <v>26.430284156590716</v>
       </c>
       <c r="G44" s="11">
-        <f>Inequality_Components_Lambda_j!G44+Inequality_Components_Lambda_j!M44-Inequality_Components_Lambda_j!S44+Inequality_Components_Lambda_j!Y44+Inequality_Components_Lambda_j!AE44-Inequality_Components_Lambda_j!AK44</f>
-        <v>127.47121163762893</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G44+Inequality_Components_Lambda_j!M44-Inequality_Components_Lambda_j!S44+Inequality_Components_Lambda_j!Y44+Inequality_Components_Lambda_j!AE44-Inequality_Components_Lambda_j!AK44)</f>
+        <v>33.076641226078138</v>
       </c>
       <c r="H44" s="11">
         <f t="shared" si="2"/>
-        <v>1037.233214213496</v>
+        <v>269.14462060533231</v>
       </c>
       <c r="I44" s="9">
         <f>(H44-H76)/Background_Calculations!$B$10</f>
-        <v>-2.7582050366031039E-8</v>
+        <v>-7.1570794104465488E-9</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -5077,36 +5077,36 @@
         <v>9</v>
       </c>
       <c r="B45" s="11">
-        <f>Inequality_Components_Lambda_j!B45+Inequality_Components_Lambda_j!H45-Inequality_Components_Lambda_j!N45+Inequality_Components_Lambda_j!T45+Inequality_Components_Lambda_j!Z45-Inequality_Components_Lambda_j!AF45</f>
-        <v>466.80653292871926</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B45+Inequality_Components_Lambda_j!H45-Inequality_Components_Lambda_j!N45+Inequality_Components_Lambda_j!T45+Inequality_Components_Lambda_j!Z45-Inequality_Components_Lambda_j!AF45)</f>
+        <v>121.12846511231201</v>
       </c>
       <c r="C45" s="11">
-        <f>Inequality_Components_Lambda_j!C45+Inequality_Components_Lambda_j!I45-Inequality_Components_Lambda_j!O45+Inequality_Components_Lambda_j!U45+Inequality_Components_Lambda_j!AA45-Inequality_Components_Lambda_j!AG45</f>
-        <v>95.964349011325623</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C45+Inequality_Components_Lambda_j!I45-Inequality_Components_Lambda_j!O45+Inequality_Components_Lambda_j!U45+Inequality_Components_Lambda_j!AA45-Inequality_Components_Lambda_j!AG45)</f>
+        <v>24.90113886863503</v>
       </c>
       <c r="D45" s="11">
-        <f>Inequality_Components_Lambda_j!D45+Inequality_Components_Lambda_j!J45-Inequality_Components_Lambda_j!P45+Inequality_Components_Lambda_j!V45+Inequality_Components_Lambda_j!AB45-Inequality_Components_Lambda_j!AH45</f>
-        <v>117.69237081478092</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D45+Inequality_Components_Lambda_j!J45-Inequality_Components_Lambda_j!P45+Inequality_Components_Lambda_j!V45+Inequality_Components_Lambda_j!AB45-Inequality_Components_Lambda_j!AH45)</f>
+        <v>30.539196062194645</v>
       </c>
       <c r="E45" s="11">
-        <f>Inequality_Components_Lambda_j!E45+Inequality_Components_Lambda_j!K45-Inequality_Components_Lambda_j!Q45+Inequality_Components_Lambda_j!W45+Inequality_Components_Lambda_j!AC45-Inequality_Components_Lambda_j!AI45</f>
-        <v>127.28677439747798</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E45+Inequality_Components_Lambda_j!K45-Inequality_Components_Lambda_j!Q45+Inequality_Components_Lambda_j!W45+Inequality_Components_Lambda_j!AC45-Inequality_Components_Lambda_j!AI45)</f>
+        <v>33.028782855997342</v>
       </c>
       <c r="F45" s="11">
-        <f>Inequality_Components_Lambda_j!F45+Inequality_Components_Lambda_j!L45-Inequality_Components_Lambda_j!R45+Inequality_Components_Lambda_j!X45+Inequality_Components_Lambda_j!AD45-Inequality_Components_Lambda_j!AJ45</f>
-        <v>101.84172188098088</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F45+Inequality_Components_Lambda_j!L45-Inequality_Components_Lambda_j!R45+Inequality_Components_Lambda_j!X45+Inequality_Components_Lambda_j!AD45-Inequality_Components_Lambda_j!AJ45)</f>
+        <v>26.426218541636942</v>
       </c>
       <c r="G45" s="11">
-        <f>Inequality_Components_Lambda_j!G45+Inequality_Components_Lambda_j!M45-Inequality_Components_Lambda_j!S45+Inequality_Components_Lambda_j!Y45+Inequality_Components_Lambda_j!AE45-Inequality_Components_Lambda_j!AK45</f>
-        <v>127.44888968241766</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G45+Inequality_Components_Lambda_j!M45-Inequality_Components_Lambda_j!S45+Inequality_Components_Lambda_j!Y45+Inequality_Components_Lambda_j!AE45-Inequality_Components_Lambda_j!AK45)</f>
+        <v>33.070849053127851</v>
       </c>
       <c r="H45" s="11">
         <f t="shared" si="2"/>
-        <v>1037.0406387157025</v>
+        <v>269.09465049390383</v>
       </c>
       <c r="I45" s="9">
         <f>(H45-H77)/Background_Calculations!$B$10</f>
-        <v>-3.7523144380643058E-8</v>
+        <v>-9.7366265559703157E-9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -5114,36 +5114,36 @@
         <v>10</v>
       </c>
       <c r="B46" s="11">
-        <f>Inequality_Components_Lambda_j!B46+Inequality_Components_Lambda_j!H46-Inequality_Components_Lambda_j!N46+Inequality_Components_Lambda_j!T46+Inequality_Components_Lambda_j!Z46-Inequality_Components_Lambda_j!AF46</f>
-        <v>466.71443900326869</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B46+Inequality_Components_Lambda_j!H46-Inequality_Components_Lambda_j!N46+Inequality_Components_Lambda_j!T46+Inequality_Components_Lambda_j!Z46-Inequality_Components_Lambda_j!AF46)</f>
+        <v>121.10456828343516</v>
       </c>
       <c r="C46" s="11">
-        <f>Inequality_Components_Lambda_j!C46+Inequality_Components_Lambda_j!I46-Inequality_Components_Lambda_j!O46+Inequality_Components_Lambda_j!U46+Inequality_Components_Lambda_j!AA46-Inequality_Components_Lambda_j!AG46</f>
-        <v>95.950479446205705</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C46+Inequality_Components_Lambda_j!I46-Inequality_Components_Lambda_j!O46+Inequality_Components_Lambda_j!U46+Inequality_Components_Lambda_j!AA46-Inequality_Components_Lambda_j!AG46)</f>
+        <v>24.897539949133602</v>
       </c>
       <c r="D46" s="11">
-        <f>Inequality_Components_Lambda_j!D46+Inequality_Components_Lambda_j!J46-Inequality_Components_Lambda_j!P46+Inequality_Components_Lambda_j!V46+Inequality_Components_Lambda_j!AB46-Inequality_Components_Lambda_j!AH46</f>
-        <v>117.67397722593896</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D46+Inequality_Components_Lambda_j!J46-Inequality_Components_Lambda_j!P46+Inequality_Components_Lambda_j!V46+Inequality_Components_Lambda_j!AB46-Inequality_Components_Lambda_j!AH46)</f>
+        <v>30.534423234423031</v>
       </c>
       <c r="E46" s="11">
-        <f>Inequality_Components_Lambda_j!E46+Inequality_Components_Lambda_j!K46-Inequality_Components_Lambda_j!Q46+Inequality_Components_Lambda_j!W46+Inequality_Components_Lambda_j!AC46-Inequality_Components_Lambda_j!AI46</f>
-        <v>127.26837842130723</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E46+Inequality_Components_Lambda_j!K46-Inequality_Components_Lambda_j!Q46+Inequality_Components_Lambda_j!W46+Inequality_Components_Lambda_j!AC46-Inequality_Components_Lambda_j!AI46)</f>
+        <v>33.024009408753948</v>
       </c>
       <c r="F46" s="11">
-        <f>Inequality_Components_Lambda_j!F46+Inequality_Components_Lambda_j!L46-Inequality_Components_Lambda_j!R46+Inequality_Components_Lambda_j!X46+Inequality_Components_Lambda_j!AD46-Inequality_Components_Lambda_j!AJ46</f>
-        <v>101.82697839039552</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F46+Inequality_Components_Lambda_j!L46-Inequality_Components_Lambda_j!R46+Inequality_Components_Lambda_j!X46+Inequality_Components_Lambda_j!AD46-Inequality_Components_Lambda_j!AJ46)</f>
+        <v>26.422392853136401</v>
       </c>
       <c r="G46" s="11">
-        <f>Inequality_Components_Lambda_j!G46+Inequality_Components_Lambda_j!M46-Inequality_Components_Lambda_j!S46+Inequality_Components_Lambda_j!Y46+Inequality_Components_Lambda_j!AE46-Inequality_Components_Lambda_j!AK46</f>
-        <v>127.42812751156458</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G46+Inequality_Components_Lambda_j!M46-Inequality_Components_Lambda_j!S46+Inequality_Components_Lambda_j!Y46+Inequality_Components_Lambda_j!AE46-Inequality_Components_Lambda_j!AK46)</f>
+        <v>33.06546161805479</v>
       </c>
       <c r="H46" s="11">
         <f t="shared" si="2"/>
-        <v>1036.8623799986808</v>
+        <v>269.0483953469369</v>
       </c>
       <c r="I46" s="9">
         <f>(H46-H78)/Background_Calculations!$B$10</f>
-        <v>-4.6725180388029169E-8</v>
+        <v>-1.2124400545530001E-8</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -5151,36 +5151,36 @@
         <v>11</v>
       </c>
       <c r="B47" s="11">
-        <f>Inequality_Components_Lambda_j!B47+Inequality_Components_Lambda_j!H47-Inequality_Components_Lambda_j!N47+Inequality_Components_Lambda_j!T47+Inequality_Components_Lambda_j!Z47-Inequality_Components_Lambda_j!AF47</f>
-        <v>466.63151376155963</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B47+Inequality_Components_Lambda_j!H47-Inequality_Components_Lambda_j!N47+Inequality_Components_Lambda_j!T47+Inequality_Components_Lambda_j!Z47-Inequality_Components_Lambda_j!AF47)</f>
+        <v>121.08305057419432</v>
       </c>
       <c r="C47" s="11">
-        <f>Inequality_Components_Lambda_j!C47+Inequality_Components_Lambda_j!I47-Inequality_Components_Lambda_j!O47+Inequality_Components_Lambda_j!U47+Inequality_Components_Lambda_j!AA47-Inequality_Components_Lambda_j!AG47</f>
-        <v>95.937544281913844</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C47+Inequality_Components_Lambda_j!I47-Inequality_Components_Lambda_j!O47+Inequality_Components_Lambda_j!U47+Inequality_Components_Lambda_j!AA47-Inequality_Components_Lambda_j!AG47)</f>
+        <v>24.894183490973475</v>
       </c>
       <c r="D47" s="11">
-        <f>Inequality_Components_Lambda_j!D47+Inequality_Components_Lambda_j!J47-Inequality_Components_Lambda_j!P47+Inequality_Components_Lambda_j!V47+Inequality_Components_Lambda_j!AB47-Inequality_Components_Lambda_j!AH47</f>
-        <v>117.65698936663502</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D47+Inequality_Components_Lambda_j!J47-Inequality_Components_Lambda_j!P47+Inequality_Components_Lambda_j!V47+Inequality_Components_Lambda_j!AB47-Inequality_Components_Lambda_j!AH47)</f>
+        <v>30.530015169886916</v>
       </c>
       <c r="E47" s="11">
-        <f>Inequality_Components_Lambda_j!E47+Inequality_Components_Lambda_j!K47-Inequality_Components_Lambda_j!Q47+Inequality_Components_Lambda_j!W47+Inequality_Components_Lambda_j!AC47-Inequality_Components_Lambda_j!AI47</f>
-        <v>127.25122167899453</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E47+Inequality_Components_Lambda_j!K47-Inequality_Components_Lambda_j!Q47+Inequality_Components_Lambda_j!W47+Inequality_Components_Lambda_j!AC47-Inequality_Components_Lambda_j!AI47)</f>
+        <v>33.019557521909896</v>
       </c>
       <c r="F47" s="11">
-        <f>Inequality_Components_Lambda_j!F47+Inequality_Components_Lambda_j!L47-Inequality_Components_Lambda_j!R47+Inequality_Components_Lambda_j!X47+Inequality_Components_Lambda_j!AD47-Inequality_Components_Lambda_j!AJ47</f>
-        <v>101.81323108708928</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F47+Inequality_Components_Lambda_j!L47-Inequality_Components_Lambda_j!R47+Inequality_Components_Lambda_j!X47+Inequality_Components_Lambda_j!AD47-Inequality_Components_Lambda_j!AJ47)</f>
+        <v>26.41882565852481</v>
       </c>
       <c r="G47" s="11">
-        <f>Inequality_Components_Lambda_j!G47+Inequality_Components_Lambda_j!M47-Inequality_Components_Lambda_j!S47+Inequality_Components_Lambda_j!Y47+Inequality_Components_Lambda_j!AE47-Inequality_Components_Lambda_j!AK47</f>
-        <v>127.4090458337096</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G47+Inequality_Components_Lambda_j!M47-Inequality_Components_Lambda_j!S47+Inequality_Components_Lambda_j!Y47+Inequality_Components_Lambda_j!AE47-Inequality_Components_Lambda_j!AK47)</f>
+        <v>33.060510242726259</v>
       </c>
       <c r="H47" s="11">
         <f t="shared" si="2"/>
-        <v>1036.699546009902</v>
+        <v>269.00614265821571</v>
       </c>
       <c r="I47" s="9">
         <f>(H47-H79)/Background_Calculations!$B$10</f>
-        <v>-5.5130964144384013E-8</v>
+        <v>-1.4305560432224528E-8</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -5188,36 +5188,36 @@
         <v>12</v>
       </c>
       <c r="B48" s="11">
-        <f>Inequality_Components_Lambda_j!B48+Inequality_Components_Lambda_j!H48-Inequality_Components_Lambda_j!N48+Inequality_Components_Lambda_j!T48+Inequality_Components_Lambda_j!Z48-Inequality_Components_Lambda_j!AF48</f>
-        <v>466.55712862921547</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B48+Inequality_Components_Lambda_j!H48-Inequality_Components_Lambda_j!N48+Inequality_Components_Lambda_j!T48+Inequality_Components_Lambda_j!Z48-Inequality_Components_Lambda_j!AF48)</f>
+        <v>121.06374888008241</v>
       </c>
       <c r="C48" s="11">
-        <f>Inequality_Components_Lambda_j!C48+Inequality_Components_Lambda_j!I48-Inequality_Components_Lambda_j!O48+Inequality_Components_Lambda_j!U48+Inequality_Components_Lambda_j!AA48-Inequality_Components_Lambda_j!AG48</f>
-        <v>95.925479459045832</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C48+Inequality_Components_Lambda_j!I48-Inequality_Components_Lambda_j!O48+Inequality_Components_Lambda_j!U48+Inequality_Components_Lambda_j!AA48-Inequality_Components_Lambda_j!AG48)</f>
+        <v>24.891052871813788</v>
       </c>
       <c r="D48" s="11">
-        <f>Inequality_Components_Lambda_j!D48+Inequality_Components_Lambda_j!J48-Inequality_Components_Lambda_j!P48+Inequality_Components_Lambda_j!V48+Inequality_Components_Lambda_j!AB48-Inequality_Components_Lambda_j!AH48</f>
-        <v>117.64131086474057</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D48+Inequality_Components_Lambda_j!J48-Inequality_Components_Lambda_j!P48+Inequality_Components_Lambda_j!V48+Inequality_Components_Lambda_j!AB48-Inequality_Components_Lambda_j!AH48)</f>
+        <v>30.525946861635489</v>
       </c>
       <c r="E48" s="11">
-        <f>Inequality_Components_Lambda_j!E48+Inequality_Components_Lambda_j!K48-Inequality_Components_Lambda_j!Q48+Inequality_Components_Lambda_j!W48+Inequality_Components_Lambda_j!AC48-Inequality_Components_Lambda_j!AI48</f>
-        <v>127.23521921279983</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E48+Inequality_Components_Lambda_j!K48-Inequality_Components_Lambda_j!Q48+Inequality_Components_Lambda_j!W48+Inequality_Components_Lambda_j!AC48-Inequality_Components_Lambda_j!AI48)</f>
+        <v>33.015405150356706</v>
       </c>
       <c r="F48" s="11">
-        <f>Inequality_Components_Lambda_j!F48+Inequality_Components_Lambda_j!L48-Inequality_Components_Lambda_j!R48+Inequality_Components_Lambda_j!X48+Inequality_Components_Lambda_j!AD48-Inequality_Components_Lambda_j!AJ48</f>
-        <v>101.80041167578501</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F48+Inequality_Components_Lambda_j!L48-Inequality_Components_Lambda_j!R48+Inequality_Components_Lambda_j!X48+Inequality_Components_Lambda_j!AD48-Inequality_Components_Lambda_j!AJ48)</f>
+        <v>26.415499236323331</v>
       </c>
       <c r="G48" s="11">
-        <f>Inequality_Components_Lambda_j!G48+Inequality_Components_Lambda_j!M48-Inequality_Components_Lambda_j!S48+Inequality_Components_Lambda_j!Y48+Inequality_Components_Lambda_j!AE48-Inequality_Components_Lambda_j!AK48</f>
-        <v>127.39152943985775</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G48+Inequality_Components_Lambda_j!M48-Inequality_Components_Lambda_j!S48+Inequality_Components_Lambda_j!Y48+Inequality_Components_Lambda_j!AE48-Inequality_Components_Lambda_j!AK48)</f>
+        <v>33.055965032340566</v>
       </c>
       <c r="H48" s="11">
         <f t="shared" si="2"/>
-        <v>1036.5510792814443</v>
+        <v>268.96761803255231</v>
       </c>
       <c r="I48" s="9">
         <f>(H48-H80)/Background_Calculations!$B$10</f>
-        <v>-6.2795084048263277E-8</v>
+        <v>-1.6294270989827095E-8</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -5225,36 +5225,36 @@
         <v>13</v>
       </c>
       <c r="B49" s="11">
-        <f>Inequality_Components_Lambda_j!B49+Inequality_Components_Lambda_j!H49-Inequality_Components_Lambda_j!N49+Inequality_Components_Lambda_j!T49+Inequality_Components_Lambda_j!Z49-Inequality_Components_Lambda_j!AF49</f>
-        <v>466.49008616104953</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B49+Inequality_Components_Lambda_j!H49-Inequality_Components_Lambda_j!N49+Inequality_Components_Lambda_j!T49+Inequality_Components_Lambda_j!Z49-Inequality_Components_Lambda_j!AF49)</f>
+        <v>121.0463524841594</v>
       </c>
       <c r="C49" s="11">
-        <f>Inequality_Components_Lambda_j!C49+Inequality_Components_Lambda_j!I49-Inequality_Components_Lambda_j!O49+Inequality_Components_Lambda_j!U49+Inequality_Components_Lambda_j!AA49-Inequality_Components_Lambda_j!AG49</f>
-        <v>95.914162943315645</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C49+Inequality_Components_Lambda_j!I49-Inequality_Components_Lambda_j!O49+Inequality_Components_Lambda_j!U49+Inequality_Components_Lambda_j!AA49-Inequality_Components_Lambda_j!AG49)</f>
+        <v>24.888116425804309</v>
       </c>
       <c r="D49" s="11">
-        <f>Inequality_Components_Lambda_j!D49+Inequality_Components_Lambda_j!J49-Inequality_Components_Lambda_j!P49+Inequality_Components_Lambda_j!V49+Inequality_Components_Lambda_j!AB49-Inequality_Components_Lambda_j!AH49</f>
-        <v>117.6267581296644</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D49+Inequality_Components_Lambda_j!J49-Inequality_Components_Lambda_j!P49+Inequality_Components_Lambda_j!V49+Inequality_Components_Lambda_j!AB49-Inequality_Components_Lambda_j!AH49)</f>
+        <v>30.522170670989858</v>
       </c>
       <c r="E49" s="11">
-        <f>Inequality_Components_Lambda_j!E49+Inequality_Components_Lambda_j!K49-Inequality_Components_Lambda_j!Q49+Inequality_Components_Lambda_j!W49+Inequality_Components_Lambda_j!AC49-Inequality_Components_Lambda_j!AI49</f>
-        <v>127.22020917674175</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E49+Inequality_Components_Lambda_j!K49-Inequality_Components_Lambda_j!Q49+Inequality_Components_Lambda_j!W49+Inequality_Components_Lambda_j!AC49-Inequality_Components_Lambda_j!AI49)</f>
+        <v>33.011510297777008</v>
       </c>
       <c r="F49" s="11">
-        <f>Inequality_Components_Lambda_j!F49+Inequality_Components_Lambda_j!L49-Inequality_Components_Lambda_j!R49+Inequality_Components_Lambda_j!X49+Inequality_Components_Lambda_j!AD49-Inequality_Components_Lambda_j!AJ49</f>
-        <v>101.78839005278446</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F49+Inequality_Components_Lambda_j!L49-Inequality_Components_Lambda_j!R49+Inequality_Components_Lambda_j!X49+Inequality_Components_Lambda_j!AD49-Inequality_Components_Lambda_j!AJ49)</f>
+        <v>26.412379826804617</v>
       </c>
       <c r="G49" s="11">
-        <f>Inequality_Components_Lambda_j!G49+Inequality_Components_Lambda_j!M49-Inequality_Components_Lambda_j!S49+Inequality_Components_Lambda_j!Y49+Inequality_Components_Lambda_j!AE49-Inequality_Components_Lambda_j!AK49</f>
-        <v>127.37535885485774</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G49+Inequality_Components_Lambda_j!M49-Inequality_Components_Lambda_j!S49+Inequality_Components_Lambda_j!Y49+Inequality_Components_Lambda_j!AE49-Inequality_Components_Lambda_j!AK49)</f>
+        <v>33.051769036777408</v>
       </c>
       <c r="H49" s="11">
         <f t="shared" si="2"/>
-        <v>1036.4149653184136</v>
+        <v>268.93229874231258</v>
       </c>
       <c r="I49" s="9">
         <f>(H49-H81)/Background_Calculations!$B$10</f>
-        <v>-6.9821531954117547E-8</v>
+        <v>-1.8117516360216416E-8</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -5262,36 +5262,36 @@
         <v>14</v>
       </c>
       <c r="B50" s="11">
-        <f>Inequality_Components_Lambda_j!B50+Inequality_Components_Lambda_j!H50-Inequality_Components_Lambda_j!N50+Inequality_Components_Lambda_j!T50+Inequality_Components_Lambda_j!Z50-Inequality_Components_Lambda_j!AF50</f>
-        <v>466.42903677254981</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B50+Inequality_Components_Lambda_j!H50-Inequality_Components_Lambda_j!N50+Inequality_Components_Lambda_j!T50+Inequality_Components_Lambda_j!Z50-Inequality_Components_Lambda_j!AF50)</f>
+        <v>121.03051119188223</v>
       </c>
       <c r="C50" s="11">
-        <f>Inequality_Components_Lambda_j!C50+Inequality_Components_Lambda_j!I50-Inequality_Components_Lambda_j!O50+Inequality_Components_Lambda_j!U50+Inequality_Components_Lambda_j!AA50-Inequality_Components_Lambda_j!AG50</f>
-        <v>95.903457195582334</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C50+Inequality_Components_Lambda_j!I50-Inequality_Components_Lambda_j!O50+Inequality_Components_Lambda_j!U50+Inequality_Components_Lambda_j!AA50-Inequality_Components_Lambda_j!AG50)</f>
+        <v>24.885338463845038</v>
       </c>
       <c r="D50" s="11">
-        <f>Inequality_Components_Lambda_j!D50+Inequality_Components_Lambda_j!J50-Inequality_Components_Lambda_j!P50+Inequality_Components_Lambda_j!V50+Inequality_Components_Lambda_j!AB50-Inequality_Components_Lambda_j!AH50</f>
-        <v>117.61312424503042</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D50+Inequality_Components_Lambda_j!J50-Inequality_Components_Lambda_j!P50+Inequality_Components_Lambda_j!V50+Inequality_Components_Lambda_j!AB50-Inequality_Components_Lambda_j!AH50)</f>
+        <v>30.518632906621246</v>
       </c>
       <c r="E50" s="11">
-        <f>Inequality_Components_Lambda_j!E50+Inequality_Components_Lambda_j!K50-Inequality_Components_Lambda_j!Q50+Inequality_Components_Lambda_j!W50+Inequality_Components_Lambda_j!AC50-Inequality_Components_Lambda_j!AI50</f>
-        <v>127.20600916177783</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E50+Inequality_Components_Lambda_j!K50-Inequality_Components_Lambda_j!Q50+Inequality_Components_Lambda_j!W50+Inequality_Components_Lambda_j!AC50-Inequality_Components_Lambda_j!AI50)</f>
+        <v>33.007825632084007</v>
       </c>
       <c r="F50" s="11">
-        <f>Inequality_Components_Lambda_j!F50+Inequality_Components_Lambda_j!L50-Inequality_Components_Lambda_j!R50+Inequality_Components_Lambda_j!X50+Inequality_Components_Lambda_j!AD50-Inequality_Components_Lambda_j!AJ50</f>
-        <v>101.77701958428929</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F50+Inequality_Components_Lambda_j!L50-Inequality_Components_Lambda_j!R50+Inequality_Components_Lambda_j!X50+Inequality_Components_Lambda_j!AD50-Inequality_Components_Lambda_j!AJ50)</f>
+        <v>26.409429380957626</v>
       </c>
       <c r="G50" s="11">
-        <f>Inequality_Components_Lambda_j!G50+Inequality_Components_Lambda_j!M50-Inequality_Components_Lambda_j!S50+Inequality_Components_Lambda_j!Y50+Inequality_Components_Lambda_j!AE50-Inequality_Components_Lambda_j!AK50</f>
-        <v>127.36028671852279</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G50+Inequality_Components_Lambda_j!M50-Inequality_Components_Lambda_j!S50+Inequality_Components_Lambda_j!Y50+Inequality_Components_Lambda_j!AE50-Inequality_Components_Lambda_j!AK50)</f>
+        <v>33.047858070217536</v>
       </c>
       <c r="H50" s="11">
         <f t="shared" si="2"/>
-        <v>1036.2889336777525</v>
+        <v>268.89959564560769</v>
       </c>
       <c r="I50" s="9">
         <f>(H50-H82)/Background_Calculations!$B$10</f>
-        <v>-7.6327512221505532E-8</v>
+        <v>-1.9805709108708379E-8</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -5311,36 +5311,36 @@
         <v>0</v>
       </c>
       <c r="B52" s="11">
-        <f>Inequality_Components_Lambda_j!B52+Inequality_Components_Lambda_j!H52-Inequality_Components_Lambda_j!N52+Inequality_Components_Lambda_j!T52+Inequality_Components_Lambda_j!Z52-Inequality_Components_Lambda_j!AF52</f>
-        <v>468.96175025039145</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B52+Inequality_Components_Lambda_j!H52-Inequality_Components_Lambda_j!N52+Inequality_Components_Lambda_j!T52+Inequality_Components_Lambda_j!Z52-Inequality_Components_Lambda_j!AF52)</f>
+        <v>121.68770785580952</v>
       </c>
       <c r="C52" s="11">
-        <f>Inequality_Components_Lambda_j!C52+Inequality_Components_Lambda_j!I52-Inequality_Components_Lambda_j!O52+Inequality_Components_Lambda_j!U52+Inequality_Components_Lambda_j!AA52-Inequality_Components_Lambda_j!AG52</f>
-        <v>96.242976483566423</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C52+Inequality_Components_Lambda_j!I52-Inequality_Components_Lambda_j!O52+Inequality_Components_Lambda_j!U52+Inequality_Components_Lambda_j!AA52-Inequality_Components_Lambda_j!AG52)</f>
+        <v>24.97343802400226</v>
       </c>
       <c r="D52" s="11">
-        <f>Inequality_Components_Lambda_j!D52+Inequality_Components_Lambda_j!J52-Inequality_Components_Lambda_j!P52+Inequality_Components_Lambda_j!V52+Inequality_Components_Lambda_j!AB52-Inequality_Components_Lambda_j!AH52</f>
-        <v>118.08929470673786</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D52+Inequality_Components_Lambda_j!J52-Inequality_Components_Lambda_j!P52+Inequality_Components_Lambda_j!V52+Inequality_Components_Lambda_j!AB52-Inequality_Components_Lambda_j!AH52)</f>
+        <v>30.642191154181695</v>
       </c>
       <c r="E52" s="11">
-        <f>Inequality_Components_Lambda_j!E52+Inequality_Components_Lambda_j!K52-Inequality_Components_Lambda_j!Q52+Inequality_Components_Lambda_j!W52+Inequality_Components_Lambda_j!AC52-Inequality_Components_Lambda_j!AI52</f>
-        <v>127.71114151697245</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E52+Inequality_Components_Lambda_j!K52-Inequality_Components_Lambda_j!Q52+Inequality_Components_Lambda_j!W52+Inequality_Components_Lambda_j!AC52-Inequality_Components_Lambda_j!AI52)</f>
+        <v>33.138899005199448</v>
       </c>
       <c r="F52" s="11">
-        <f>Inequality_Components_Lambda_j!F52+Inequality_Components_Lambda_j!L52-Inequality_Components_Lambda_j!R52+Inequality_Components_Lambda_j!X52+Inequality_Components_Lambda_j!AD52-Inequality_Components_Lambda_j!AJ52</f>
-        <v>102.18245844238673</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F52+Inequality_Components_Lambda_j!L52-Inequality_Components_Lambda_j!R52+Inequality_Components_Lambda_j!X52+Inequality_Components_Lambda_j!AD52-Inequality_Components_Lambda_j!AJ52)</f>
+        <v>26.514633963828643</v>
       </c>
       <c r="G52" s="11">
-        <f>Inequality_Components_Lambda_j!G52+Inequality_Components_Lambda_j!M52-Inequality_Components_Lambda_j!S52+Inequality_Components_Lambda_j!Y52+Inequality_Components_Lambda_j!AE52-Inequality_Components_Lambda_j!AK52</f>
-        <v>128.1199345341067</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G52+Inequality_Components_Lambda_j!M52-Inequality_Components_Lambda_j!S52+Inequality_Components_Lambda_j!Y52+Inequality_Components_Lambda_j!AE52-Inequality_Components_Lambda_j!AK52)</f>
+        <v>33.244973936078075</v>
       </c>
       <c r="H52" s="11">
         <f>SUM(B52:G52)</f>
-        <v>1041.3075559341617</v>
+        <v>270.2018439390996</v>
       </c>
       <c r="I52" s="9">
         <f>(H52-H68)/Background_Calculations!$B$10</f>
-        <v>1.8274280693339899E-7</v>
+        <v>4.741869308315431E-8</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -5348,36 +5348,36 @@
         <v>1</v>
       </c>
       <c r="B53" s="11">
-        <f>Inequality_Components_Lambda_j!B53+Inequality_Components_Lambda_j!H53-Inequality_Components_Lambda_j!N53+Inequality_Components_Lambda_j!T53+Inequality_Components_Lambda_j!Z53-Inequality_Components_Lambda_j!AF53</f>
-        <v>468.27411064628188</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B53+Inequality_Components_Lambda_j!H53-Inequality_Components_Lambda_j!N53+Inequality_Components_Lambda_j!T53+Inequality_Components_Lambda_j!Z53-Inequality_Components_Lambda_j!AF53)</f>
+        <v>121.50927691296549</v>
       </c>
       <c r="C53" s="11">
-        <f>Inequality_Components_Lambda_j!C53+Inequality_Components_Lambda_j!I53-Inequality_Components_Lambda_j!O53+Inequality_Components_Lambda_j!U53+Inequality_Components_Lambda_j!AA53-Inequality_Components_Lambda_j!AG53</f>
-        <v>96.161827457726318</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C53+Inequality_Components_Lambda_j!I53-Inequality_Components_Lambda_j!O53+Inequality_Components_Lambda_j!U53+Inequality_Components_Lambda_j!AA53-Inequality_Components_Lambda_j!AG53)</f>
+        <v>24.95238121298528</v>
       </c>
       <c r="D53" s="11">
-        <f>Inequality_Components_Lambda_j!D53+Inequality_Components_Lambda_j!J53-Inequality_Components_Lambda_j!P53+Inequality_Components_Lambda_j!V53+Inequality_Components_Lambda_j!AB53-Inequality_Components_Lambda_j!AH53</f>
-        <v>117.96968467801604</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D53+Inequality_Components_Lambda_j!J53-Inequality_Components_Lambda_j!P53+Inequality_Components_Lambda_j!V53+Inequality_Components_Lambda_j!AB53-Inequality_Components_Lambda_j!AH53)</f>
+        <v>30.611154358059295</v>
       </c>
       <c r="E53" s="11">
-        <f>Inequality_Components_Lambda_j!E53+Inequality_Components_Lambda_j!K53-Inequality_Components_Lambda_j!Q53+Inequality_Components_Lambda_j!W53+Inequality_Components_Lambda_j!AC53-Inequality_Components_Lambda_j!AI53</f>
-        <v>127.584132678752</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E53+Inequality_Components_Lambda_j!K53-Inequality_Components_Lambda_j!Q53+Inequality_Components_Lambda_j!W53+Inequality_Components_Lambda_j!AC53-Inequality_Components_Lambda_j!AI53)</f>
+        <v>33.105942342119306</v>
       </c>
       <c r="F53" s="11">
-        <f>Inequality_Components_Lambda_j!F53+Inequality_Components_Lambda_j!L53-Inequality_Components_Lambda_j!R53+Inequality_Components_Lambda_j!X53+Inequality_Components_Lambda_j!AD53-Inequality_Components_Lambda_j!AJ53</f>
-        <v>102.08040394845385</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F53+Inequality_Components_Lambda_j!L53-Inequality_Components_Lambda_j!R53+Inequality_Components_Lambda_j!X53+Inequality_Components_Lambda_j!AD53-Inequality_Components_Lambda_j!AJ53)</f>
+        <v>26.488152534508561</v>
       </c>
       <c r="G53" s="11">
-        <f>Inequality_Components_Lambda_j!G53+Inequality_Components_Lambda_j!M53-Inequality_Components_Lambda_j!S53+Inequality_Components_Lambda_j!Y53+Inequality_Components_Lambda_j!AE53-Inequality_Components_Lambda_j!AK53</f>
-        <v>127.90478082649285</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G53+Inequality_Components_Lambda_j!M53-Inequality_Components_Lambda_j!S53+Inequality_Components_Lambda_j!Y53+Inequality_Components_Lambda_j!AE53-Inequality_Components_Lambda_j!AK53)</f>
+        <v>33.189145157926703</v>
       </c>
       <c r="H53" s="11">
         <f t="shared" ref="H53:H66" si="3">SUM(B53:G53)</f>
-        <v>1039.9749402357229</v>
+        <v>269.85605251856464</v>
       </c>
       <c r="I53" s="9">
         <f>(H53-H69)/Background_Calculations!$B$10</f>
-        <v>1.1395078460805483E-7</v>
+        <v>2.9568317202679125E-8</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -5385,36 +5385,36 @@
         <v>2</v>
       </c>
       <c r="B54" s="11">
-        <f>Inequality_Components_Lambda_j!B54+Inequality_Components_Lambda_j!H54-Inequality_Components_Lambda_j!N54+Inequality_Components_Lambda_j!T54+Inequality_Components_Lambda_j!Z54-Inequality_Components_Lambda_j!AF54</f>
-        <v>467.46995446970999</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B54+Inequality_Components_Lambda_j!H54-Inequality_Components_Lambda_j!N54+Inequality_Components_Lambda_j!T54+Inequality_Components_Lambda_j!Z54-Inequality_Components_Lambda_j!AF54)</f>
+        <v>121.30061187400895</v>
       </c>
       <c r="C54" s="11">
-        <f>Inequality_Components_Lambda_j!C54+Inequality_Components_Lambda_j!I54-Inequality_Components_Lambda_j!O54+Inequality_Components_Lambda_j!U54+Inequality_Components_Lambda_j!AA54-Inequality_Components_Lambda_j!AG54</f>
-        <v>96.067487377285303</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C54+Inequality_Components_Lambda_j!I54-Inequality_Components_Lambda_j!O54+Inequality_Components_Lambda_j!U54+Inequality_Components_Lambda_j!AA54-Inequality_Components_Lambda_j!AG54)</f>
+        <v>24.927901544565266</v>
       </c>
       <c r="D54" s="11">
-        <f>Inequality_Components_Lambda_j!D54+Inequality_Components_Lambda_j!J54-Inequality_Components_Lambda_j!P54+Inequality_Components_Lambda_j!V54+Inequality_Components_Lambda_j!AB54-Inequality_Components_Lambda_j!AH54</f>
-        <v>117.83022978771726</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D54+Inequality_Components_Lambda_j!J54-Inequality_Components_Lambda_j!P54+Inequality_Components_Lambda_j!V54+Inequality_Components_Lambda_j!AB54-Inequality_Components_Lambda_j!AH54)</f>
+        <v>30.574968153234103</v>
       </c>
       <c r="E54" s="11">
-        <f>Inequality_Components_Lambda_j!E54+Inequality_Components_Lambda_j!K54-Inequality_Components_Lambda_j!Q54+Inequality_Components_Lambda_j!W54+Inequality_Components_Lambda_j!AC54-Inequality_Components_Lambda_j!AI54</f>
-        <v>127.43575434027504</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E54+Inequality_Components_Lambda_j!K54-Inequality_Components_Lambda_j!Q54+Inequality_Components_Lambda_j!W54+Inequality_Components_Lambda_j!AC54-Inequality_Components_Lambda_j!AI54)</f>
+        <v>33.067440652173225</v>
       </c>
       <c r="F54" s="11">
-        <f>Inequality_Components_Lambda_j!F54+Inequality_Components_Lambda_j!L54-Inequality_Components_Lambda_j!R54+Inequality_Components_Lambda_j!X54+Inequality_Components_Lambda_j!AD54-Inequality_Components_Lambda_j!AJ54</f>
-        <v>101.96117107920503</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F54+Inequality_Components_Lambda_j!L54-Inequality_Components_Lambda_j!R54+Inequality_Components_Lambda_j!X54+Inequality_Components_Lambda_j!AD54-Inequality_Components_Lambda_j!AJ54)</f>
+        <v>26.457213604942954</v>
       </c>
       <c r="G54" s="11">
-        <f>Inequality_Components_Lambda_j!G54+Inequality_Components_Lambda_j!M54-Inequality_Components_Lambda_j!S54+Inequality_Components_Lambda_j!Y54+Inequality_Components_Lambda_j!AE54-Inequality_Components_Lambda_j!AK54</f>
-        <v>127.65123206424508</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G54+Inequality_Components_Lambda_j!M54-Inequality_Components_Lambda_j!S54+Inequality_Components_Lambda_j!Y54+Inequality_Components_Lambda_j!AE54-Inequality_Components_Lambda_j!AK54)</f>
+        <v>33.123353507133999</v>
       </c>
       <c r="H54" s="11">
         <f t="shared" si="3"/>
-        <v>1038.4158291184376</v>
+        <v>269.45148933605844</v>
       </c>
       <c r="I54" s="9">
         <f>(H54-H70)/Background_Calculations!$B$10</f>
-        <v>3.3466660855320498E-8</v>
+        <v>8.6840371243460865E-9</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -5422,36 +5422,36 @@
         <v>3</v>
       </c>
       <c r="B55" s="11">
-        <f>Inequality_Components_Lambda_j!B55+Inequality_Components_Lambda_j!H55-Inequality_Components_Lambda_j!N55+Inequality_Components_Lambda_j!T55+Inequality_Components_Lambda_j!Z55-Inequality_Components_Lambda_j!AF55</f>
-        <v>467.08980914635532</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B55+Inequality_Components_Lambda_j!H55-Inequality_Components_Lambda_j!N55+Inequality_Components_Lambda_j!T55+Inequality_Components_Lambda_j!Z55-Inequality_Components_Lambda_j!AF55)</f>
+        <v>121.20197053913155</v>
       </c>
       <c r="C55" s="11">
-        <f>Inequality_Components_Lambda_j!C55+Inequality_Components_Lambda_j!I55-Inequality_Components_Lambda_j!O55+Inequality_Components_Lambda_j!U55+Inequality_Components_Lambda_j!AA55-Inequality_Components_Lambda_j!AG55</f>
-        <v>96.020745907766539</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C55+Inequality_Components_Lambda_j!I55-Inequality_Components_Lambda_j!O55+Inequality_Components_Lambda_j!U55+Inequality_Components_Lambda_j!AA55-Inequality_Components_Lambda_j!AG55)</f>
+        <v>24.915772917263542</v>
       </c>
       <c r="D55" s="11">
-        <f>Inequality_Components_Lambda_j!D55+Inequality_Components_Lambda_j!J55-Inequality_Components_Lambda_j!P55+Inequality_Components_Lambda_j!V55+Inequality_Components_Lambda_j!AB55-Inequality_Components_Lambda_j!AH55</f>
-        <v>117.76238311022529</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D55+Inequality_Components_Lambda_j!J55-Inequality_Components_Lambda_j!P55+Inequality_Components_Lambda_j!V55+Inequality_Components_Lambda_j!AB55-Inequality_Components_Lambda_j!AH55)</f>
+        <v>30.55736307848073</v>
       </c>
       <c r="E55" s="11">
-        <f>Inequality_Components_Lambda_j!E55+Inequality_Components_Lambda_j!K55-Inequality_Components_Lambda_j!Q55+Inequality_Components_Lambda_j!W55+Inequality_Components_Lambda_j!AC55-Inequality_Components_Lambda_j!AI55</f>
-        <v>127.3634141740789</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E55+Inequality_Components_Lambda_j!K55-Inequality_Components_Lambda_j!Q55+Inequality_Components_Lambda_j!W55+Inequality_Components_Lambda_j!AC55-Inequality_Components_Lambda_j!AI55)</f>
+        <v>33.04866959247461</v>
       </c>
       <c r="F55" s="11">
-        <f>Inequality_Components_Lambda_j!F55+Inequality_Components_Lambda_j!L55-Inequality_Components_Lambda_j!R55+Inequality_Components_Lambda_j!X55+Inequality_Components_Lambda_j!AD55-Inequality_Components_Lambda_j!AJ55</f>
-        <v>101.90306328289191</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F55+Inequality_Components_Lambda_j!L55-Inequality_Components_Lambda_j!R55+Inequality_Components_Lambda_j!X55+Inequality_Components_Lambda_j!AD55-Inequality_Components_Lambda_j!AJ55)</f>
+        <v>26.44213560649613</v>
       </c>
       <c r="G55" s="11">
-        <f>Inequality_Components_Lambda_j!G55+Inequality_Components_Lambda_j!M55-Inequality_Components_Lambda_j!S55+Inequality_Components_Lambda_j!Y55+Inequality_Components_Lambda_j!AE55-Inequality_Components_Lambda_j!AK55</f>
-        <v>127.53217108931698</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G55+Inequality_Components_Lambda_j!M55-Inequality_Components_Lambda_j!S55+Inequality_Components_Lambda_j!Y55+Inequality_Components_Lambda_j!AE55-Inequality_Components_Lambda_j!AK55)</f>
+        <v>33.092459181261269</v>
       </c>
       <c r="H55" s="11">
         <f t="shared" si="3"/>
-        <v>1037.671586710635</v>
+        <v>269.25837091510783</v>
       </c>
       <c r="I55" s="9">
         <f>(H55-H71)/Background_Calculations!$B$10</f>
-        <v>-4.9524725775274106E-9</v>
+        <v>-1.2850835614104137E-9</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -5459,36 +5459,36 @@
         <v>4</v>
       </c>
       <c r="B56" s="11">
-        <f>Inequality_Components_Lambda_j!B56+Inequality_Components_Lambda_j!H56-Inequality_Components_Lambda_j!N56+Inequality_Components_Lambda_j!T56+Inequality_Components_Lambda_j!Z56-Inequality_Components_Lambda_j!AF56</f>
-        <v>467.03866757726939</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B56+Inequality_Components_Lambda_j!H56-Inequality_Components_Lambda_j!N56+Inequality_Components_Lambda_j!T56+Inequality_Components_Lambda_j!Z56-Inequality_Components_Lambda_j!AF56)</f>
+        <v>121.18870015979914</v>
       </c>
       <c r="C56" s="11">
-        <f>Inequality_Components_Lambda_j!C56+Inequality_Components_Lambda_j!I56-Inequality_Components_Lambda_j!O56+Inequality_Components_Lambda_j!U56+Inequality_Components_Lambda_j!AA56-Inequality_Components_Lambda_j!AG56</f>
-        <v>96.010779242244539</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C56+Inequality_Components_Lambda_j!I56-Inequality_Components_Lambda_j!O56+Inequality_Components_Lambda_j!U56+Inequality_Components_Lambda_j!AA56-Inequality_Components_Lambda_j!AG56)</f>
+        <v>24.913186734740787</v>
       </c>
       <c r="D56" s="11">
-        <f>Inequality_Components_Lambda_j!D56+Inequality_Components_Lambda_j!J56-Inequality_Components_Lambda_j!P56+Inequality_Components_Lambda_j!V56+Inequality_Components_Lambda_j!AB56-Inequality_Components_Lambda_j!AH56</f>
-        <v>117.74986111426296</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D56+Inequality_Components_Lambda_j!J56-Inequality_Components_Lambda_j!P56+Inequality_Components_Lambda_j!V56+Inequality_Components_Lambda_j!AB56-Inequality_Components_Lambda_j!AH56)</f>
+        <v>30.554113830571659</v>
       </c>
       <c r="E56" s="11">
-        <f>Inequality_Components_Lambda_j!E56+Inequality_Components_Lambda_j!K56-Inequality_Components_Lambda_j!Q56+Inequality_Components_Lambda_j!W56+Inequality_Components_Lambda_j!AC56-Inequality_Components_Lambda_j!AI56</f>
-        <v>127.34939777388659</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E56+Inequality_Components_Lambda_j!K56-Inequality_Components_Lambda_j!Q56+Inequality_Components_Lambda_j!W56+Inequality_Components_Lambda_j!AC56-Inequality_Components_Lambda_j!AI56)</f>
+        <v>33.0450325717349</v>
       </c>
       <c r="F56" s="11">
-        <f>Inequality_Components_Lambda_j!F56+Inequality_Components_Lambda_j!L56-Inequality_Components_Lambda_j!R56+Inequality_Components_Lambda_j!X56+Inequality_Components_Lambda_j!AD56-Inequality_Components_Lambda_j!AJ56</f>
-        <v>101.89184041744889</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F56+Inequality_Components_Lambda_j!L56-Inequality_Components_Lambda_j!R56+Inequality_Components_Lambda_j!X56+Inequality_Components_Lambda_j!AD56-Inequality_Components_Lambda_j!AJ56)</f>
+        <v>26.439223461165287</v>
       </c>
       <c r="G56" s="11">
-        <f>Inequality_Components_Lambda_j!G56+Inequality_Components_Lambda_j!M56-Inequality_Components_Lambda_j!S56+Inequality_Components_Lambda_j!Y56+Inequality_Components_Lambda_j!AE56-Inequality_Components_Lambda_j!AK56</f>
-        <v>127.51541225953837</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G56+Inequality_Components_Lambda_j!M56-Inequality_Components_Lambda_j!S56+Inequality_Components_Lambda_j!Y56+Inequality_Components_Lambda_j!AE56-Inequality_Components_Lambda_j!AK56)</f>
+        <v>33.08811054604525</v>
       </c>
       <c r="H56" s="11">
         <f t="shared" si="3"/>
-        <v>1037.5559583846507</v>
+        <v>269.22836730405703</v>
       </c>
       <c r="I56" s="9">
         <f>(H56-H72)/Background_Calculations!$B$10</f>
-        <v>-1.0921415005469969E-8</v>
+        <v>-2.8339239988041877E-9</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -5496,36 +5496,36 @@
         <v>5</v>
       </c>
       <c r="B57" s="11">
-        <f>Inequality_Components_Lambda_j!B57+Inequality_Components_Lambda_j!H57-Inequality_Components_Lambda_j!N57+Inequality_Components_Lambda_j!T57+Inequality_Components_Lambda_j!Z57-Inequality_Components_Lambda_j!AF57</f>
-        <v>466.99457715790908</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B57+Inequality_Components_Lambda_j!H57-Inequality_Components_Lambda_j!N57+Inequality_Components_Lambda_j!T57+Inequality_Components_Lambda_j!Z57-Inequality_Components_Lambda_j!AF57)</f>
+        <v>121.177259435545</v>
       </c>
       <c r="C57" s="11">
-        <f>Inequality_Components_Lambda_j!C57+Inequality_Components_Lambda_j!I57-Inequality_Components_Lambda_j!O57+Inequality_Components_Lambda_j!U57+Inequality_Components_Lambda_j!AA57-Inequality_Components_Lambda_j!AG57</f>
-        <v>96.001551356253728</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C57+Inequality_Components_Lambda_j!I57-Inequality_Components_Lambda_j!O57+Inequality_Components_Lambda_j!U57+Inequality_Components_Lambda_j!AA57-Inequality_Components_Lambda_j!AG57)</f>
+        <v>24.910792253114138</v>
       </c>
       <c r="D57" s="11">
-        <f>Inequality_Components_Lambda_j!D57+Inequality_Components_Lambda_j!J57-Inequality_Components_Lambda_j!P57+Inequality_Components_Lambda_j!V57+Inequality_Components_Lambda_j!AB57-Inequality_Components_Lambda_j!AH57</f>
-        <v>117.73845055161476</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D57+Inequality_Components_Lambda_j!J57-Inequality_Components_Lambda_j!P57+Inequality_Components_Lambda_j!V57+Inequality_Components_Lambda_j!AB57-Inequality_Components_Lambda_j!AH57)</f>
+        <v>30.551152980964492</v>
       </c>
       <c r="E57" s="11">
-        <f>Inequality_Components_Lambda_j!E57+Inequality_Components_Lambda_j!K57-Inequality_Components_Lambda_j!Q57+Inequality_Components_Lambda_j!W57+Inequality_Components_Lambda_j!AC57-Inequality_Components_Lambda_j!AI57</f>
-        <v>127.33642056679041</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E57+Inequality_Components_Lambda_j!K57-Inequality_Components_Lambda_j!Q57+Inequality_Components_Lambda_j!W57+Inequality_Components_Lambda_j!AC57-Inequality_Components_Lambda_j!AI57)</f>
+        <v>33.041665204172276</v>
       </c>
       <c r="F57" s="11">
-        <f>Inequality_Components_Lambda_j!F57+Inequality_Components_Lambda_j!L57-Inequality_Components_Lambda_j!R57+Inequality_Components_Lambda_j!X57+Inequality_Components_Lambda_j!AD57-Inequality_Components_Lambda_j!AJ57</f>
-        <v>101.88145293181428</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F57+Inequality_Components_Lambda_j!L57-Inequality_Components_Lambda_j!R57+Inequality_Components_Lambda_j!X57+Inequality_Components_Lambda_j!AD57-Inequality_Components_Lambda_j!AJ57)</f>
+        <v>26.43652808288212</v>
       </c>
       <c r="G57" s="11">
-        <f>Inequality_Components_Lambda_j!G57+Inequality_Components_Lambda_j!M57-Inequality_Components_Lambda_j!S57+Inequality_Components_Lambda_j!Y57+Inequality_Components_Lambda_j!AE57-Inequality_Components_Lambda_j!AK57</f>
-        <v>127.50020699149128</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G57+Inequality_Components_Lambda_j!M57-Inequality_Components_Lambda_j!S57+Inequality_Components_Lambda_j!Y57+Inequality_Components_Lambda_j!AE57-Inequality_Components_Lambda_j!AK57)</f>
+        <v>33.084165034039223</v>
       </c>
       <c r="H57" s="11">
         <f t="shared" si="3"/>
-        <v>1037.4526595558734</v>
+        <v>269.20156299071726</v>
       </c>
       <c r="I57" s="9">
         <f>(H57-H73)/Background_Calculations!$B$10</f>
-        <v>-1.6253886582799512E-8</v>
+        <v>-4.217610926584666E-9</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -5533,36 +5533,36 @@
         <v>6</v>
       </c>
       <c r="B58" s="11">
-        <f>Inequality_Components_Lambda_j!B58+Inequality_Components_Lambda_j!H58-Inequality_Components_Lambda_j!N58+Inequality_Components_Lambda_j!T58+Inequality_Components_Lambda_j!Z58-Inequality_Components_Lambda_j!AF58</f>
-        <v>466.93777751308477</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B58+Inequality_Components_Lambda_j!H58-Inequality_Components_Lambda_j!N58+Inequality_Components_Lambda_j!T58+Inequality_Components_Lambda_j!Z58-Inequality_Components_Lambda_j!AF58)</f>
+        <v>121.16252088046666</v>
       </c>
       <c r="C58" s="11">
-        <f>Inequality_Components_Lambda_j!C58+Inequality_Components_Lambda_j!I58-Inequality_Components_Lambda_j!O58+Inequality_Components_Lambda_j!U58+Inequality_Components_Lambda_j!AA58-Inequality_Components_Lambda_j!AG58</f>
-        <v>95.99117664583602</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C58+Inequality_Components_Lambda_j!I58-Inequality_Components_Lambda_j!O58+Inequality_Components_Lambda_j!U58+Inequality_Components_Lambda_j!AA58-Inequality_Components_Lambda_j!AG58)</f>
+        <v>24.908100189785468</v>
       </c>
       <c r="D58" s="11">
-        <f>Inequality_Components_Lambda_j!D58+Inequality_Components_Lambda_j!J58-Inequality_Components_Lambda_j!P58+Inequality_Components_Lambda_j!V58+Inequality_Components_Lambda_j!AB58-Inequality_Components_Lambda_j!AH58</f>
-        <v>117.72531468551716</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D58+Inequality_Components_Lambda_j!J58-Inequality_Components_Lambda_j!P58+Inequality_Components_Lambda_j!V58+Inequality_Components_Lambda_j!AB58-Inequality_Components_Lambda_j!AH58)</f>
+        <v>30.547744444052338</v>
       </c>
       <c r="E58" s="11">
-        <f>Inequality_Components_Lambda_j!E58+Inequality_Components_Lambda_j!K58-Inequality_Components_Lambda_j!Q58+Inequality_Components_Lambda_j!W58+Inequality_Components_Lambda_j!AC58-Inequality_Components_Lambda_j!AI58</f>
-        <v>127.32235918511925</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E58+Inequality_Components_Lambda_j!K58-Inequality_Components_Lambda_j!Q58+Inequality_Components_Lambda_j!W58+Inequality_Components_Lambda_j!AC58-Inequality_Components_Lambda_j!AI58)</f>
+        <v>33.038016511493318</v>
       </c>
       <c r="F58" s="11">
-        <f>Inequality_Components_Lambda_j!F58+Inequality_Components_Lambda_j!L58-Inequality_Components_Lambda_j!R58+Inequality_Components_Lambda_j!X58+Inequality_Components_Lambda_j!AD58-Inequality_Components_Lambda_j!AJ58</f>
-        <v>101.87019390695167</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F58+Inequality_Components_Lambda_j!L58-Inequality_Components_Lambda_j!R58+Inequality_Components_Lambda_j!X58+Inequality_Components_Lambda_j!AD58-Inequality_Components_Lambda_j!AJ58)</f>
+        <v>26.43360655478843</v>
       </c>
       <c r="G58" s="11">
-        <f>Inequality_Components_Lambda_j!G58+Inequality_Components_Lambda_j!M58-Inequality_Components_Lambda_j!S58+Inequality_Components_Lambda_j!Y58+Inequality_Components_Lambda_j!AE58-Inequality_Components_Lambda_j!AK58</f>
-        <v>127.48459288242442</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G58+Inequality_Components_Lambda_j!M58-Inequality_Components_Lambda_j!S58+Inequality_Components_Lambda_j!Y58+Inequality_Components_Lambda_j!AE58-Inequality_Components_Lambda_j!AK58)</f>
+        <v>33.080113434646428</v>
       </c>
       <c r="H58" s="11">
         <f t="shared" si="3"/>
-        <v>1037.3314148189334</v>
+        <v>269.17010201523266</v>
       </c>
       <c r="I58" s="9">
         <f>(H58-H74)/Background_Calculations!$B$10</f>
-        <v>-2.2512758259145088E-8</v>
+        <v>-5.8416831406893719E-9</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -5570,36 +5570,36 @@
         <v>7</v>
       </c>
       <c r="B59" s="11">
-        <f>Inequality_Components_Lambda_j!B59+Inequality_Components_Lambda_j!H59-Inequality_Components_Lambda_j!N59+Inequality_Components_Lambda_j!T59+Inequality_Components_Lambda_j!Z59-Inequality_Components_Lambda_j!AF59</f>
-        <v>466.8706049972235</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B59+Inequality_Components_Lambda_j!H59-Inequality_Components_Lambda_j!N59+Inequality_Components_Lambda_j!T59+Inequality_Components_Lambda_j!Z59-Inequality_Components_Lambda_j!AF59)</f>
+        <v>121.14509073934811</v>
       </c>
       <c r="C59" s="11">
-        <f>Inequality_Components_Lambda_j!C59+Inequality_Components_Lambda_j!I59-Inequality_Components_Lambda_j!O59+Inequality_Components_Lambda_j!U59+Inequality_Components_Lambda_j!AA59-Inequality_Components_Lambda_j!AG59</f>
-        <v>95.979846876657732</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C59+Inequality_Components_Lambda_j!I59-Inequality_Components_Lambda_j!O59+Inequality_Components_Lambda_j!U59+Inequality_Components_Lambda_j!AA59-Inequality_Components_Lambda_j!AG59)</f>
+        <v>24.905160304728518</v>
       </c>
       <c r="D59" s="11">
-        <f>Inequality_Components_Lambda_j!D59+Inequality_Components_Lambda_j!J59-Inequality_Components_Lambda_j!P59+Inequality_Components_Lambda_j!V59+Inequality_Components_Lambda_j!AB59-Inequality_Components_Lambda_j!AH59</f>
-        <v>117.71074201171346</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D59+Inequality_Components_Lambda_j!J59-Inequality_Components_Lambda_j!P59+Inequality_Components_Lambda_j!V59+Inequality_Components_Lambda_j!AB59-Inequality_Components_Lambda_j!AH59)</f>
+        <v>30.543963079641369</v>
       </c>
       <c r="E59" s="11">
-        <f>Inequality_Components_Lambda_j!E59+Inequality_Components_Lambda_j!K59-Inequality_Components_Lambda_j!Q59+Inequality_Components_Lambda_j!W59+Inequality_Components_Lambda_j!AC59-Inequality_Components_Lambda_j!AI59</f>
-        <v>127.30733157189178</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E59+Inequality_Components_Lambda_j!K59-Inequality_Components_Lambda_j!Q59+Inequality_Components_Lambda_j!W59+Inequality_Components_Lambda_j!AC59-Inequality_Components_Lambda_j!AI59)</f>
+        <v>33.034117097933006</v>
       </c>
       <c r="F59" s="11">
-        <f>Inequality_Components_Lambda_j!F59+Inequality_Components_Lambda_j!L59-Inequality_Components_Lambda_j!R59+Inequality_Components_Lambda_j!X59+Inequality_Components_Lambda_j!AD59-Inequality_Components_Lambda_j!AJ59</f>
-        <v>101.85815815413017</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F59+Inequality_Components_Lambda_j!L59-Inequality_Components_Lambda_j!R59+Inequality_Components_Lambda_j!X59+Inequality_Components_Lambda_j!AD59-Inequality_Components_Lambda_j!AJ59)</f>
+        <v>26.430483478818193</v>
       </c>
       <c r="G59" s="11">
-        <f>Inequality_Components_Lambda_j!G59+Inequality_Components_Lambda_j!M59-Inequality_Components_Lambda_j!S59+Inequality_Components_Lambda_j!Y59+Inequality_Components_Lambda_j!AE59-Inequality_Components_Lambda_j!AK59</f>
-        <v>127.4683984614794</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G59+Inequality_Components_Lambda_j!M59-Inequality_Components_Lambda_j!S59+Inequality_Components_Lambda_j!Y59+Inequality_Components_Lambda_j!AE59-Inequality_Components_Lambda_j!AK59)</f>
+        <v>33.07591125405537</v>
       </c>
       <c r="H59" s="11">
         <f t="shared" si="3"/>
-        <v>1037.1950820730958</v>
+        <v>269.13472595452458</v>
       </c>
       <c r="I59" s="9">
         <f>(H59-H75)/Background_Calculations!$B$10</f>
-        <v>-2.9550500127501289E-8</v>
+        <v>-7.6678591048954726E-9</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -5607,36 +5607,36 @@
         <v>8</v>
       </c>
       <c r="B60" s="11">
-        <f>Inequality_Components_Lambda_j!B60+Inequality_Components_Lambda_j!H60-Inequality_Components_Lambda_j!N60+Inequality_Components_Lambda_j!T60+Inequality_Components_Lambda_j!Z60-Inequality_Components_Lambda_j!AF60</f>
-        <v>466.79744922304729</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B60+Inequality_Components_Lambda_j!H60-Inequality_Components_Lambda_j!N60+Inequality_Components_Lambda_j!T60+Inequality_Components_Lambda_j!Z60-Inequality_Components_Lambda_j!AF60)</f>
+        <v>121.12610804305963</v>
       </c>
       <c r="C60" s="11">
-        <f>Inequality_Components_Lambda_j!C60+Inequality_Components_Lambda_j!I60-Inequality_Components_Lambda_j!O60+Inequality_Components_Lambda_j!U60+Inequality_Components_Lambda_j!AA60-Inequality_Components_Lambda_j!AG60</f>
-        <v>95.96790734039817</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C60+Inequality_Components_Lambda_j!I60-Inequality_Components_Lambda_j!O60+Inequality_Components_Lambda_j!U60+Inequality_Components_Lambda_j!AA60-Inequality_Components_Lambda_j!AG60)</f>
+        <v>24.902062195342175</v>
       </c>
       <c r="D60" s="11">
-        <f>Inequality_Components_Lambda_j!D60+Inequality_Components_Lambda_j!J60-Inequality_Components_Lambda_j!P60+Inequality_Components_Lambda_j!V60+Inequality_Components_Lambda_j!AB60-Inequality_Components_Lambda_j!AH60</f>
-        <v>117.69525199326311</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D60+Inequality_Components_Lambda_j!J60-Inequality_Components_Lambda_j!P60+Inequality_Components_Lambda_j!V60+Inequality_Components_Lambda_j!AB60-Inequality_Components_Lambda_j!AH60)</f>
+        <v>30.539943679682075</v>
       </c>
       <c r="E60" s="11">
-        <f>Inequality_Components_Lambda_j!E60+Inequality_Components_Lambda_j!K60-Inequality_Components_Lambda_j!Q60+Inequality_Components_Lambda_j!W60+Inequality_Components_Lambda_j!AC60-Inequality_Components_Lambda_j!AI60</f>
-        <v>127.29149526501814</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E60+Inequality_Components_Lambda_j!K60-Inequality_Components_Lambda_j!Q60+Inequality_Components_Lambda_j!W60+Inequality_Components_Lambda_j!AC60-Inequality_Components_Lambda_j!AI60)</f>
+        <v>33.030007841936488</v>
       </c>
       <c r="F60" s="11">
-        <f>Inequality_Components_Lambda_j!F60+Inequality_Components_Lambda_j!L60-Inequality_Components_Lambda_j!R60+Inequality_Components_Lambda_j!X60+Inequality_Components_Lambda_j!AD60-Inequality_Components_Lambda_j!AJ60</f>
-        <v>101.84547231390358</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F60+Inequality_Components_Lambda_j!L60-Inequality_Components_Lambda_j!R60+Inequality_Components_Lambda_j!X60+Inequality_Components_Lambda_j!AD60-Inequality_Components_Lambda_j!AJ60)</f>
+        <v>26.427191716070862</v>
       </c>
       <c r="G60" s="11">
-        <f>Inequality_Components_Lambda_j!G60+Inequality_Components_Lambda_j!M60-Inequality_Components_Lambda_j!S60+Inequality_Components_Lambda_j!Y60+Inequality_Components_Lambda_j!AE60-Inequality_Components_Lambda_j!AK60</f>
-        <v>127.45110739198726</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G60+Inequality_Components_Lambda_j!M60-Inequality_Components_Lambda_j!S60+Inequality_Components_Lambda_j!Y60+Inequality_Components_Lambda_j!AE60-Inequality_Components_Lambda_j!AK60)</f>
+        <v>33.071424511561446</v>
       </c>
       <c r="H60" s="11">
         <f t="shared" si="3"/>
-        <v>1037.0486835276176</v>
+        <v>269.09673798765266</v>
       </c>
       <c r="I60" s="9">
         <f>(H60-H76)/Background_Calculations!$B$10</f>
-        <v>-3.7107856701291907E-8</v>
+        <v>-9.6288663691873784E-9</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -5644,36 +5644,36 @@
         <v>9</v>
       </c>
       <c r="B61" s="11">
-        <f>Inequality_Components_Lambda_j!B61+Inequality_Components_Lambda_j!H61-Inequality_Components_Lambda_j!N61+Inequality_Components_Lambda_j!T61+Inequality_Components_Lambda_j!Z61-Inequality_Components_Lambda_j!AF61</f>
-        <v>466.724027222828</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B61+Inequality_Components_Lambda_j!H61-Inequality_Components_Lambda_j!N61+Inequality_Components_Lambda_j!T61+Inequality_Components_Lambda_j!Z61-Inequality_Components_Lambda_j!AF61)</f>
+        <v>121.10705626557862</v>
       </c>
       <c r="C61" s="11">
-        <f>Inequality_Components_Lambda_j!C61+Inequality_Components_Lambda_j!I61-Inequality_Components_Lambda_j!O61+Inequality_Components_Lambda_j!U61+Inequality_Components_Lambda_j!AA61-Inequality_Components_Lambda_j!AG61</f>
-        <v>95.955940672454062</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C61+Inequality_Components_Lambda_j!I61-Inequality_Components_Lambda_j!O61+Inequality_Components_Lambda_j!U61+Inequality_Components_Lambda_j!AA61-Inequality_Components_Lambda_j!AG61)</f>
+        <v>24.898957045738793</v>
       </c>
       <c r="D61" s="11">
-        <f>Inequality_Components_Lambda_j!D61+Inequality_Components_Lambda_j!J61-Inequality_Components_Lambda_j!P61+Inequality_Components_Lambda_j!V61+Inequality_Components_Lambda_j!AB61-Inequality_Components_Lambda_j!AH61</f>
-        <v>117.67972115741486</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D61+Inequality_Components_Lambda_j!J61-Inequality_Components_Lambda_j!P61+Inequality_Components_Lambda_j!V61+Inequality_Components_Lambda_j!AB61-Inequality_Components_Lambda_j!AH61)</f>
+        <v>30.535913688292691</v>
       </c>
       <c r="E61" s="11">
-        <f>Inequality_Components_Lambda_j!E61+Inequality_Components_Lambda_j!K61-Inequality_Components_Lambda_j!Q61+Inequality_Components_Lambda_j!W61+Inequality_Components_Lambda_j!AC61-Inequality_Components_Lambda_j!AI61</f>
-        <v>127.27562297519037</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E61+Inequality_Components_Lambda_j!K61-Inequality_Components_Lambda_j!Q61+Inequality_Components_Lambda_j!W61+Inequality_Components_Lambda_j!AC61-Inequality_Components_Lambda_j!AI61)</f>
+        <v>33.025889248966948</v>
       </c>
       <c r="F61" s="11">
-        <f>Inequality_Components_Lambda_j!F61+Inequality_Components_Lambda_j!L61-Inequality_Components_Lambda_j!R61+Inequality_Components_Lambda_j!X61+Inequality_Components_Lambda_j!AD61-Inequality_Components_Lambda_j!AJ61</f>
-        <v>101.83275754793314</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F61+Inequality_Components_Lambda_j!L61-Inequality_Components_Lambda_j!R61+Inequality_Components_Lambda_j!X61+Inequality_Components_Lambda_j!AD61-Inequality_Components_Lambda_j!AJ61)</f>
+        <v>26.423892447578197</v>
       </c>
       <c r="G61" s="11">
-        <f>Inequality_Components_Lambda_j!G61+Inequality_Components_Lambda_j!M61-Inequality_Components_Lambda_j!S61+Inequality_Components_Lambda_j!Y61+Inequality_Components_Lambda_j!AE61-Inequality_Components_Lambda_j!AK61</f>
-        <v>127.43376752694128</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G61+Inequality_Components_Lambda_j!M61-Inequality_Components_Lambda_j!S61+Inequality_Components_Lambda_j!Y61+Inequality_Components_Lambda_j!AE61-Inequality_Components_Lambda_j!AK61)</f>
+        <v>33.066925107439793</v>
       </c>
       <c r="H61" s="11">
         <f t="shared" si="3"/>
-        <v>1036.9018371027616</v>
+        <v>269.05863380359506</v>
       </c>
       <c r="I61" s="9">
         <f>(H61-H77)/Background_Calculations!$B$10</f>
-        <v>-4.4688333615172977E-8</v>
+        <v>-1.1595872973905105E-8</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -5681,36 +5681,36 @@
         <v>10</v>
       </c>
       <c r="B62" s="11">
-        <f>Inequality_Components_Lambda_j!B62+Inequality_Components_Lambda_j!H62-Inequality_Components_Lambda_j!N62+Inequality_Components_Lambda_j!T62+Inequality_Components_Lambda_j!Z62-Inequality_Components_Lambda_j!AF62</f>
-        <v>466.65351485808117</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B62+Inequality_Components_Lambda_j!H62-Inequality_Components_Lambda_j!N62+Inequality_Components_Lambda_j!T62+Inequality_Components_Lambda_j!Z62-Inequality_Components_Lambda_j!AF62)</f>
+        <v>121.08875948969668</v>
       </c>
       <c r="C62" s="11">
-        <f>Inequality_Components_Lambda_j!C62+Inequality_Components_Lambda_j!I62-Inequality_Components_Lambda_j!O62+Inequality_Components_Lambda_j!U62+Inequality_Components_Lambda_j!AA62-Inequality_Components_Lambda_j!AG62</f>
-        <v>95.944270531892897</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C62+Inequality_Components_Lambda_j!I62-Inequality_Components_Lambda_j!O62+Inequality_Components_Lambda_j!U62+Inequality_Components_Lambda_j!AA62-Inequality_Components_Lambda_j!AG62)</f>
+        <v>24.895928840017358</v>
       </c>
       <c r="D62" s="11">
-        <f>Inequality_Components_Lambda_j!D62+Inequality_Components_Lambda_j!J62-Inequality_Components_Lambda_j!P62+Inequality_Components_Lambda_j!V62+Inequality_Components_Lambda_j!AB62-Inequality_Components_Lambda_j!AH62</f>
-        <v>117.66463642273493</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D62+Inequality_Components_Lambda_j!J62-Inequality_Components_Lambda_j!P62+Inequality_Components_Lambda_j!V62+Inequality_Components_Lambda_j!AB62-Inequality_Components_Lambda_j!AH62)</f>
+        <v>30.531999452673617</v>
       </c>
       <c r="E62" s="11">
-        <f>Inequality_Components_Lambda_j!E62+Inequality_Components_Lambda_j!K62-Inequality_Components_Lambda_j!Q62+Inequality_Components_Lambda_j!W62+Inequality_Components_Lambda_j!AC62-Inequality_Components_Lambda_j!AI62</f>
-        <v>127.26014394996785</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E62+Inequality_Components_Lambda_j!K62-Inequality_Components_Lambda_j!Q62+Inequality_Components_Lambda_j!W62+Inequality_Components_Lambda_j!AC62-Inequality_Components_Lambda_j!AI62)</f>
+        <v>33.021872701565876</v>
       </c>
       <c r="F62" s="11">
-        <f>Inequality_Components_Lambda_j!F62+Inequality_Components_Lambda_j!L62-Inequality_Components_Lambda_j!R62+Inequality_Components_Lambda_j!X62+Inequality_Components_Lambda_j!AD62-Inequality_Components_Lambda_j!AJ62</f>
-        <v>101.82035891696384</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F62+Inequality_Components_Lambda_j!L62-Inequality_Components_Lambda_j!R62+Inequality_Components_Lambda_j!X62+Inequality_Components_Lambda_j!AD62-Inequality_Components_Lambda_j!AJ62)</f>
+        <v>26.420675210815499</v>
       </c>
       <c r="G62" s="11">
-        <f>Inequality_Components_Lambda_j!G62+Inequality_Components_Lambda_j!M62-Inequality_Components_Lambda_j!S62+Inequality_Components_Lambda_j!Y62+Inequality_Components_Lambda_j!AE62-Inequality_Components_Lambda_j!AK62</f>
-        <v>127.41696095785974</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G62+Inequality_Components_Lambda_j!M62-Inequality_Components_Lambda_j!S62+Inequality_Components_Lambda_j!Y62+Inequality_Components_Lambda_j!AE62-Inequality_Components_Lambda_j!AK62)</f>
+        <v>33.062564084675437</v>
       </c>
       <c r="H62" s="11">
         <f t="shared" si="3"/>
-        <v>1036.7598856375005</v>
+        <v>269.02179977944445</v>
       </c>
       <c r="I62" s="9">
         <f>(H62-H78)/Background_Calculations!$B$10</f>
-        <v>-5.2016123899200353E-8</v>
+        <v>-1.3497311636731503E-8</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -5718,36 +5718,36 @@
         <v>11</v>
       </c>
       <c r="B63" s="11">
-        <f>Inequality_Components_Lambda_j!B63+Inequality_Components_Lambda_j!H63-Inequality_Components_Lambda_j!N63+Inequality_Components_Lambda_j!T63+Inequality_Components_Lambda_j!Z63-Inequality_Components_Lambda_j!AF63</f>
-        <v>466.58723415974112</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B63+Inequality_Components_Lambda_j!H63-Inequality_Components_Lambda_j!N63+Inequality_Components_Lambda_j!T63+Inequality_Components_Lambda_j!Z63-Inequality_Components_Lambda_j!AF63)</f>
+        <v>121.0715607602656</v>
       </c>
       <c r="C63" s="11">
-        <f>Inequality_Components_Lambda_j!C63+Inequality_Components_Lambda_j!I63-Inequality_Components_Lambda_j!O63+Inequality_Components_Lambda_j!U63+Inequality_Components_Lambda_j!AA63-Inequality_Components_Lambda_j!AG63</f>
-        <v>95.933031649809607</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C63+Inequality_Components_Lambda_j!I63-Inequality_Components_Lambda_j!O63+Inequality_Components_Lambda_j!U63+Inequality_Components_Lambda_j!AA63-Inequality_Components_Lambda_j!AG63)</f>
+        <v>24.893012538637027</v>
       </c>
       <c r="D63" s="11">
-        <f>Inequality_Components_Lambda_j!D63+Inequality_Components_Lambda_j!J63-Inequality_Components_Lambda_j!P63+Inequality_Components_Lambda_j!V63+Inequality_Components_Lambda_j!AB63-Inequality_Components_Lambda_j!AH63</f>
-        <v>117.6502004811239</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D63+Inequality_Components_Lambda_j!J63-Inequality_Components_Lambda_j!P63+Inequality_Components_Lambda_j!V63+Inequality_Components_Lambda_j!AB63-Inequality_Components_Lambda_j!AH63)</f>
+        <v>30.52825356797311</v>
       </c>
       <c r="E63" s="11">
-        <f>Inequality_Components_Lambda_j!E63+Inequality_Components_Lambda_j!K63-Inequality_Components_Lambda_j!Q63+Inequality_Components_Lambda_j!W63+Inequality_Components_Lambda_j!AC63-Inequality_Components_Lambda_j!AI63</f>
-        <v>127.24523687426773</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E63+Inequality_Components_Lambda_j!K63-Inequality_Components_Lambda_j!Q63+Inequality_Components_Lambda_j!W63+Inequality_Components_Lambda_j!AC63-Inequality_Components_Lambda_j!AI63)</f>
+        <v>33.018004565472019</v>
       </c>
       <c r="F63" s="11">
-        <f>Inequality_Components_Lambda_j!F63+Inequality_Components_Lambda_j!L63-Inequality_Components_Lambda_j!R63+Inequality_Components_Lambda_j!X63+Inequality_Components_Lambda_j!AD63-Inequality_Components_Lambda_j!AJ63</f>
-        <v>101.80842006106829</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F63+Inequality_Components_Lambda_j!L63-Inequality_Components_Lambda_j!R63+Inequality_Components_Lambda_j!X63+Inequality_Components_Lambda_j!AD63-Inequality_Components_Lambda_j!AJ63)</f>
+        <v>26.417577277972203</v>
       </c>
       <c r="G63" s="11">
-        <f>Inequality_Components_Lambda_j!G63+Inequality_Components_Lambda_j!M63-Inequality_Components_Lambda_j!S63+Inequality_Components_Lambda_j!Y63+Inequality_Components_Lambda_j!AE63-Inequality_Components_Lambda_j!AK63</f>
-        <v>127.40092999473946</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G63+Inequality_Components_Lambda_j!M63-Inequality_Components_Lambda_j!S63+Inequality_Components_Lambda_j!Y63+Inequality_Components_Lambda_j!AE63-Inequality_Components_Lambda_j!AK63)</f>
+        <v>33.058404318648066</v>
       </c>
       <c r="H63" s="11">
         <f t="shared" si="3"/>
-        <v>1036.62505322075</v>
+        <v>268.98681302896802</v>
       </c>
       <c r="I63" s="9">
         <f>(H63-H79)/Background_Calculations!$B$10</f>
-        <v>-5.8976416078065711E-8</v>
+        <v>-1.5303390705652776E-8</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -5755,36 +5755,36 @@
         <v>12</v>
       </c>
       <c r="B64" s="11">
-        <f>Inequality_Components_Lambda_j!B64+Inequality_Components_Lambda_j!H64-Inequality_Components_Lambda_j!N64+Inequality_Components_Lambda_j!T64+Inequality_Components_Lambda_j!Z64-Inequality_Components_Lambda_j!AF64</f>
-        <v>466.52540283118924</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B64+Inequality_Components_Lambda_j!H64-Inequality_Components_Lambda_j!N64+Inequality_Components_Lambda_j!T64+Inequality_Components_Lambda_j!Z64-Inequality_Components_Lambda_j!AF64)</f>
+        <v>121.0555165676611</v>
       </c>
       <c r="C64" s="11">
-        <f>Inequality_Components_Lambda_j!C64+Inequality_Components_Lambda_j!I64-Inequality_Components_Lambda_j!O64+Inequality_Components_Lambda_j!U64+Inequality_Components_Lambda_j!AA64-Inequality_Components_Lambda_j!AG64</f>
-        <v>95.922246212837052</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C64+Inequality_Components_Lambda_j!I64-Inequality_Components_Lambda_j!O64+Inequality_Components_Lambda_j!U64+Inequality_Components_Lambda_j!AA64-Inequality_Components_Lambda_j!AG64)</f>
+        <v>24.890213898656874</v>
       </c>
       <c r="D64" s="11">
-        <f>Inequality_Components_Lambda_j!D64+Inequality_Components_Lambda_j!J64-Inequality_Components_Lambda_j!P64+Inequality_Components_Lambda_j!V64+Inequality_Components_Lambda_j!AB64-Inequality_Components_Lambda_j!AH64</f>
-        <v>117.63644671055438</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D64+Inequality_Components_Lambda_j!J64-Inequality_Components_Lambda_j!P64+Inequality_Components_Lambda_j!V64+Inequality_Components_Lambda_j!AB64-Inequality_Components_Lambda_j!AH64)</f>
+        <v>30.524684695215178</v>
       </c>
       <c r="E64" s="11">
-        <f>Inequality_Components_Lambda_j!E64+Inequality_Components_Lambda_j!K64-Inequality_Components_Lambda_j!Q64+Inequality_Components_Lambda_j!W64+Inequality_Components_Lambda_j!AC64-Inequality_Components_Lambda_j!AI64</f>
-        <v>127.23093117274999</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E64+Inequality_Components_Lambda_j!K64-Inequality_Components_Lambda_j!Q64+Inequality_Components_Lambda_j!W64+Inequality_Components_Lambda_j!AC64-Inequality_Components_Lambda_j!AI64)</f>
+        <v>33.014292475891082</v>
       </c>
       <c r="F64" s="11">
-        <f>Inequality_Components_Lambda_j!F64+Inequality_Components_Lambda_j!L64-Inequality_Components_Lambda_j!R64+Inequality_Components_Lambda_j!X64+Inequality_Components_Lambda_j!AD64-Inequality_Components_Lambda_j!AJ64</f>
-        <v>101.79696463395148</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F64+Inequality_Components_Lambda_j!L64-Inequality_Components_Lambda_j!R64+Inequality_Components_Lambda_j!X64+Inequality_Components_Lambda_j!AD64-Inequality_Components_Lambda_j!AJ64)</f>
+        <v>26.414604786787987</v>
       </c>
       <c r="G64" s="11">
-        <f>Inequality_Components_Lambda_j!G64+Inequality_Components_Lambda_j!M64-Inequality_Components_Lambda_j!S64+Inequality_Components_Lambda_j!Y64+Inequality_Components_Lambda_j!AE64-Inequality_Components_Lambda_j!AK64</f>
-        <v>127.38571453960107</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G64+Inequality_Components_Lambda_j!M64-Inequality_Components_Lambda_j!S64+Inequality_Components_Lambda_j!Y64+Inequality_Components_Lambda_j!AE64-Inequality_Components_Lambda_j!AK64)</f>
+        <v>33.054456163262714</v>
       </c>
       <c r="H64" s="11">
         <f t="shared" si="3"/>
-        <v>1036.4977061008833</v>
+        <v>268.95376858747488</v>
       </c>
       <c r="I64" s="9">
         <f>(H64-H80)/Background_Calculations!$B$10</f>
-        <v>-6.5550303751161247E-8</v>
+        <v>-1.7009204286857967E-8</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -5792,36 +5792,36 @@
         <v>13</v>
       </c>
       <c r="B65" s="11">
-        <f>Inequality_Components_Lambda_j!B65+Inequality_Components_Lambda_j!H65-Inequality_Components_Lambda_j!N65+Inequality_Components_Lambda_j!T65+Inequality_Components_Lambda_j!Z65-Inequality_Components_Lambda_j!AF65</f>
-        <v>466.46766613235388</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B65+Inequality_Components_Lambda_j!H65-Inequality_Components_Lambda_j!N65+Inequality_Components_Lambda_j!T65+Inequality_Components_Lambda_j!Z65-Inequality_Components_Lambda_j!AF65)</f>
+        <v>121.04053486278499</v>
       </c>
       <c r="C65" s="11">
-        <f>Inequality_Components_Lambda_j!C65+Inequality_Components_Lambda_j!I65-Inequality_Components_Lambda_j!O65+Inequality_Components_Lambda_j!U65+Inequality_Components_Lambda_j!AA65-Inequality_Components_Lambda_j!AG65</f>
-        <v>95.911878068630344</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C65+Inequality_Components_Lambda_j!I65-Inequality_Components_Lambda_j!O65+Inequality_Components_Lambda_j!U65+Inequality_Components_Lambda_j!AA65-Inequality_Components_Lambda_j!AG65)</f>
+        <v>24.887523539149814</v>
       </c>
       <c r="D65" s="11">
-        <f>Inequality_Components_Lambda_j!D65+Inequality_Components_Lambda_j!J65-Inequality_Components_Lambda_j!P65+Inequality_Components_Lambda_j!V65+Inequality_Components_Lambda_j!AB65-Inequality_Components_Lambda_j!AH65</f>
-        <v>117.62332072278357</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D65+Inequality_Components_Lambda_j!J65-Inequality_Components_Lambda_j!P65+Inequality_Components_Lambda_j!V65+Inequality_Components_Lambda_j!AB65-Inequality_Components_Lambda_j!AH65)</f>
+        <v>30.521278721563128</v>
       </c>
       <c r="E65" s="11">
-        <f>Inequality_Components_Lambda_j!E65+Inequality_Components_Lambda_j!K65-Inequality_Components_Lambda_j!Q65+Inequality_Components_Lambda_j!W65+Inequality_Components_Lambda_j!AC65-Inequality_Components_Lambda_j!AI65</f>
-        <v>127.2171788989569</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E65+Inequality_Components_Lambda_j!K65-Inequality_Components_Lambda_j!Q65+Inequality_Components_Lambda_j!W65+Inequality_Components_Lambda_j!AC65-Inequality_Components_Lambda_j!AI65)</f>
+        <v>33.01072399152153</v>
       </c>
       <c r="F65" s="11">
-        <f>Inequality_Components_Lambda_j!F65+Inequality_Components_Lambda_j!L65-Inequality_Components_Lambda_j!R65+Inequality_Components_Lambda_j!X65+Inequality_Components_Lambda_j!AD65-Inequality_Components_Lambda_j!AJ65</f>
-        <v>101.78595409272575</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F65+Inequality_Components_Lambda_j!L65-Inequality_Components_Lambda_j!R65+Inequality_Components_Lambda_j!X65+Inequality_Components_Lambda_j!AD65-Inequality_Components_Lambda_j!AJ65)</f>
+        <v>26.411747736030016</v>
       </c>
       <c r="G65" s="11">
-        <f>Inequality_Components_Lambda_j!G65+Inequality_Components_Lambda_j!M65-Inequality_Components_Lambda_j!S65+Inequality_Components_Lambda_j!Y65+Inequality_Components_Lambda_j!AE65-Inequality_Components_Lambda_j!AK65</f>
-        <v>127.3712495734928</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G65+Inequality_Components_Lambda_j!M65-Inequality_Components_Lambda_j!S65+Inequality_Components_Lambda_j!Y65+Inequality_Components_Lambda_j!AE65-Inequality_Components_Lambda_j!AK65)</f>
+        <v>33.050702747192034</v>
       </c>
       <c r="H65" s="11">
         <f t="shared" si="3"/>
-        <v>1036.3772474889433</v>
+        <v>268.9225115982415</v>
       </c>
       <c r="I65" s="9">
         <f>(H65-H81)/Background_Calculations!$B$10</f>
-        <v>-7.1768594239230978E-8</v>
+        <v>-1.8622746363305907E-8</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -5829,36 +5829,36 @@
         <v>14</v>
       </c>
       <c r="B66" s="11">
-        <f>Inequality_Components_Lambda_j!B66+Inequality_Components_Lambda_j!H66-Inequality_Components_Lambda_j!N66+Inequality_Components_Lambda_j!T66+Inequality_Components_Lambda_j!Z66-Inequality_Components_Lambda_j!AF66</f>
-        <v>466.41342246708257</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!B66+Inequality_Components_Lambda_j!H66-Inequality_Components_Lambda_j!N66+Inequality_Components_Lambda_j!T66+Inequality_Components_Lambda_j!Z66-Inequality_Components_Lambda_j!AF66)</f>
+        <v>121.02645954152683</v>
       </c>
       <c r="C66" s="11">
-        <f>Inequality_Components_Lambda_j!C66+Inequality_Components_Lambda_j!I66-Inequality_Components_Lambda_j!O66+Inequality_Components_Lambda_j!U66+Inequality_Components_Lambda_j!AA66-Inequality_Components_Lambda_j!AG66</f>
-        <v>95.901865907195742</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!C66+Inequality_Components_Lambda_j!I66-Inequality_Components_Lambda_j!O66+Inequality_Components_Lambda_j!U66+Inequality_Components_Lambda_j!AA66-Inequality_Components_Lambda_j!AG66)</f>
+        <v>24.884925551200887</v>
       </c>
       <c r="D66" s="11">
-        <f>Inequality_Components_Lambda_j!D66+Inequality_Components_Lambda_j!J66-Inequality_Components_Lambda_j!P66+Inequality_Components_Lambda_j!V66+Inequality_Components_Lambda_j!AB66-Inequality_Components_Lambda_j!AH66</f>
-        <v>117.61073028194586</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!D66+Inequality_Components_Lambda_j!J66-Inequality_Components_Lambda_j!P66+Inequality_Components_Lambda_j!V66+Inequality_Components_Lambda_j!AB66-Inequality_Components_Lambda_j!AH66)</f>
+        <v>30.518011713356984</v>
       </c>
       <c r="E66" s="11">
-        <f>Inequality_Components_Lambda_j!E66+Inequality_Components_Lambda_j!K66-Inequality_Components_Lambda_j!Q66+Inequality_Components_Lambda_j!W66+Inequality_Components_Lambda_j!AC66-Inequality_Components_Lambda_j!AI66</f>
-        <v>127.20389874150916</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!E66+Inequality_Components_Lambda_j!K66-Inequality_Components_Lambda_j!Q66+Inequality_Components_Lambda_j!W66+Inequality_Components_Lambda_j!AC66-Inequality_Components_Lambda_j!AI66)</f>
+        <v>33.007278013424347</v>
       </c>
       <c r="F66" s="11">
-        <f>Inequality_Components_Lambda_j!F66+Inequality_Components_Lambda_j!L66-Inequality_Components_Lambda_j!R66+Inequality_Components_Lambda_j!X66+Inequality_Components_Lambda_j!AD66-Inequality_Components_Lambda_j!AJ66</f>
-        <v>101.77532307332675</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!F66+Inequality_Components_Lambda_j!L66-Inequality_Components_Lambda_j!R66+Inequality_Components_Lambda_j!X66+Inequality_Components_Lambda_j!AD66-Inequality_Components_Lambda_j!AJ66)</f>
+        <v>26.40898916482001</v>
       </c>
       <c r="G66" s="11">
-        <f>Inequality_Components_Lambda_j!G66+Inequality_Components_Lambda_j!M66-Inequality_Components_Lambda_j!S66+Inequality_Components_Lambda_j!Y66+Inequality_Components_Lambda_j!AE66-Inequality_Components_Lambda_j!AK66</f>
-        <v>127.35742483215527</v>
+        <f>(1-Background_Calculations!$B$11)*(Inequality_Components_Lambda_j!G66+Inequality_Components_Lambda_j!M66-Inequality_Components_Lambda_j!S66+Inequality_Components_Lambda_j!Y66+Inequality_Components_Lambda_j!AE66-Inequality_Components_Lambda_j!AK66)</f>
+        <v>33.047115458710266</v>
       </c>
       <c r="H66" s="11">
         <f t="shared" si="3"/>
-        <v>1036.2626653032153</v>
+        <v>268.89277944303933</v>
       </c>
       <c r="I66" s="9">
         <f>(H66-H82)/Background_Calculations!$B$10</f>
-        <v>-7.7683533023102899E-8</v>
+        <v>-2.0157573760915297E-8</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5877,32 +5877,32 @@
         <v>0</v>
       </c>
       <c r="B68" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C68" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D68" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E68" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F68" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G68" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H68" s="11">
         <f>SUM(B68:G68)</f>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -5910,32 +5910,32 @@
         <v>1</v>
       </c>
       <c r="B69" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C69" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D69" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E69" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F69" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G69" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H69" s="11">
         <f t="shared" ref="H69:H82" si="4">SUM(B69:G69)</f>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5943,32 +5943,32 @@
         <v>2</v>
       </c>
       <c r="B70" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C70" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D70" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E70" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F70" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G70" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H70" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5976,32 +5976,32 @@
         <v>3</v>
       </c>
       <c r="B71" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C71" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D71" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E71" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F71" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G71" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H71" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -6009,32 +6009,32 @@
         <v>4</v>
       </c>
       <c r="B72" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C72" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D72" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E72" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F72" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G72" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H72" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -6042,32 +6042,32 @@
         <v>5</v>
       </c>
       <c r="B73" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C73" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D73" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E73" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F73" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G73" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H73" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -6075,32 +6075,32 @@
         <v>6</v>
       </c>
       <c r="B74" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C74" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D74" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E74" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F74" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G74" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H74" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -6108,32 +6108,32 @@
         <v>7</v>
       </c>
       <c r="B75" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C75" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D75" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E75" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F75" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G75" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H75" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -6141,32 +6141,32 @@
         <v>8</v>
       </c>
       <c r="B76" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C76" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D76" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E76" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F76" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G76" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H76" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -6174,32 +6174,32 @@
         <v>9</v>
       </c>
       <c r="B77" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C77" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D77" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E77" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F77" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G77" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H77" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -6207,32 +6207,32 @@
         <v>10</v>
       </c>
       <c r="B78" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C78" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D78" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E78" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F78" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G78" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H78" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -6240,32 +6240,32 @@
         <v>11</v>
       </c>
       <c r="B79" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C79" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D79" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E79" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F79" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G79" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H79" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -6273,32 +6273,32 @@
         <v>12</v>
       </c>
       <c r="B80" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C80" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D80" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E80" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F80" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G80" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H80" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -6306,32 +6306,32 @@
         <v>13</v>
       </c>
       <c r="B81" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C81" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D81" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E81" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F81" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G81" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H81" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -6339,32 +6339,32 @@
         <v>14</v>
       </c>
       <c r="B82" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>467.10159034233345</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!B$3*(1-Background_Calculations!B$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>121.20502756187086</v>
       </c>
       <c r="C82" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>96.035660576822735</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!C$3*(1-Background_Calculations!C$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>24.919643023705927</v>
       </c>
       <c r="D82" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>117.77739654143545</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!D$3*(1-Background_Calculations!D$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>30.561258812045441</v>
       </c>
       <c r="E82" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.38399989087245</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!E$3*(1-Background_Calculations!E$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.054011240679046</v>
       </c>
       <c r="F82" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>101.91946803433856</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!F$3*(1-Background_Calculations!F$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>26.446392364324293</v>
       </c>
       <c r="G82" s="11">
-        <f>Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24</f>
-        <v>127.54940894201242</v>
+        <f>(1-Background_Calculations!$B$11)*(Background_Calculations!$B$10*(Background_Calculations!$B$9*Background_Calculations!G$3*(1-Background_Calculations!G$6)/(1-Background_Calculations!$B$11))*Quarantine_Input!$B$24)</f>
+        <v>33.096932114889107</v>
       </c>
       <c r="H82" s="11">
         <f t="shared" si="4"/>
-        <v>1037.7675243278152</v>
+        <v>269.28326511751465</v>
       </c>
     </row>
   </sheetData>
@@ -6384,8 +6384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1DE64A-064F-481D-9FBF-B445490B2E7D}">
   <dimension ref="A1:AK66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>